<commit_message>
update named ranges for hkd 6m yc bootstrap
</commit_message>
<xml_diff>
--- a/QuantLibXL/Data2/XLS/HKD_YC6MBootstrapping.xlsx
+++ b/QuantLibXL/Data2/XLS/HKD_YC6MBootstrapping.xlsx
@@ -13,53 +13,37 @@
     <sheet name="Selected" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="Accuracy">'General Settings'!$D$23</definedName>
-    <definedName name="BondBasisDayCounter">#REF!</definedName>
-    <definedName name="Calendar" localSheetId="1">#REF!</definedName>
-    <definedName name="Calendar">'General Settings'!$D$18</definedName>
-    <definedName name="Currency" localSheetId="1">'General Settings'!$J$14</definedName>
-    <definedName name="Currency">'General Settings'!$D$4</definedName>
-    <definedName name="DayCounter">'General Settings'!$D$19</definedName>
+    <definedName name="Accuracy">'General Settings'!$D$19</definedName>
+    <definedName name="Calendar">'General Settings'!$D$14</definedName>
+    <definedName name="Currency">'General Settings'!$J$14</definedName>
+    <definedName name="DayCounter">'General Settings'!$D$15</definedName>
     <definedName name="DepoInclusionCriteria">Selected!$B$5</definedName>
     <definedName name="FamilyName">'General Settings'!$J$15</definedName>
     <definedName name="FileOverwrite">'General Settings'!$J$9</definedName>
     <definedName name="FrontFuturesRollingDays">Selected!$B$4</definedName>
     <definedName name="GENERAL_SETTINGS">'General Settings'!$H$12</definedName>
-    <definedName name="IborType">'General Settings'!$D$7</definedName>
-    <definedName name="Index1M">#REF!</definedName>
-    <definedName name="Index1Y">#REF!</definedName>
-    <definedName name="Index3M">#REF!</definedName>
-    <definedName name="Index6M">#REF!</definedName>
-    <definedName name="IndexTenor">'General Settings'!$D$6</definedName>
-    <definedName name="InterpolatorID">'General Settings'!$D$25</definedName>
+    <definedName name="IborType">'General Settings'!$D$6</definedName>
+    <definedName name="IndexTenor">'General Settings'!$D$5</definedName>
+    <definedName name="InterpolatorID">'General Settings'!$D$21</definedName>
     <definedName name="MinDistance">RateHelpers!$F$2:$F$19</definedName>
-    <definedName name="MoneyMarketDayCounter">#REF!</definedName>
-    <definedName name="Months">'General Settings'!$D$5</definedName>
-    <definedName name="NDays">'General Settings'!$D$17</definedName>
+    <definedName name="Months">'General Settings'!$D$4</definedName>
+    <definedName name="NDays">'General Settings'!$D$13</definedName>
     <definedName name="nIMMFutures">Selected!$B$2</definedName>
     <definedName name="nSerialFutures">Selected!$B$3</definedName>
-    <definedName name="ObjectOverwrite" localSheetId="1">'General Settings'!$J$6</definedName>
-    <definedName name="ObjectOverwrite">'General Settings'!$D$12</definedName>
-    <definedName name="Permanent" localSheetId="1">'General Settings'!$J$5</definedName>
-    <definedName name="Permanent">'General Settings'!$D$10</definedName>
+    <definedName name="ObjectOverwrite">'General Settings'!$J$6</definedName>
+    <definedName name="Permanent">'General Settings'!$J$5</definedName>
     <definedName name="QuoteSuffix">'General Settings'!$J$16</definedName>
-    <definedName name="RateHelperPrefix" localSheetId="1">#REF!</definedName>
-    <definedName name="RateHelperPrefix">'General Settings'!$D$9</definedName>
+    <definedName name="RateHelperPrefix">'General Settings'!$D$8</definedName>
     <definedName name="RateHelpers">RateHelpers!$A$2:$A$19</definedName>
     <definedName name="RateHelpersIncluded">RateHelpers!$D$2:$D$19</definedName>
     <definedName name="RateHelpersPriority">RateHelpers!$E$2:$E$19</definedName>
     <definedName name="RateHelpersSelected">Selected!$A$7</definedName>
-    <definedName name="ReutersFloatingLegCode">#REF!</definedName>
     <definedName name="SerializationPath">'General Settings'!$J$8</definedName>
     <definedName name="Serialize">'General Settings'!$J$7</definedName>
-    <definedName name="SwapFixedFreq">'General Settings'!$D$8</definedName>
-    <definedName name="SwapMainSetConventions">#REF!</definedName>
-    <definedName name="SwapSecondarySetConventions">#REF!</definedName>
-    <definedName name="TraitsID">'General Settings'!$D$24</definedName>
-    <definedName name="Trigger" localSheetId="1">'General Settings'!$J$4</definedName>
-    <definedName name="Trigger">'General Settings'!$D$11</definedName>
-    <definedName name="YieldCurve">'General Settings'!$D$14</definedName>
-    <definedName name="YieldCurveFrequency">#REF!</definedName>
+    <definedName name="SwapFixedFreq">'General Settings'!$D$7</definedName>
+    <definedName name="TraitsID">'General Settings'!$D$20</definedName>
+    <definedName name="Trigger">'General Settings'!$J$4</definedName>
+    <definedName name="YieldCurve">'General Settings'!$D$10</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
@@ -71,20 +55,7 @@
     <author>Ferdinando Ametrano</author>
   </authors>
   <commentList>
-    <comment ref="D10" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>TRUE if the object must be permanent (i.e. resistant to garbage collection). Default is FALSE.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D16" authorId="0">
+    <comment ref="D12" authorId="0">
       <text>
         <r>
           <rPr>
@@ -97,7 +68,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D17" authorId="0">
+    <comment ref="D13" authorId="0">
       <text>
         <r>
           <rPr>
@@ -110,7 +81,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D24" authorId="0">
+    <comment ref="D20" authorId="0">
       <text>
         <r>
           <rPr>
@@ -123,7 +94,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D25" authorId="0">
+    <comment ref="D21" authorId="0">
       <text>
         <r>
           <rPr>
@@ -227,7 +198,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="84">
   <si>
     <t>Earliest Date</t>
   </si>
@@ -1139,7 +1110,7 @@
     <xf numFmtId="173" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="173" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="134">
+  <cellXfs count="133">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1319,12 +1290,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="3" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="9" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="10" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1347,14 +1312,9 @@
     <xf numFmtId="0" fontId="18" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="20" fillId="10" borderId="24" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="20" fillId="10" borderId="27" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="20" fillId="10" borderId="25" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="18" fillId="10" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1432,6 +1392,16 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="31" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="10">
     <cellStyle name="Migliaia (0)_AZIONI" xfId="4"/>
@@ -1749,568 +1719,532 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="2.7109375" style="79" customWidth="1"/>
-    <col min="3" max="3" width="18" style="79" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.85546875" style="79" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22" style="79" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="2.7109375" style="79" customWidth="1"/>
-    <col min="9" max="9" width="12.140625" style="79" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="21.140625" style="79" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="2.7109375" style="79" customWidth="1"/>
-    <col min="12" max="16384" width="8" style="79"/>
+    <col min="1" max="2" width="2.7109375" style="77" customWidth="1"/>
+    <col min="3" max="3" width="18" style="77" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.85546875" style="77" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22" style="77" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="2.7109375" style="77" customWidth="1"/>
+    <col min="9" max="9" width="12.140625" style="77" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="33.42578125" style="77" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="2.7109375" style="77" customWidth="1"/>
+    <col min="12" max="16384" width="8" style="77"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="80"/>
-      <c r="B1" s="80" t="str">
+      <c r="A1" s="78"/>
+      <c r="B1" s="78" t="str">
         <f>_xll.qlxlVersion(TRUE,Trigger)</f>
         <v>QuantLibXL 1.3.0 - MS VC++ 9.0 - Multithreaded Static Runtime library - Release Configuration - Nov 12 2013 12:02:30</v>
       </c>
-      <c r="C1" s="80"/>
-      <c r="D1" s="80"/>
-      <c r="E1" s="80"/>
-      <c r="F1" s="80"/>
-      <c r="G1" s="80"/>
-      <c r="H1" s="80"/>
-      <c r="I1" s="80"/>
-      <c r="J1" s="80"/>
-      <c r="K1" s="80"/>
+      <c r="C1" s="78"/>
+      <c r="D1" s="78"/>
+      <c r="E1" s="78"/>
+      <c r="F1" s="78"/>
+      <c r="G1" s="78"/>
+      <c r="H1" s="78"/>
+      <c r="I1" s="78"/>
+      <c r="J1" s="78"/>
+      <c r="K1" s="78"/>
     </row>
     <row r="2" spans="1:11" ht="18" x14ac:dyDescent="0.25">
-      <c r="A2" s="80"/>
-      <c r="B2" s="131" t="s">
+      <c r="A2" s="78"/>
+      <c r="B2" s="126" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="132"/>
-      <c r="D2" s="132"/>
-      <c r="E2" s="132"/>
-      <c r="F2" s="133"/>
-      <c r="G2" s="80"/>
-      <c r="H2" s="131" t="s">
+      <c r="C2" s="127"/>
+      <c r="D2" s="127"/>
+      <c r="E2" s="127"/>
+      <c r="F2" s="128"/>
+      <c r="G2" s="78"/>
+      <c r="H2" s="126" t="s">
         <v>68</v>
       </c>
-      <c r="I2" s="132"/>
-      <c r="J2" s="132"/>
-      <c r="K2" s="132"/>
+      <c r="I2" s="127"/>
+      <c r="J2" s="127"/>
+      <c r="K2" s="127"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A3" s="80"/>
-      <c r="B3" s="81"/>
-      <c r="C3" s="82"/>
-      <c r="D3" s="83"/>
-      <c r="E3" s="83"/>
-      <c r="F3" s="84"/>
-      <c r="G3" s="80"/>
-      <c r="H3" s="85"/>
-      <c r="I3" s="86"/>
-      <c r="J3" s="86"/>
-      <c r="K3" s="87"/>
+      <c r="A3" s="78"/>
+      <c r="B3" s="79"/>
+      <c r="C3" s="80"/>
+      <c r="D3" s="81"/>
+      <c r="E3" s="81"/>
+      <c r="F3" s="82"/>
+      <c r="G3" s="78"/>
+      <c r="H3" s="83"/>
+      <c r="I3" s="84"/>
+      <c r="J3" s="84"/>
+      <c r="K3" s="85"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" s="80"/>
-      <c r="B4" s="81"/>
-      <c r="C4" s="88" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="89" t="s">
-        <v>47</v>
-      </c>
-      <c r="E4" s="83"/>
-      <c r="F4" s="84"/>
-      <c r="G4" s="80"/>
-      <c r="H4" s="85"/>
-      <c r="I4" s="90" t="s">
+      <c r="A4" s="78"/>
+      <c r="B4" s="79"/>
+      <c r="C4" s="86" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" s="131">
         <v>6</v>
       </c>
-      <c r="J4" s="91">
+      <c r="E4" s="81"/>
+      <c r="F4" s="82"/>
+      <c r="G4" s="78"/>
+      <c r="H4" s="83"/>
+      <c r="I4" s="88" t="s">
+        <v>6</v>
+      </c>
+      <c r="J4" s="89">
         <v>41598.740243055552</v>
       </c>
-      <c r="K4" s="92"/>
+      <c r="K4" s="90"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A5" s="80"/>
-      <c r="B5" s="81"/>
-      <c r="C5" s="93" t="s">
-        <v>38</v>
-      </c>
-      <c r="D5" s="94">
-        <v>6</v>
-      </c>
-      <c r="E5" s="83"/>
-      <c r="F5" s="84"/>
-      <c r="G5" s="80"/>
-      <c r="H5" s="85"/>
-      <c r="I5" s="90" t="s">
+      <c r="A5" s="78"/>
+      <c r="B5" s="79"/>
+      <c r="C5" s="91" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5" s="92" t="str">
+        <f>_xll.qlPeriodEquivalent(D4&amp;"M")</f>
+        <v>6M</v>
+      </c>
+      <c r="E5" s="81"/>
+      <c r="F5" s="82"/>
+      <c r="G5" s="78"/>
+      <c r="H5" s="83"/>
+      <c r="I5" s="88" t="s">
         <v>13</v>
       </c>
-      <c r="J5" s="91" t="b">
+      <c r="J5" s="89" t="b">
         <v>1</v>
       </c>
-      <c r="K5" s="92"/>
+      <c r="K5" s="90"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6" s="80"/>
-      <c r="B6" s="81"/>
-      <c r="C6" s="93" t="s">
-        <v>34</v>
-      </c>
-      <c r="D6" s="94" t="str">
-        <f>_xll.qlPeriodEquivalent(D5&amp;"M")</f>
-        <v>6M</v>
-      </c>
-      <c r="E6" s="83"/>
-      <c r="F6" s="84"/>
-      <c r="G6" s="80"/>
-      <c r="H6" s="85"/>
-      <c r="I6" s="90" t="s">
+      <c r="A6" s="78"/>
+      <c r="B6" s="79"/>
+      <c r="C6" s="91" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" s="92" t="s">
+        <v>48</v>
+      </c>
+      <c r="E6" s="81"/>
+      <c r="F6" s="82"/>
+      <c r="G6" s="78"/>
+      <c r="H6" s="83"/>
+      <c r="I6" s="88" t="s">
         <v>26</v>
       </c>
-      <c r="J6" s="91" t="b">
+      <c r="J6" s="89" t="b">
         <v>0</v>
       </c>
-      <c r="K6" s="92"/>
+      <c r="K6" s="90"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A7" s="80"/>
-      <c r="B7" s="81"/>
-      <c r="C7" s="93" t="s">
-        <v>39</v>
-      </c>
-      <c r="D7" s="94" t="s">
-        <v>48</v>
-      </c>
-      <c r="E7" s="83"/>
-      <c r="F7" s="84"/>
-      <c r="G7" s="80"/>
-      <c r="H7" s="85"/>
-      <c r="I7" s="90" t="s">
+      <c r="A7" s="78"/>
+      <c r="B7" s="79"/>
+      <c r="C7" s="91" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" s="92" t="s">
+        <v>49</v>
+      </c>
+      <c r="E7" s="81"/>
+      <c r="F7" s="82"/>
+      <c r="G7" s="78"/>
+      <c r="H7" s="83"/>
+      <c r="I7" s="88" t="s">
         <v>67</v>
       </c>
-      <c r="J7" s="91" t="b">
+      <c r="J7" s="89" t="b">
         <v>1</v>
       </c>
-      <c r="K7" s="92"/>
+      <c r="K7" s="90"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A8" s="80"/>
-      <c r="B8" s="81"/>
-      <c r="C8" s="93" t="s">
-        <v>40</v>
-      </c>
-      <c r="D8" s="94" t="s">
-        <v>49</v>
-      </c>
-      <c r="E8" s="83"/>
-      <c r="F8" s="84"/>
-      <c r="G8" s="80"/>
-      <c r="H8" s="85"/>
-      <c r="I8" s="90" t="s">
-        <v>66</v>
-      </c>
-      <c r="J8" s="91" t="e">
-        <f ca="1">SUBSTITUTE(LEFT(CELL("filename",#REF!),FIND("[",CELL("filename",#REF!),1)-1),"\XLS\","\XML\")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="K8" s="92"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A9" s="80"/>
-      <c r="B9" s="81"/>
-      <c r="C9" s="93" t="s">
+      <c r="A8" s="78"/>
+      <c r="B8" s="79"/>
+      <c r="C8" s="132" t="s">
         <v>23</v>
       </c>
-      <c r="D9" s="94" t="str">
+      <c r="D8" s="96" t="str">
         <f>Currency&amp;"_YC"&amp;IndexTenor&amp;"RH"</f>
         <v>HKD_YC6MRH</v>
       </c>
-      <c r="E9" s="83"/>
-      <c r="F9" s="84"/>
-      <c r="G9" s="80"/>
-      <c r="H9" s="85"/>
-      <c r="I9" s="90" t="s">
+      <c r="E8" s="81"/>
+      <c r="F8" s="82"/>
+      <c r="G8" s="78"/>
+      <c r="H8" s="83"/>
+      <c r="I8" s="88" t="s">
+        <v>66</v>
+      </c>
+      <c r="J8" s="89" t="str">
+        <f ca="1">SUBSTITUTE(LEFT(CELL("filename",A1),FIND("[",CELL("filename",A1),1)-1),"\XLS\","\XML\")</f>
+        <v>C:\Projects\quantlib\QuantLibXL\Data2\XML\</v>
+      </c>
+      <c r="K8" s="90"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9" s="78"/>
+      <c r="B9" s="79"/>
+      <c r="C9" s="97"/>
+      <c r="D9" s="97"/>
+      <c r="E9" s="81"/>
+      <c r="F9" s="82"/>
+      <c r="G9" s="78"/>
+      <c r="H9" s="83"/>
+      <c r="I9" s="88" t="s">
         <v>65</v>
       </c>
-      <c r="J9" s="91" t="b">
+      <c r="J9" s="89" t="b">
         <v>1</v>
       </c>
-      <c r="K9" s="92"/>
+      <c r="K9" s="90"/>
     </row>
     <row r="10" spans="1:11" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="80"/>
-      <c r="B10" s="81"/>
-      <c r="C10" s="95" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10" s="94" t="b">
-        <v>1</v>
-      </c>
-      <c r="E10" s="83"/>
-      <c r="F10" s="84"/>
-      <c r="G10" s="80"/>
-      <c r="H10" s="96"/>
-      <c r="I10" s="97"/>
-      <c r="J10" s="97"/>
-      <c r="K10" s="98"/>
+      <c r="A10" s="78"/>
+      <c r="B10" s="79"/>
+      <c r="C10" s="101" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="89" t="str">
+        <f>_xll.qlPiecewiseYieldCurve(D12,NDays,Calendar,RateHelpersSelected,DayCounter,IF(ISERROR(D18),NA(),D16:E16),IF(ISERROR(D18),NA(),D17:E17),Accuracy,TraitsID,InterpolatorID,Permanent,,ObjectOverwrite)</f>
+        <v>_HKDYC6M#0003</v>
+      </c>
+      <c r="E10" s="81"/>
+      <c r="F10" s="82"/>
+      <c r="G10" s="78"/>
+      <c r="H10" s="93"/>
+      <c r="I10" s="94"/>
+      <c r="J10" s="94"/>
+      <c r="K10" s="95"/>
     </row>
     <row r="11" spans="1:11" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="80"/>
-      <c r="B11" s="81"/>
-      <c r="C11" s="95" t="s">
-        <v>6</v>
-      </c>
-      <c r="D11" s="99">
-        <v>41598.749120370368</v>
-      </c>
-      <c r="E11" s="83"/>
-      <c r="F11" s="84"/>
-      <c r="G11" s="80"/>
-      <c r="H11" s="80"/>
-      <c r="I11" s="80"/>
-      <c r="J11" s="80"/>
-      <c r="K11" s="80"/>
-    </row>
-    <row r="12" spans="1:11" ht="18" x14ac:dyDescent="0.25">
-      <c r="A12" s="80"/>
-      <c r="B12" s="81"/>
-      <c r="C12" s="100" t="s">
-        <v>26</v>
-      </c>
-      <c r="D12" s="101" t="b">
-        <v>1</v>
-      </c>
-      <c r="E12" s="83"/>
-      <c r="F12" s="84"/>
-      <c r="G12" s="80"/>
-      <c r="H12" s="131" t="s">
-        <v>64</v>
-      </c>
-      <c r="I12" s="132"/>
-      <c r="J12" s="132"/>
-      <c r="K12" s="132"/>
-    </row>
-    <row r="13" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A13" s="80"/>
-      <c r="B13" s="81"/>
-      <c r="C13" s="102"/>
-      <c r="D13" s="102"/>
-      <c r="E13" s="83"/>
-      <c r="F13" s="84"/>
-      <c r="G13" s="80"/>
-      <c r="H13" s="103"/>
-      <c r="I13" s="104"/>
-      <c r="J13" s="104"/>
-      <c r="K13" s="105"/>
-    </row>
-    <row r="14" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A14" s="80"/>
-      <c r="B14" s="81"/>
-      <c r="C14" s="106" t="s">
-        <v>14</v>
-      </c>
-      <c r="D14" s="91" t="str">
-        <f>_xll.qlPiecewiseYieldCurve(D16,NDays,Calendar,RateHelpersSelected,DayCounter,IF(ISERROR(D22),NA(),D20:E20),IF(ISERROR(D22),NA(),D21:E21),Accuracy,TraitsID,InterpolatorID,Permanent,,ObjectOverwrite)</f>
-        <v>_HKDYC6M#0001</v>
-      </c>
-      <c r="E14" s="83"/>
-      <c r="F14" s="84"/>
-      <c r="G14" s="80"/>
-      <c r="H14" s="103"/>
-      <c r="I14" s="107" t="s">
-        <v>5</v>
-      </c>
-      <c r="J14" s="91" t="s">
-        <v>47</v>
-      </c>
-      <c r="K14" s="105"/>
-    </row>
-    <row r="15" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A15" s="80"/>
-      <c r="B15" s="81"/>
-      <c r="C15" s="108" t="s">
+      <c r="A11" s="78"/>
+      <c r="B11" s="79"/>
+      <c r="C11" s="103" t="s">
         <v>15</v>
       </c>
-      <c r="D15" s="91" t="str">
+      <c r="D11" s="89" t="str">
         <f>_xll.ohRangeRetrieveError(YieldCurve)</f>
         <v/>
       </c>
-      <c r="E15" s="83"/>
-      <c r="F15" s="84"/>
-      <c r="G15" s="80"/>
-      <c r="H15" s="103"/>
-      <c r="I15" s="107" t="s">
-        <v>63</v>
-      </c>
-      <c r="J15" s="91" t="s">
-        <v>62</v>
-      </c>
-      <c r="K15" s="105"/>
-    </row>
-    <row r="16" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A16" s="80"/>
-      <c r="B16" s="81"/>
-      <c r="C16" s="106" t="s">
+      <c r="E11" s="81"/>
+      <c r="F11" s="82"/>
+      <c r="G11" s="78"/>
+      <c r="H11" s="78"/>
+      <c r="I11" s="78"/>
+      <c r="J11" s="78"/>
+      <c r="K11" s="78"/>
+    </row>
+    <row r="12" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+      <c r="A12" s="78"/>
+      <c r="B12" s="79"/>
+      <c r="C12" s="101" t="s">
         <v>9</v>
       </c>
-      <c r="D16" s="109" t="str">
+      <c r="D12" s="104" t="str">
         <f>"_"&amp;Currency&amp;"YC"&amp;IndexTenor</f>
         <v>_HKDYC6M</v>
       </c>
-      <c r="E16" s="83"/>
-      <c r="F16" s="84"/>
-      <c r="G16" s="80"/>
-      <c r="H16" s="103"/>
-      <c r="I16" s="107" t="s">
-        <v>61</v>
-      </c>
-      <c r="J16" s="91" t="s">
-        <v>60</v>
-      </c>
-      <c r="K16" s="105"/>
-    </row>
-    <row r="17" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="80"/>
-      <c r="B17" s="81"/>
-      <c r="C17" s="110" t="s">
+      <c r="E12" s="81"/>
+      <c r="F12" s="82"/>
+      <c r="G12" s="78"/>
+      <c r="H12" s="126" t="s">
+        <v>64</v>
+      </c>
+      <c r="I12" s="127"/>
+      <c r="J12" s="127"/>
+      <c r="K12" s="127"/>
+    </row>
+    <row r="13" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A13" s="78"/>
+      <c r="B13" s="79"/>
+      <c r="C13" s="105" t="s">
         <v>10</v>
       </c>
-      <c r="D17" s="111">
+      <c r="D13" s="106">
         <v>0</v>
       </c>
-      <c r="E17" s="83"/>
-      <c r="F17" s="84"/>
-      <c r="G17" s="80"/>
-      <c r="H17" s="112"/>
-      <c r="I17" s="113"/>
-      <c r="J17" s="113"/>
-      <c r="K17" s="114"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A18" s="80"/>
-      <c r="B18" s="81"/>
-      <c r="C18" s="110" t="s">
+      <c r="E13" s="81"/>
+      <c r="F13" s="82"/>
+      <c r="G13" s="78"/>
+      <c r="H13" s="98"/>
+      <c r="I13" s="99"/>
+      <c r="J13" s="99"/>
+      <c r="K13" s="100"/>
+    </row>
+    <row r="14" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A14" s="78"/>
+      <c r="B14" s="79"/>
+      <c r="C14" s="105" t="s">
         <v>4</v>
       </c>
-      <c r="D18" s="115" t="s">
+      <c r="D14" s="110" t="s">
         <v>50</v>
       </c>
-      <c r="E18" s="83"/>
-      <c r="F18" s="84"/>
-      <c r="G18" s="80"/>
-      <c r="H18" s="80"/>
-      <c r="I18" s="80"/>
-      <c r="J18" s="80"/>
-      <c r="K18" s="80"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A19" s="80"/>
-      <c r="B19" s="81"/>
-      <c r="C19" s="110" t="s">
+      <c r="E14" s="81"/>
+      <c r="F14" s="82"/>
+      <c r="G14" s="78"/>
+      <c r="H14" s="98"/>
+      <c r="I14" s="102" t="s">
+        <v>5</v>
+      </c>
+      <c r="J14" s="89" t="s">
+        <v>47</v>
+      </c>
+      <c r="K14" s="100"/>
+    </row>
+    <row r="15" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A15" s="78"/>
+      <c r="B15" s="79"/>
+      <c r="C15" s="105" t="s">
         <v>8</v>
       </c>
-      <c r="D19" s="115"/>
-      <c r="E19" s="83"/>
-      <c r="F19" s="84"/>
-      <c r="G19" s="80"/>
-      <c r="H19" s="80"/>
-      <c r="I19" s="80"/>
-      <c r="J19" s="80"/>
-      <c r="K19" s="80"/>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A20" s="80"/>
-      <c r="B20" s="81"/>
-      <c r="C20" s="110" t="s">
+      <c r="D15" s="110"/>
+      <c r="E15" s="81"/>
+      <c r="F15" s="82"/>
+      <c r="G15" s="78"/>
+      <c r="H15" s="98"/>
+      <c r="I15" s="102" t="s">
+        <v>63</v>
+      </c>
+      <c r="J15" s="89" t="s">
+        <v>62</v>
+      </c>
+      <c r="K15" s="100"/>
+    </row>
+    <row r="16" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A16" s="78"/>
+      <c r="B16" s="79"/>
+      <c r="C16" s="105" t="s">
         <v>36</v>
       </c>
-      <c r="D20" s="116" t="str">
+      <c r="D16" s="111" t="str">
         <f>Currency&amp;"TOY_SYNTH"&amp;IndexTenor&amp;"_Quote"</f>
         <v>HKDTOY_SYNTH6M_Quote</v>
       </c>
-      <c r="E20" s="89" t="str">
+      <c r="E16" s="87" t="str">
         <f>Currency&amp;"TOY2_SYNTH"&amp;IndexTenor&amp;"_Quote"</f>
         <v>HKDTOY2_SYNTH6M_Quote</v>
       </c>
-      <c r="F20" s="84"/>
-      <c r="G20" s="80"/>
-      <c r="H20" s="80"/>
-      <c r="I20" s="80"/>
-      <c r="J20" s="80"/>
-      <c r="K20" s="80"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A21" s="80"/>
-      <c r="B21" s="81"/>
-      <c r="C21" s="110" t="s">
+      <c r="F16" s="82"/>
+      <c r="G16" s="78"/>
+      <c r="H16" s="98"/>
+      <c r="I16" s="102" t="s">
+        <v>61</v>
+      </c>
+      <c r="J16" s="89" t="s">
+        <v>60</v>
+      </c>
+      <c r="K16" s="100"/>
+    </row>
+    <row r="17" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="78"/>
+      <c r="B17" s="79"/>
+      <c r="C17" s="105" t="s">
         <v>37</v>
       </c>
-      <c r="D21" s="117">
+      <c r="D17" s="112">
         <f>DATE(YEAR(_xll.qlCalendarAdvance(Calendar,_xll.qlSettingsEvaluationDate(Trigger),NDays&amp;"D")),12,31)</f>
         <v>41639</v>
       </c>
-      <c r="E21" s="118">
-        <f>DATE(YEAR(D21+1),12,31)</f>
+      <c r="E17" s="113">
+        <f>DATE(YEAR(D17+1),12,31)</f>
         <v>42004</v>
       </c>
-      <c r="F21" s="84"/>
-      <c r="G21" s="80"/>
-      <c r="H21" s="80"/>
-      <c r="I21" s="80"/>
-      <c r="J21" s="80"/>
-      <c r="K21" s="80"/>
+      <c r="F17" s="82"/>
+      <c r="G17" s="78"/>
+      <c r="H17" s="107"/>
+      <c r="I17" s="108"/>
+      <c r="J17" s="108"/>
+      <c r="K17" s="109"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A18" s="78"/>
+      <c r="B18" s="79"/>
+      <c r="C18" s="105" t="s">
+        <v>42</v>
+      </c>
+      <c r="D18" s="114" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E18" s="115" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F18" s="82"/>
+      <c r="G18" s="78"/>
+      <c r="H18" s="78"/>
+      <c r="I18" s="78"/>
+      <c r="J18" s="78"/>
+      <c r="K18" s="78"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A19" s="78"/>
+      <c r="B19" s="79"/>
+      <c r="C19" s="105" t="s">
+        <v>22</v>
+      </c>
+      <c r="D19" s="116"/>
+      <c r="E19" s="81"/>
+      <c r="F19" s="82"/>
+      <c r="G19" s="78"/>
+      <c r="H19" s="78"/>
+      <c r="I19" s="78"/>
+      <c r="J19" s="78"/>
+      <c r="K19" s="78"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A20" s="78"/>
+      <c r="B20" s="79"/>
+      <c r="C20" s="105" t="s">
+        <v>11</v>
+      </c>
+      <c r="D20" s="92" t="s">
+        <v>35</v>
+      </c>
+      <c r="E20" s="81"/>
+      <c r="F20" s="82"/>
+      <c r="G20" s="78"/>
+      <c r="H20" s="78"/>
+      <c r="I20" s="78"/>
+      <c r="J20" s="78"/>
+      <c r="K20" s="78"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A21" s="78"/>
+      <c r="B21" s="79"/>
+      <c r="C21" s="103" t="s">
+        <v>12</v>
+      </c>
+      <c r="D21" s="96" t="s">
+        <v>51</v>
+      </c>
+      <c r="E21" s="81"/>
+      <c r="F21" s="82"/>
+      <c r="G21" s="78"/>
+      <c r="H21" s="78"/>
+      <c r="I21" s="78"/>
+      <c r="J21" s="78"/>
+      <c r="K21" s="78"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A22" s="80"/>
-      <c r="B22" s="81"/>
-      <c r="C22" s="110" t="s">
-        <v>42</v>
-      </c>
-      <c r="D22" s="119" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="E22" s="120" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="F22" s="84"/>
-      <c r="G22" s="80"/>
-      <c r="H22" s="80"/>
-      <c r="I22" s="80"/>
-      <c r="J22" s="80"/>
-      <c r="K22" s="80"/>
+      <c r="A22" s="78"/>
+      <c r="B22" s="79"/>
+      <c r="C22" s="97"/>
+      <c r="D22" s="97"/>
+      <c r="E22" s="81"/>
+      <c r="F22" s="82"/>
+      <c r="G22" s="78"/>
+      <c r="H22" s="78"/>
+      <c r="I22" s="78"/>
+      <c r="J22" s="78"/>
+      <c r="K22" s="78"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A23" s="80"/>
-      <c r="B23" s="81"/>
-      <c r="C23" s="110" t="s">
-        <v>22</v>
-      </c>
-      <c r="D23" s="121"/>
-      <c r="E23" s="83"/>
-      <c r="F23" s="84"/>
-      <c r="G23" s="80"/>
-      <c r="H23" s="80"/>
-      <c r="I23" s="80"/>
-      <c r="J23" s="80"/>
-      <c r="K23" s="80"/>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A24" s="80"/>
-      <c r="B24" s="81"/>
-      <c r="C24" s="110" t="s">
-        <v>11</v>
-      </c>
-      <c r="D24" s="94" t="s">
-        <v>35</v>
-      </c>
-      <c r="E24" s="83"/>
-      <c r="F24" s="84"/>
-      <c r="G24" s="80"/>
-      <c r="H24" s="80"/>
-      <c r="I24" s="80"/>
-      <c r="J24" s="80"/>
-      <c r="K24" s="80"/>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A25" s="80"/>
-      <c r="B25" s="81"/>
-      <c r="C25" s="108" t="s">
-        <v>12</v>
-      </c>
-      <c r="D25" s="101" t="s">
-        <v>51</v>
-      </c>
-      <c r="E25" s="83"/>
-      <c r="F25" s="84"/>
-      <c r="G25" s="80"/>
-      <c r="H25" s="80"/>
-      <c r="I25" s="80"/>
-      <c r="J25" s="80"/>
-      <c r="K25" s="80"/>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A26" s="80"/>
-      <c r="B26" s="81"/>
-      <c r="C26" s="102"/>
-      <c r="D26" s="102"/>
-      <c r="E26" s="83"/>
-      <c r="F26" s="84"/>
-      <c r="G26" s="80"/>
-      <c r="H26" s="80"/>
-      <c r="I26" s="80"/>
-      <c r="J26" s="80"/>
-      <c r="K26" s="80"/>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A27" s="80"/>
-      <c r="B27" s="81"/>
-      <c r="C27" s="122">
+      <c r="A23" s="78"/>
+      <c r="B23" s="79"/>
+      <c r="C23" s="117">
         <f>_xll.qlTermStructureReferenceDate(YieldCurve)</f>
-        <v>41598</v>
-      </c>
-      <c r="D27" s="123">
+        <v>41599</v>
+      </c>
+      <c r="D23" s="118">
         <f>MAX(_xll.ohPack(Selected!I1:I126))</f>
         <v>1</v>
       </c>
-      <c r="E27" s="83"/>
-      <c r="F27" s="84"/>
-      <c r="G27" s="80"/>
-      <c r="H27" s="80"/>
-      <c r="I27" s="80"/>
-      <c r="J27" s="80"/>
-      <c r="K27" s="80"/>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A28" s="80"/>
-      <c r="B28" s="81"/>
-      <c r="C28" s="124">
+      <c r="E23" s="81"/>
+      <c r="F23" s="82"/>
+      <c r="G23" s="78"/>
+      <c r="H23" s="78"/>
+      <c r="I23" s="78"/>
+      <c r="J23" s="78"/>
+      <c r="K23" s="78"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A24" s="78"/>
+      <c r="B24" s="79"/>
+      <c r="C24" s="119">
         <f>MAX(_xll.ohPack(Selected!H2:H126))</f>
-        <v>42328</v>
-      </c>
-      <c r="D28" s="94">
+        <v>42331</v>
+      </c>
+      <c r="D24" s="92">
         <f>MIN(_xll.ohPack(Selected!I1:I126))</f>
-        <v>0.98768738870458617</v>
-      </c>
-      <c r="E28" s="83"/>
-      <c r="F28" s="84"/>
-      <c r="G28" s="80"/>
-      <c r="H28" s="80"/>
-      <c r="I28" s="80"/>
-      <c r="J28" s="80"/>
-      <c r="K28" s="80"/>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A29" s="80"/>
-      <c r="B29" s="81"/>
-      <c r="C29" s="125" t="s">
+        <v>0.98764373182174425</v>
+      </c>
+      <c r="E24" s="81"/>
+      <c r="F24" s="82"/>
+      <c r="G24" s="78"/>
+      <c r="H24" s="78"/>
+      <c r="I24" s="78"/>
+      <c r="J24" s="78"/>
+      <c r="K24" s="78"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A25" s="78"/>
+      <c r="B25" s="79"/>
+      <c r="C25" s="120" t="s">
         <v>15</v>
       </c>
-      <c r="D29" s="126" t="str">
+      <c r="D25" s="121" t="str">
         <f>_xll.ohRangeRetrieveError(Selected!I1)</f>
         <v/>
       </c>
-      <c r="E29" s="83"/>
-      <c r="F29" s="84"/>
-      <c r="G29" s="80"/>
-      <c r="H29" s="80"/>
-      <c r="I29" s="80"/>
-      <c r="J29" s="80"/>
-      <c r="K29" s="80"/>
-    </row>
-    <row r="30" spans="1:11" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="80"/>
-      <c r="B30" s="127"/>
-      <c r="C30" s="128"/>
-      <c r="D30" s="129">
+      <c r="E25" s="81"/>
+      <c r="F25" s="82"/>
+      <c r="G25" s="78"/>
+      <c r="H25" s="78"/>
+      <c r="I25" s="78"/>
+      <c r="J25" s="78"/>
+      <c r="K25" s="78"/>
+    </row>
+    <row r="26" spans="1:11" ht="12" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="78"/>
+      <c r="B26" s="122"/>
+      <c r="C26" s="123"/>
+      <c r="D26" s="124">
         <v>0.98768738899999997</v>
       </c>
-      <c r="E30" s="128"/>
-      <c r="F30" s="130"/>
-      <c r="G30" s="80"/>
-      <c r="H30" s="80"/>
-      <c r="I30" s="80"/>
-      <c r="J30" s="80"/>
-      <c r="K30" s="80"/>
+      <c r="E26" s="123"/>
+      <c r="F26" s="125"/>
+      <c r="G26" s="78"/>
+      <c r="H26" s="78"/>
+      <c r="I26" s="78"/>
+      <c r="J26" s="78"/>
+      <c r="K26" s="78"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A27" s="78"/>
+      <c r="G27" s="78"/>
+      <c r="H27" s="78"/>
+      <c r="I27" s="78"/>
+      <c r="J27" s="78"/>
+      <c r="K27" s="78"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A28" s="78"/>
+      <c r="G28" s="78"/>
+      <c r="H28" s="78"/>
+      <c r="I28" s="78"/>
+      <c r="J28" s="78"/>
+      <c r="K28" s="78"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A29" s="78"/>
+      <c r="G29" s="78"/>
+      <c r="H29" s="78"/>
+      <c r="I29" s="78"/>
+      <c r="J29" s="78"/>
+      <c r="K29" s="78"/>
+    </row>
+    <row r="30" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="78"/>
+      <c r="G30" s="78"/>
+      <c r="H30" s="78"/>
+      <c r="I30" s="78"/>
+      <c r="J30" s="78"/>
+      <c r="K30" s="78"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -2319,21 +2253,18 @@
     <mergeCell ref="H12:K12"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
-  <dataValidations count="7">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D19">
+  <dataValidations count="6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D15">
       <formula1>"Actual/Actual (ISDA),Actual/360,30/360 (Bond Basis),30E/360 (Eurobond Basis),Actual/365 (Fixed),Actual/Actual (ISMA),Actual/Actual (AFB),'1/1,30/360 (Italian),Simple"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D24">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D20">
       <formula1>"Discount,ZeroYield,ForwardRate"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5">
       <formula1>"1D,1W,1M,2M,3M,6M,1Y"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D25">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D21">
       <formula1>"Linear,BackwardFlat,ForwardFlat,Linear,LogLinear,CubicNaturalSpline,LogCubicNaturalSpline,MonotonicCubicNaturalSpline,MonotonicLogCubicNaturalSpline,FritschButlandCubic,FritschButlandLogCubic,KrugerCubic,KrugerLogCubic"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D4">
-      <formula1>"EUR,USD,GBP,JPY,CHF,HKD"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J14">
       <formula1>"EUR,USD,GBP,JPY,CHF,HKD,CHY,AUD,PLN,HUF"</formula1>
@@ -2408,9 +2339,9 @@
         <f>$H$1&amp;"_FRAs.xml"</f>
         <v>HKD_YC6MRH_FRAs.xml</v>
       </c>
-      <c r="I2" s="62" t="e">
+      <c r="I2" s="62">
         <f ca="1">IF(Serialize,_xll.ohObjectSave(I3:I22,SerializationPath&amp;H2,FileOverwrite,,Serialize),"---")</f>
-        <v>#VALUE!</v>
+        <v>20</v>
       </c>
       <c r="J2" s="61" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(I2)</f>
@@ -3265,11 +3196,11 @@
       </c>
       <c r="G2" s="5">
         <f>_xll.qlRateHelperEarliestDate($A2,Trigger)</f>
-        <v>41628</v>
+        <v>41631</v>
       </c>
       <c r="H2" s="11">
         <f>_xll.qlRateHelperLatestDate($A2,Trigger)</f>
-        <v>41810</v>
+        <v>41813</v>
       </c>
       <c r="I2" s="76">
         <v>10</v>
@@ -3298,7 +3229,7 @@
       </c>
       <c r="G3" s="5">
         <f>_xll.qlRateHelperEarliestDate($A3,Trigger)</f>
-        <v>41659</v>
+        <v>41660</v>
       </c>
       <c r="H3" s="11">
         <f>_xll.qlRateHelperLatestDate($A3,Trigger)</f>
@@ -3331,11 +3262,11 @@
       </c>
       <c r="G4" s="5">
         <f>_xll.qlRateHelperEarliestDate($A4,Trigger)</f>
-        <v>41690</v>
+        <v>41691</v>
       </c>
       <c r="H4" s="11">
         <f>_xll.qlRateHelperLatestDate($A4,Trigger)</f>
-        <v>41871</v>
+        <v>41872</v>
       </c>
       <c r="I4" s="76">
         <v>30</v>
@@ -3364,7 +3295,7 @@
       </c>
       <c r="G5" s="5">
         <f>_xll.qlRateHelperEarliestDate($A5,Trigger)</f>
-        <v>41718</v>
+        <v>41719</v>
       </c>
       <c r="H5" s="11">
         <f>_xll.qlRateHelperLatestDate($A5,Trigger)</f>
@@ -3430,11 +3361,11 @@
       </c>
       <c r="G7" s="5">
         <f>_xll.qlRateHelperEarliestDate($A7,Trigger)</f>
-        <v>41779</v>
+        <v>41780</v>
       </c>
       <c r="H7" s="11">
         <f>_xll.qlRateHelperLatestDate($A7,Trigger)</f>
-        <v>41963</v>
+        <v>41964</v>
       </c>
       <c r="I7" s="76">
         <v>60</v>
@@ -3463,11 +3394,11 @@
       </c>
       <c r="G8" s="5">
         <f>_xll.qlRateHelperEarliestDate($A8,Trigger)</f>
-        <v>41810</v>
+        <v>41813</v>
       </c>
       <c r="H8" s="11">
         <f>_xll.qlRateHelperLatestDate($A8,Trigger)</f>
-        <v>41995</v>
+        <v>41996</v>
       </c>
       <c r="I8" s="76">
         <v>70</v>
@@ -3523,11 +3454,11 @@
       </c>
       <c r="G10" s="5">
         <f>_xll.qlRateHelperEarliestDate($A10,Trigger)</f>
-        <v>41871</v>
+        <v>41872</v>
       </c>
       <c r="H10" s="11">
         <f>_xll.qlRateHelperLatestDate($A10,Trigger)</f>
-        <v>42055</v>
+        <v>42058</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
@@ -3577,11 +3508,11 @@
       </c>
       <c r="G12" s="5">
         <f>_xll.qlRateHelperEarliestDate($A12,Trigger)</f>
-        <v>41932</v>
+        <v>41933</v>
       </c>
       <c r="H12" s="11">
         <f>_xll.qlRateHelperLatestDate($A12,Trigger)</f>
-        <v>42114</v>
+        <v>42115</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
@@ -3604,11 +3535,11 @@
       </c>
       <c r="G13" s="5">
         <f>_xll.qlRateHelperEarliestDate($A13,Trigger)</f>
-        <v>41963</v>
+        <v>41964</v>
       </c>
       <c r="H13" s="11">
         <f>_xll.qlRateHelperLatestDate($A13,Trigger)</f>
-        <v>42144</v>
+        <v>42145</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
@@ -3658,11 +3589,11 @@
       </c>
       <c r="G15" s="5">
         <f>_xll.qlRateHelperEarliestDate($A15,Trigger)</f>
-        <v>42024</v>
+        <v>42025</v>
       </c>
       <c r="H15" s="11">
         <f>_xll.qlRateHelperLatestDate($A15,Trigger)</f>
-        <v>42205</v>
+        <v>42206</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
@@ -3685,11 +3616,11 @@
       </c>
       <c r="G16" s="5">
         <f>_xll.qlRateHelperEarliestDate($A16,Trigger)</f>
-        <v>42055</v>
+        <v>42058</v>
       </c>
       <c r="H16" s="11">
         <f>_xll.qlRateHelperLatestDate($A16,Trigger)</f>
-        <v>42236</v>
+        <v>42240</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
@@ -3712,11 +3643,11 @@
       </c>
       <c r="G17" s="5">
         <f>_xll.qlRateHelperEarliestDate($A17,Trigger)</f>
-        <v>42083</v>
+        <v>42086</v>
       </c>
       <c r="H17" s="11">
         <f>_xll.qlRateHelperLatestDate($A17,Trigger)</f>
-        <v>42268</v>
+        <v>42270</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
@@ -3739,11 +3670,11 @@
       </c>
       <c r="G18" s="5">
         <f>_xll.qlRateHelperEarliestDate($A18,Trigger)</f>
-        <v>42114</v>
+        <v>42115</v>
       </c>
       <c r="H18" s="11">
         <f>_xll.qlRateHelperLatestDate($A18,Trigger)</f>
-        <v>42297</v>
+        <v>42298</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
@@ -3766,11 +3697,11 @@
       </c>
       <c r="G19" s="9">
         <f>_xll.qlRateHelperEarliestDate($A19,Trigger)</f>
-        <v>42144</v>
+        <v>42145</v>
       </c>
       <c r="H19" s="12">
         <f>_xll.qlRateHelperLatestDate($A19,Trigger)</f>
-        <v>42328</v>
+        <v>42331</v>
       </c>
     </row>
   </sheetData>
@@ -3807,10 +3738,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="129" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="78"/>
+      <c r="B1" s="130"/>
       <c r="D1" s="15" t="s">
         <v>20</v>
       </c>
@@ -3856,14 +3787,14 @@
       </c>
       <c r="G2" s="23">
         <f>_xll.qlRateHelperEarliestDate($D2)</f>
-        <v>41628</v>
+        <v>41631</v>
       </c>
       <c r="H2" s="24">
         <f>_xll.qlRateHelperLatestDate($D2)</f>
-        <v>41810</v>
+        <v>41813</v>
       </c>
       <c r="I2" s="18">
-        <v>0.99716148001926685</v>
+        <v>0.99713473992907398</v>
       </c>
       <c r="K2" s="22">
         <v>4.8999999999999998E-3</v>
@@ -3895,14 +3826,14 @@
       </c>
       <c r="G3" s="23">
         <f>_xll.qlRateHelperEarliestDate($D3)</f>
-        <v>41659</v>
+        <v>41660</v>
       </c>
       <c r="H3" s="24">
         <f>_xll.qlRateHelperLatestDate($D3)</f>
         <v>41841</v>
       </c>
       <c r="I3" s="18">
-        <v>0.99674708919205179</v>
+        <v>0.99676043774521694</v>
       </c>
       <c r="K3" s="22">
         <v>4.8999999999999998E-3</v>
@@ -3934,14 +3865,14 @@
       </c>
       <c r="G4" s="23">
         <f>_xll.qlRateHelperEarliestDate($D4)</f>
-        <v>41690</v>
+        <v>41691</v>
       </c>
       <c r="H4" s="24">
         <f>_xll.qlRateHelperLatestDate($D4)</f>
-        <v>41871</v>
+        <v>41872</v>
       </c>
       <c r="I4" s="18">
-        <v>0.99629692792739299</v>
+        <v>0.99629692792739322</v>
       </c>
       <c r="K4" s="22">
         <v>5.0000000000000001E-3</v>
@@ -3973,14 +3904,14 @@
       </c>
       <c r="G5" s="23">
         <f>_xll.qlRateHelperEarliestDate($D5)</f>
-        <v>41718</v>
+        <v>41719</v>
       </c>
       <c r="H5" s="24">
         <f>_xll.qlRateHelperLatestDate($D5)</f>
         <v>41904</v>
       </c>
       <c r="I5" s="18">
-        <v>0.99575368878051163</v>
+        <v>0.99576783756968001</v>
       </c>
       <c r="K5" s="22">
         <v>5.1999999999999998E-3</v>
@@ -4020,7 +3951,7 @@
         <v>41934</v>
       </c>
       <c r="I6" s="18">
-        <v>0.99530584866957905</v>
+        <v>0.99531919410258307</v>
       </c>
       <c r="K6" s="22">
         <v>5.3E-3</v>
@@ -4032,7 +3963,7 @@
     <row r="7" spans="1:12" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="29" t="str">
         <f>_xll.ohGroup(RateHelperPrefix&amp;"_RateHelpersSelected",_xll.ohPack(Selected!D2:D126),TRUE,,ObjectOverwrite)</f>
-        <v>HKD_YC6MRH_RateHelpersSelected#0001</v>
+        <v>HKD_YC6MRH_RateHelpersSelected#0003</v>
       </c>
       <c r="B7" s="30" t="str">
         <f>_xll.ohRangeRetrieveError(RateHelpersSelected)</f>
@@ -4054,11 +3985,11 @@
       </c>
       <c r="G7" s="23">
         <f>_xll.qlRateHelperEarliestDate($D7)</f>
-        <v>41779</v>
+        <v>41780</v>
       </c>
       <c r="H7" s="24">
         <f>_xll.qlRateHelperLatestDate($D7)</f>
-        <v>41963</v>
+        <v>41964</v>
       </c>
       <c r="I7" s="18">
         <v>0.99486782211827718</v>
@@ -4087,11 +4018,11 @@
       </c>
       <c r="G8" s="23">
         <f>_xll.qlRateHelperEarliestDate($D8)</f>
-        <v>41963</v>
+        <v>41964</v>
       </c>
       <c r="H8" s="24">
         <f>_xll.qlRateHelperLatestDate($D8)</f>
-        <v>42144</v>
+        <v>42145</v>
       </c>
       <c r="I8" s="18">
         <v>0.99172040044191578</v>
@@ -4120,14 +4051,14 @@
       </c>
       <c r="G9" s="23">
         <f>_xll.qlRateHelperEarliestDate($D9)</f>
-        <v>42144</v>
+        <v>42145</v>
       </c>
       <c r="H9" s="24">
         <f>_xll.qlRateHelperLatestDate($D9)</f>
-        <v>42328</v>
+        <v>42331</v>
       </c>
       <c r="I9" s="18">
-        <v>0.98768738870458617</v>
+        <v>0.98764373182174425</v>
       </c>
       <c r="K9" s="22">
         <v>8.0999999999999996E-3</v>

</xml_diff>

<commit_message>
reduce the size of the ratehelper selected range
</commit_message>
<xml_diff>
--- a/QuantLibXL/Data2/XLS/HKD_YC6MBootstrapping.xlsx
+++ b/QuantLibXL/Data2/XLS/HKD_YC6MBootstrapping.xlsx
@@ -1110,7 +1110,7 @@
     <xf numFmtId="173" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="173" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="133">
+  <cellXfs count="135">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1385,6 +1385,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="10" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="33" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1398,10 +1402,10 @@
     <xf numFmtId="0" fontId="8" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="10">
     <cellStyle name="Migliaia (0)_AZIONI" xfId="4"/>
@@ -1748,20 +1752,20 @@
     </row>
     <row r="2" spans="1:11" ht="18" x14ac:dyDescent="0.25">
       <c r="A2" s="78"/>
-      <c r="B2" s="126" t="s">
+      <c r="B2" s="128" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="127"/>
-      <c r="D2" s="127"/>
-      <c r="E2" s="127"/>
-      <c r="F2" s="128"/>
+      <c r="C2" s="129"/>
+      <c r="D2" s="129"/>
+      <c r="E2" s="129"/>
+      <c r="F2" s="130"/>
       <c r="G2" s="78"/>
-      <c r="H2" s="126" t="s">
+      <c r="H2" s="128" t="s">
         <v>68</v>
       </c>
-      <c r="I2" s="127"/>
-      <c r="J2" s="127"/>
-      <c r="K2" s="127"/>
+      <c r="I2" s="129"/>
+      <c r="J2" s="129"/>
+      <c r="K2" s="129"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="78"/>
@@ -1782,7 +1786,7 @@
       <c r="C4" s="86" t="s">
         <v>38</v>
       </c>
-      <c r="D4" s="131">
+      <c r="D4" s="126">
         <v>6</v>
       </c>
       <c r="E4" s="81"/>
@@ -1793,7 +1797,7 @@
         <v>6</v>
       </c>
       <c r="J4" s="89">
-        <v>41598.740243055552</v>
+        <v>41599.394988425927</v>
       </c>
       <c r="K4" s="90"/>
     </row>
@@ -1864,7 +1868,7 @@
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="78"/>
       <c r="B8" s="79"/>
-      <c r="C8" s="132" t="s">
+      <c r="C8" s="127" t="s">
         <v>23</v>
       </c>
       <c r="D8" s="96" t="str">
@@ -1909,7 +1913,7 @@
       </c>
       <c r="D10" s="89" t="str">
         <f>_xll.qlPiecewiseYieldCurve(D12,NDays,Calendar,RateHelpersSelected,DayCounter,IF(ISERROR(D18),NA(),D16:E16),IF(ISERROR(D18),NA(),D17:E17),Accuracy,TraitsID,InterpolatorID,Permanent,,ObjectOverwrite)</f>
-        <v>_HKDYC6M#0003</v>
+        <v>_HKDYC6M#0001</v>
       </c>
       <c r="E10" s="81"/>
       <c r="F10" s="82"/>
@@ -1950,12 +1954,12 @@
       <c r="E12" s="81"/>
       <c r="F12" s="82"/>
       <c r="G12" s="78"/>
-      <c r="H12" s="126" t="s">
+      <c r="H12" s="128" t="s">
         <v>64</v>
       </c>
-      <c r="I12" s="127"/>
-      <c r="J12" s="127"/>
-      <c r="K12" s="127"/>
+      <c r="I12" s="129"/>
+      <c r="J12" s="129"/>
+      <c r="K12" s="129"/>
     </row>
     <row r="13" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="78"/>
@@ -2151,7 +2155,7 @@
         <v>41599</v>
       </c>
       <c r="D23" s="118">
-        <f>MAX(_xll.ohPack(Selected!I1:I126))</f>
+        <f>MAX(_xll.ohPack(Selected!I1:I20))</f>
         <v>1</v>
       </c>
       <c r="E23" s="81"/>
@@ -2166,11 +2170,11 @@
       <c r="A24" s="78"/>
       <c r="B24" s="79"/>
       <c r="C24" s="119">
-        <f>MAX(_xll.ohPack(Selected!H2:H126))</f>
+        <f>MAX(_xll.ohPack(Selected!H2:H20))</f>
         <v>42331</v>
       </c>
       <c r="D24" s="92">
-        <f>MIN(_xll.ohPack(Selected!I1:I126))</f>
+        <f>MIN(_xll.ohPack(Selected!I1:I20))</f>
         <v>0.98764373182174425</v>
       </c>
       <c r="E24" s="81"/>
@@ -2378,7 +2382,7 @@
       </c>
       <c r="I3" s="52" t="str">
         <f>_xll.qlFraRateHelper(H3,G3,B3,E3,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC6MRH_T6F1#0003</v>
+        <v>HKD_YC6MRH_T6F1#0000</v>
       </c>
       <c r="J3" s="61" t="str">
         <f>_xll.ohRangeRetrieveError(I3)</f>
@@ -2415,7 +2419,7 @@
       </c>
       <c r="I4" s="57" t="str">
         <f>_xll.qlFraRateHelper(H4,G4,B4,E4,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC6MRH_TOM6F1#0003</v>
+        <v>HKD_YC6MRH_TOM6F1#0000</v>
       </c>
       <c r="J4" s="56" t="str">
         <f>_xll.ohRangeRetrieveError(I4)</f>
@@ -2453,7 +2457,7 @@
       </c>
       <c r="I5" s="52" t="str">
         <f>_xll.qlFraRateHelper(H5,G5,B5,E5,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC6MRH_1x7F#0003</v>
+        <v>HKD_YC6MRH_1x7F#0000</v>
       </c>
       <c r="J5" s="51" t="str">
         <f>_xll.ohRangeRetrieveError(I5)</f>
@@ -2491,7 +2495,7 @@
       </c>
       <c r="I6" s="46" t="str">
         <f>_xll.qlFraRateHelper(H6,G6,B6,E6,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC6MRH_2x8F#0003</v>
+        <v>HKD_YC6MRH_2x8F#0000</v>
       </c>
       <c r="J6" s="45" t="str">
         <f>_xll.ohRangeRetrieveError(I6)</f>
@@ -2529,7 +2533,7 @@
       </c>
       <c r="I7" s="46" t="str">
         <f>_xll.qlFraRateHelper(H7,G7,B7,E7,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC6MRH_3x9F#0003</v>
+        <v>HKD_YC6MRH_3x9F#0000</v>
       </c>
       <c r="J7" s="45" t="str">
         <f>_xll.ohRangeRetrieveError(I7)</f>
@@ -2567,7 +2571,7 @@
       </c>
       <c r="I8" s="46" t="str">
         <f>_xll.qlFraRateHelper(H8,G8,B8,E8,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC6MRH_4x10F#0003</v>
+        <v>HKD_YC6MRH_4x10F#0000</v>
       </c>
       <c r="J8" s="45" t="str">
         <f>_xll.ohRangeRetrieveError(I8)</f>
@@ -2605,7 +2609,7 @@
       </c>
       <c r="I9" s="46" t="str">
         <f>_xll.qlFraRateHelper(H9,G9,B9,E9,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC6MRH_5x11F#0003</v>
+        <v>HKD_YC6MRH_5x11F#0000</v>
       </c>
       <c r="J9" s="45" t="str">
         <f>_xll.ohRangeRetrieveError(I9)</f>
@@ -2643,7 +2647,7 @@
       </c>
       <c r="I10" s="46" t="str">
         <f>_xll.qlFraRateHelper(H10,G10,B10,E10,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC6MRH_6x12F#0003</v>
+        <v>HKD_YC6MRH_6x12F#0000</v>
       </c>
       <c r="J10" s="45" t="str">
         <f>_xll.ohRangeRetrieveError(I10)</f>
@@ -2681,7 +2685,7 @@
       </c>
       <c r="I11" s="46" t="str">
         <f>_xll.qlFraRateHelper(H11,G11,B11,E11,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC6MRH_7x13F#0003</v>
+        <v>HKD_YC6MRH_7x13F#0000</v>
       </c>
       <c r="J11" s="45" t="str">
         <f>_xll.ohRangeRetrieveError(I11)</f>
@@ -2719,7 +2723,7 @@
       </c>
       <c r="I12" s="46" t="str">
         <f>_xll.qlFraRateHelper(H12,G12,B12,E12,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC6MRH_8x14F#0003</v>
+        <v>HKD_YC6MRH_8x14F#0000</v>
       </c>
       <c r="J12" s="45" t="str">
         <f>_xll.ohRangeRetrieveError(I12)</f>
@@ -2757,7 +2761,7 @@
       </c>
       <c r="I13" s="46" t="str">
         <f>_xll.qlFraRateHelper(H13,G13,B13,E13,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC6MRH_9x15F#0003</v>
+        <v>HKD_YC6MRH_9x15F#0000</v>
       </c>
       <c r="J13" s="45" t="str">
         <f>_xll.ohRangeRetrieveError(I13)</f>
@@ -2795,7 +2799,7 @@
       </c>
       <c r="I14" s="46" t="str">
         <f>_xll.qlFraRateHelper(H14,G14,B14,E14,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC6MRH_10x16F#0003</v>
+        <v>HKD_YC6MRH_10x16F#0000</v>
       </c>
       <c r="J14" s="45" t="str">
         <f>_xll.ohRangeRetrieveError(I14)</f>
@@ -2833,7 +2837,7 @@
       </c>
       <c r="I15" s="46" t="str">
         <f>_xll.qlFraRateHelper(H15,G15,B15,E15,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC6MRH_11x17F#0003</v>
+        <v>HKD_YC6MRH_11x17F#0000</v>
       </c>
       <c r="J15" s="45" t="str">
         <f>_xll.ohRangeRetrieveError(I15)</f>
@@ -2871,7 +2875,7 @@
       </c>
       <c r="I16" s="46" t="str">
         <f>_xll.qlFraRateHelper(H16,G16,B16,E16,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC6MRH_12x18F#0003</v>
+        <v>HKD_YC6MRH_12x18F#0000</v>
       </c>
       <c r="J16" s="45" t="str">
         <f>_xll.ohRangeRetrieveError(I16)</f>
@@ -2909,7 +2913,7 @@
       </c>
       <c r="I17" s="46" t="str">
         <f>_xll.qlFraRateHelper(H17,G17,B17,E17,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC6MRH_13x19F#0003</v>
+        <v>HKD_YC6MRH_13x19F#0000</v>
       </c>
       <c r="J17" s="45" t="str">
         <f>_xll.ohRangeRetrieveError(I17)</f>
@@ -2947,7 +2951,7 @@
       </c>
       <c r="I18" s="46" t="str">
         <f>_xll.qlFraRateHelper(H18,G18,B18,E18,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC6MRH_14x20F#0003</v>
+        <v>HKD_YC6MRH_14x20F#0000</v>
       </c>
       <c r="J18" s="45" t="str">
         <f>_xll.ohRangeRetrieveError(I18)</f>
@@ -2985,7 +2989,7 @@
       </c>
       <c r="I19" s="46" t="str">
         <f>_xll.qlFraRateHelper(H19,G19,B19,E19,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC6MRH_15x21F#0003</v>
+        <v>HKD_YC6MRH_15x21F#0000</v>
       </c>
       <c r="J19" s="45" t="str">
         <f>_xll.ohRangeRetrieveError(I19)</f>
@@ -3023,7 +3027,7 @@
       </c>
       <c r="I20" s="46" t="str">
         <f>_xll.qlFraRateHelper(H20,G20,B20,E20,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC6MRH_16x22F#0003</v>
+        <v>HKD_YC6MRH_16x22F#0000</v>
       </c>
       <c r="J20" s="45" t="str">
         <f>_xll.ohRangeRetrieveError(I20)</f>
@@ -3061,7 +3065,7 @@
       </c>
       <c r="I21" s="46" t="str">
         <f>_xll.qlFraRateHelper(H21,G21,B21,E21,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC6MRH_17x23F#0003</v>
+        <v>HKD_YC6MRH_17x23F#0000</v>
       </c>
       <c r="J21" s="45" t="str">
         <f>_xll.ohRangeRetrieveError(I21)</f>
@@ -3099,7 +3103,7 @@
       </c>
       <c r="I22" s="46" t="str">
         <f>_xll.qlFraRateHelper(H22,G22,B22,E22,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC6MRH_18x24F#0003</v>
+        <v>HKD_YC6MRH_18x24F#0000</v>
       </c>
       <c r="J22" s="45" t="str">
         <f>_xll.ohRangeRetrieveError(I22)</f>
@@ -3716,7 +3720,7 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:L126"/>
+  <dimension ref="A1:L22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:B1"/>
@@ -3738,10 +3742,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="129" t="s">
+      <c r="A1" s="131" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="130"/>
+      <c r="B1" s="132"/>
       <c r="D1" s="15" t="s">
         <v>20</v>
       </c>
@@ -3756,7 +3760,7 @@
         <v>1</v>
       </c>
       <c r="I1" s="18">
-        <f t="array" ref="I1:I126">_xll.qlPiecewiseYieldCurveData(YieldCurve)</f>
+        <f t="array" ref="I1:I20">_xll.qlPiecewiseYieldCurveData(YieldCurve)</f>
         <v>1</v>
       </c>
       <c r="L1" s="18">
@@ -3774,7 +3778,7 @@
         <v>52</v>
       </c>
       <c r="D2" s="21" t="str">
-        <f t="array" ref="D2:D126">_xll.qlRateHelperSelection(_xll.ohFilter(RateHelpers,RateHelpersIncluded),_xll.ohFilter(RateHelpersPriority,RateHelpersIncluded),nIMMFutures,nSerialFutures,FrontFuturesRollingDays,DepoInclusionCriteria,_xll.ohFilter(MinDistance,RateHelpersIncluded),Trigger)</f>
+        <f t="array" ref="D2:D20">_xll.qlRateHelperSelection(_xll.ohFilter(RateHelpers,RateHelpersIncluded),_xll.ohFilter(RateHelpersPriority,RateHelpersIncluded),nIMMFutures,nSerialFutures,FrontFuturesRollingDays,DepoInclusionCriteria,_xll.ohFilter(MinDistance,RateHelpersIncluded),Trigger)</f>
         <v>HKD_YC6MRH_1x7F</v>
       </c>
       <c r="E2" s="22">
@@ -3962,7 +3966,7 @@
     </row>
     <row r="7" spans="1:12" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="29" t="str">
-        <f>_xll.ohGroup(RateHelperPrefix&amp;"_RateHelpersSelected",_xll.ohPack(Selected!D2:D126),TRUE,,ObjectOverwrite)</f>
+        <f>_xll.ohGroup(RateHelperPrefix&amp;"_RateHelpersSelected",_xll.ohPack(Selected!D2:D20),TRUE,,ObjectOverwrite)</f>
         <v>HKD_YC6MRH_RateHelpersSelected#0003</v>
       </c>
       <c r="B7" s="30" t="str">
@@ -4307,23 +4311,23 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="20" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D20" s="21" t="e">
+    <row r="20" spans="4:9" ht="12" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D20" s="31" t="e">
         <v>#N/A</v>
       </c>
-      <c r="E20" s="22" t="e">
+      <c r="E20" s="32" t="e">
         <f>_xll.qlRateHelperRate($D20)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="F20" s="22" t="str">
+      <c r="F20" s="32" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D20)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D20)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D20)),_xll.qlSwapRateHelperSpread($D20))</f>
         <v>--</v>
       </c>
-      <c r="G20" s="23" t="e">
+      <c r="G20" s="33" t="e">
         <f>_xll.qlRateHelperEarliestDate($D20)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="H20" s="24" t="e">
+      <c r="H20" s="34" t="e">
         <f>_xll.qlRateHelperLatestDate($D20)</f>
         <v>#VALUE!</v>
       </c>
@@ -4331,2549 +4335,9 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="21" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D21" s="21" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E21" s="22" t="e">
-        <f>_xll.qlRateHelperRate($D21)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F21" s="22" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D21)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D21)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D21)),_xll.qlSwapRateHelperSpread($D21))</f>
-        <v>--</v>
-      </c>
-      <c r="G21" s="23" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D21)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H21" s="24" t="e">
-        <f>_xll.qlRateHelperLatestDate($D21)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I21" s="18" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
     <row r="22" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D22" s="21" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E22" s="22" t="e">
-        <f>_xll.qlRateHelperRate($D22)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F22" s="22" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D22)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D22)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D22)),_xll.qlSwapRateHelperSpread($D22))</f>
-        <v>--</v>
-      </c>
-      <c r="G22" s="23" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D22)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H22" s="24" t="e">
-        <f>_xll.qlRateHelperLatestDate($D22)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I22" s="18" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="23" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D23" s="21" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E23" s="22" t="e">
-        <f>_xll.qlRateHelperRate($D23)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F23" s="22" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D23)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D23)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D23)),_xll.qlSwapRateHelperSpread($D23))</f>
-        <v>--</v>
-      </c>
-      <c r="G23" s="23" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D23)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H23" s="24" t="e">
-        <f>_xll.qlRateHelperLatestDate($D23)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I23" s="18" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="24" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D24" s="21" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E24" s="22" t="e">
-        <f>_xll.qlRateHelperRate($D24)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F24" s="22" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D24)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D24)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D24)),_xll.qlSwapRateHelperSpread($D24))</f>
-        <v>--</v>
-      </c>
-      <c r="G24" s="23" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D24)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H24" s="24" t="e">
-        <f>_xll.qlRateHelperLatestDate($D24)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I24" s="18" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="25" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D25" s="21" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E25" s="22" t="e">
-        <f>_xll.qlRateHelperRate($D25)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F25" s="22" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D25)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D25)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D25)),_xll.qlSwapRateHelperSpread($D25))</f>
-        <v>--</v>
-      </c>
-      <c r="G25" s="23" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D25)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H25" s="24" t="e">
-        <f>_xll.qlRateHelperLatestDate($D25)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I25" s="18" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="26" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D26" s="21" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E26" s="22" t="e">
-        <f>_xll.qlRateHelperRate($D26)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F26" s="22" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D26)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D26)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D26)),_xll.qlSwapRateHelperSpread($D26))</f>
-        <v>--</v>
-      </c>
-      <c r="G26" s="23" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D26)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H26" s="24" t="e">
-        <f>_xll.qlRateHelperLatestDate($D26)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I26" s="18" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="27" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D27" s="21" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E27" s="22" t="e">
-        <f>_xll.qlRateHelperRate($D27)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F27" s="22" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D27)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D27)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D27)),_xll.qlSwapRateHelperSpread($D27))</f>
-        <v>--</v>
-      </c>
-      <c r="G27" s="23" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D27)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H27" s="24" t="e">
-        <f>_xll.qlRateHelperLatestDate($D27)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I27" s="18" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="28" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D28" s="21" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E28" s="22" t="e">
-        <f>_xll.qlRateHelperRate($D28)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F28" s="22" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D28)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D28)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D28)),_xll.qlSwapRateHelperSpread($D28))</f>
-        <v>--</v>
-      </c>
-      <c r="G28" s="23" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D28)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H28" s="24" t="e">
-        <f>_xll.qlRateHelperLatestDate($D28)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I28" s="18" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="29" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D29" s="21" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E29" s="22" t="e">
-        <f>_xll.qlRateHelperRate($D29)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F29" s="22" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D29)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D29)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D29)),_xll.qlSwapRateHelperSpread($D29))</f>
-        <v>--</v>
-      </c>
-      <c r="G29" s="23" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D29)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H29" s="24" t="e">
-        <f>_xll.qlRateHelperLatestDate($D29)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I29" s="18" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="30" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D30" s="21" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E30" s="22" t="e">
-        <f>_xll.qlRateHelperRate($D30)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F30" s="22" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D30)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D30)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D30)),_xll.qlSwapRateHelperSpread($D30))</f>
-        <v>--</v>
-      </c>
-      <c r="G30" s="23" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D30)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H30" s="24" t="e">
-        <f>_xll.qlRateHelperLatestDate($D30)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I30" s="18" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="31" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D31" s="21" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E31" s="22" t="e">
-        <f>_xll.qlRateHelperRate($D31)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F31" s="22" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D31)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D31)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D31)),_xll.qlSwapRateHelperSpread($D31))</f>
-        <v>--</v>
-      </c>
-      <c r="G31" s="23" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D31)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H31" s="24" t="e">
-        <f>_xll.qlRateHelperLatestDate($D31)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I31" s="18" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="32" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D32" s="21" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E32" s="22" t="e">
-        <f>_xll.qlRateHelperRate($D32)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F32" s="22" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D32)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D32)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D32)),_xll.qlSwapRateHelperSpread($D32))</f>
-        <v>--</v>
-      </c>
-      <c r="G32" s="23" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D32)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H32" s="24" t="e">
-        <f>_xll.qlRateHelperLatestDate($D32)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I32" s="18" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="33" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D33" s="21" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E33" s="22" t="e">
-        <f>_xll.qlRateHelperRate($D33)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F33" s="22" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D33)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D33)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D33)),_xll.qlSwapRateHelperSpread($D33))</f>
-        <v>--</v>
-      </c>
-      <c r="G33" s="23" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D33)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H33" s="24" t="e">
-        <f>_xll.qlRateHelperLatestDate($D33)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I33" s="18" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="34" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D34" s="21" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E34" s="22" t="e">
-        <f>_xll.qlRateHelperRate($D34)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F34" s="22" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D34)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D34)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D34)),_xll.qlSwapRateHelperSpread($D34))</f>
-        <v>--</v>
-      </c>
-      <c r="G34" s="23" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D34)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H34" s="24" t="e">
-        <f>_xll.qlRateHelperLatestDate($D34)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I34" s="18" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="35" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D35" s="21" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E35" s="22" t="e">
-        <f>_xll.qlRateHelperRate($D35)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F35" s="22" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D35)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D35)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D35)),_xll.qlSwapRateHelperSpread($D35))</f>
-        <v>--</v>
-      </c>
-      <c r="G35" s="23" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D35)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H35" s="24" t="e">
-        <f>_xll.qlRateHelperLatestDate($D35)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I35" s="18" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="36" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D36" s="21" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E36" s="22" t="e">
-        <f>_xll.qlRateHelperRate($D36)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F36" s="22" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D36)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D36)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D36)),_xll.qlSwapRateHelperSpread($D36))</f>
-        <v>--</v>
-      </c>
-      <c r="G36" s="23" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D36)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H36" s="24" t="e">
-        <f>_xll.qlRateHelperLatestDate($D36)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I36" s="18" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="37" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D37" s="21" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E37" s="22" t="e">
-        <f>_xll.qlRateHelperRate($D37)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F37" s="22" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D37)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D37)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D37)),_xll.qlSwapRateHelperSpread($D37))</f>
-        <v>--</v>
-      </c>
-      <c r="G37" s="23" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D37)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H37" s="24" t="e">
-        <f>_xll.qlRateHelperLatestDate($D37)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I37" s="18" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="38" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D38" s="21" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E38" s="22" t="e">
-        <f>_xll.qlRateHelperRate($D38)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F38" s="22" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D38)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D38)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D38)),_xll.qlSwapRateHelperSpread($D38))</f>
-        <v>--</v>
-      </c>
-      <c r="G38" s="23" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D38)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H38" s="24" t="e">
-        <f>_xll.qlRateHelperLatestDate($D38)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I38" s="18" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="39" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D39" s="21" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E39" s="22" t="e">
-        <f>_xll.qlRateHelperRate($D39)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F39" s="22" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D39)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D39)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D39)),_xll.qlSwapRateHelperSpread($D39))</f>
-        <v>--</v>
-      </c>
-      <c r="G39" s="23" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D39)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H39" s="24" t="e">
-        <f>_xll.qlRateHelperLatestDate($D39)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I39" s="18" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="40" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D40" s="21" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E40" s="22" t="e">
-        <f>_xll.qlRateHelperRate($D40)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F40" s="22" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D40)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D40)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D40)),_xll.qlSwapRateHelperSpread($D40))</f>
-        <v>--</v>
-      </c>
-      <c r="G40" s="23" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D40)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H40" s="24" t="e">
-        <f>_xll.qlRateHelperLatestDate($D40)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I40" s="18" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="41" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D41" s="21" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E41" s="22" t="e">
-        <f>_xll.qlRateHelperRate($D41)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F41" s="22" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D41)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D41)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D41)),_xll.qlSwapRateHelperSpread($D41))</f>
-        <v>--</v>
-      </c>
-      <c r="G41" s="23" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D41)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H41" s="24" t="e">
-        <f>_xll.qlRateHelperLatestDate($D41)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I41" s="18" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="42" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D42" s="21" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E42" s="22" t="e">
-        <f>_xll.qlRateHelperRate($D42)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F42" s="22" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D42)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D42)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D42)),_xll.qlSwapRateHelperSpread($D42))</f>
-        <v>--</v>
-      </c>
-      <c r="G42" s="23" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D42)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H42" s="24" t="e">
-        <f>_xll.qlRateHelperLatestDate($D42)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I42" s="18" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="43" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D43" s="21" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E43" s="22" t="e">
-        <f>_xll.qlRateHelperRate($D43)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F43" s="22" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D43)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D43)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D43)),_xll.qlSwapRateHelperSpread($D43))</f>
-        <v>--</v>
-      </c>
-      <c r="G43" s="23" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D43)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H43" s="24" t="e">
-        <f>_xll.qlRateHelperLatestDate($D43)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I43" s="18" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="44" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D44" s="21" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E44" s="22" t="e">
-        <f>_xll.qlRateHelperRate($D44)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F44" s="22" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D44)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D44)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D44)),_xll.qlSwapRateHelperSpread($D44))</f>
-        <v>--</v>
-      </c>
-      <c r="G44" s="23" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D44)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H44" s="24" t="e">
-        <f>_xll.qlRateHelperLatestDate($D44)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I44" s="18" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="45" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D45" s="21" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E45" s="22" t="e">
-        <f>_xll.qlRateHelperRate($D45)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F45" s="22" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D45)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D45)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D45)),_xll.qlSwapRateHelperSpread($D45))</f>
-        <v>--</v>
-      </c>
-      <c r="G45" s="23" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D45)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H45" s="24" t="e">
-        <f>_xll.qlRateHelperLatestDate($D45)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I45" s="18" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="46" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D46" s="21" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E46" s="22" t="e">
-        <f>_xll.qlRateHelperRate($D46)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F46" s="22" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D46)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D46)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D46)),_xll.qlSwapRateHelperSpread($D46))</f>
-        <v>--</v>
-      </c>
-      <c r="G46" s="23" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D46)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H46" s="24" t="e">
-        <f>_xll.qlRateHelperLatestDate($D46)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I46" s="18" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="47" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D47" s="21" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E47" s="22" t="e">
-        <f>_xll.qlRateHelperRate($D47)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F47" s="22" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D47)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D47)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D47)),_xll.qlSwapRateHelperSpread($D47))</f>
-        <v>--</v>
-      </c>
-      <c r="G47" s="23" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D47)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H47" s="24" t="e">
-        <f>_xll.qlRateHelperLatestDate($D47)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I47" s="18" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="48" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D48" s="21" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E48" s="22" t="e">
-        <f>_xll.qlRateHelperRate($D48)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F48" s="22" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D48)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D48)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D48)),_xll.qlSwapRateHelperSpread($D48))</f>
-        <v>--</v>
-      </c>
-      <c r="G48" s="23" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D48)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H48" s="24" t="e">
-        <f>_xll.qlRateHelperLatestDate($D48)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I48" s="18" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="49" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D49" s="21" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E49" s="22" t="e">
-        <f>_xll.qlRateHelperRate($D49)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F49" s="22" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D49)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D49)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D49)),_xll.qlSwapRateHelperSpread($D49))</f>
-        <v>--</v>
-      </c>
-      <c r="G49" s="23" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D49)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H49" s="24" t="e">
-        <f>_xll.qlRateHelperLatestDate($D49)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I49" s="18" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="50" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D50" s="21" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E50" s="22" t="e">
-        <f>_xll.qlRateHelperRate($D50)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F50" s="22" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D50)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D50)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D50)),_xll.qlSwapRateHelperSpread($D50))</f>
-        <v>--</v>
-      </c>
-      <c r="G50" s="23" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D50)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H50" s="24" t="e">
-        <f>_xll.qlRateHelperLatestDate($D50)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I50" s="18" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="51" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D51" s="21" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E51" s="22" t="e">
-        <f>_xll.qlRateHelperRate($D51)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F51" s="22" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D51)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D51)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D51)),_xll.qlSwapRateHelperSpread($D51))</f>
-        <v>--</v>
-      </c>
-      <c r="G51" s="23" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D51)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H51" s="24" t="e">
-        <f>_xll.qlRateHelperLatestDate($D51)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I51" s="18" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="52" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D52" s="21" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E52" s="22" t="e">
-        <f>_xll.qlRateHelperRate($D52)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F52" s="22" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D52)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D52)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D52)),_xll.qlSwapRateHelperSpread($D52))</f>
-        <v>--</v>
-      </c>
-      <c r="G52" s="23" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D52)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H52" s="24" t="e">
-        <f>_xll.qlRateHelperLatestDate($D52)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I52" s="18" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="53" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D53" s="21" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E53" s="22" t="e">
-        <f>_xll.qlRateHelperRate($D53)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F53" s="22" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D53)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D53)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D53)),_xll.qlSwapRateHelperSpread($D53))</f>
-        <v>--</v>
-      </c>
-      <c r="G53" s="23" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D53)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H53" s="24" t="e">
-        <f>_xll.qlRateHelperLatestDate($D53)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I53" s="18" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="54" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D54" s="21" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E54" s="22" t="e">
-        <f>_xll.qlRateHelperRate($D54)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F54" s="22" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D54)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D54)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D54)),_xll.qlSwapRateHelperSpread($D54))</f>
-        <v>--</v>
-      </c>
-      <c r="G54" s="23" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D54)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H54" s="24" t="e">
-        <f>_xll.qlRateHelperLatestDate($D54)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I54" s="18" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="55" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D55" s="21" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E55" s="22" t="e">
-        <f>_xll.qlRateHelperRate($D55)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F55" s="22" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D55)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D55)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D55)),_xll.qlSwapRateHelperSpread($D55))</f>
-        <v>--</v>
-      </c>
-      <c r="G55" s="23" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D55)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H55" s="24" t="e">
-        <f>_xll.qlRateHelperLatestDate($D55)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I55" s="18" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="56" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D56" s="21" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E56" s="22" t="e">
-        <f>_xll.qlRateHelperRate($D56)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F56" s="22" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D56)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D56)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D56)),_xll.qlSwapRateHelperSpread($D56))</f>
-        <v>--</v>
-      </c>
-      <c r="G56" s="23" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D56)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H56" s="24" t="e">
-        <f>_xll.qlRateHelperLatestDate($D56)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I56" s="18" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="57" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D57" s="21" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E57" s="22" t="e">
-        <f>_xll.qlRateHelperRate($D57)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F57" s="22" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D57)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D57)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D57)),_xll.qlSwapRateHelperSpread($D57))</f>
-        <v>--</v>
-      </c>
-      <c r="G57" s="23" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D57)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H57" s="24" t="e">
-        <f>_xll.qlRateHelperLatestDate($D57)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I57" s="18" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="58" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D58" s="21" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E58" s="22" t="e">
-        <f>_xll.qlRateHelperRate($D58)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F58" s="22" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D58)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D58)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D58)),_xll.qlSwapRateHelperSpread($D58))</f>
-        <v>--</v>
-      </c>
-      <c r="G58" s="23" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D58)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H58" s="24" t="e">
-        <f>_xll.qlRateHelperLatestDate($D58)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I58" s="18" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="59" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D59" s="21" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E59" s="22" t="e">
-        <f>_xll.qlRateHelperRate($D59)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F59" s="22" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D59)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D59)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D59)),_xll.qlSwapRateHelperSpread($D59))</f>
-        <v>--</v>
-      </c>
-      <c r="G59" s="23" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D59)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H59" s="24" t="e">
-        <f>_xll.qlRateHelperLatestDate($D59)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I59" s="18" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="60" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D60" s="21" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E60" s="22" t="e">
-        <f>_xll.qlRateHelperRate($D60)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F60" s="22" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D60)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D60)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D60)),_xll.qlSwapRateHelperSpread($D60))</f>
-        <v>--</v>
-      </c>
-      <c r="G60" s="23" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D60)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H60" s="24" t="e">
-        <f>_xll.qlRateHelperLatestDate($D60)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I60" s="18" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="61" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D61" s="21" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E61" s="22" t="e">
-        <f>_xll.qlRateHelperRate($D61)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F61" s="22" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D61)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D61)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D61)),_xll.qlSwapRateHelperSpread($D61))</f>
-        <v>--</v>
-      </c>
-      <c r="G61" s="23" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D61)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H61" s="24" t="e">
-        <f>_xll.qlRateHelperLatestDate($D61)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I61" s="18" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="62" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D62" s="21" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E62" s="22" t="e">
-        <f>_xll.qlRateHelperRate($D62)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F62" s="22" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D62)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D62)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D62)),_xll.qlSwapRateHelperSpread($D62))</f>
-        <v>--</v>
-      </c>
-      <c r="G62" s="23" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D62)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H62" s="24" t="e">
-        <f>_xll.qlRateHelperLatestDate($D62)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I62" s="18" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="63" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D63" s="21" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E63" s="22" t="e">
-        <f>_xll.qlRateHelperRate($D63)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F63" s="22" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D63)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D63)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D63)),_xll.qlSwapRateHelperSpread($D63))</f>
-        <v>--</v>
-      </c>
-      <c r="G63" s="23" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D63)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H63" s="24" t="e">
-        <f>_xll.qlRateHelperLatestDate($D63)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I63" s="18" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="64" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D64" s="21" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E64" s="22" t="e">
-        <f>_xll.qlRateHelperRate($D64)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F64" s="22" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D64)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D64)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D64)),_xll.qlSwapRateHelperSpread($D64))</f>
-        <v>--</v>
-      </c>
-      <c r="G64" s="23" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D64)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H64" s="24" t="e">
-        <f>_xll.qlRateHelperLatestDate($D64)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I64" s="18" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="65" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D65" s="21" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E65" s="22" t="e">
-        <f>_xll.qlRateHelperRate($D65)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F65" s="22" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D65)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D65)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D65)),_xll.qlSwapRateHelperSpread($D65))</f>
-        <v>--</v>
-      </c>
-      <c r="G65" s="23" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D65)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H65" s="24" t="e">
-        <f>_xll.qlRateHelperLatestDate($D65)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I65" s="18" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="66" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D66" s="21" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E66" s="22" t="e">
-        <f>_xll.qlRateHelperRate($D66)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F66" s="22" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D66)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D66)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D66)),_xll.qlSwapRateHelperSpread($D66))</f>
-        <v>--</v>
-      </c>
-      <c r="G66" s="23" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D66)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H66" s="24" t="e">
-        <f>_xll.qlRateHelperLatestDate($D66)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I66" s="18" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="67" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D67" s="21" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E67" s="22" t="e">
-        <f>_xll.qlRateHelperRate($D67)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F67" s="22" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D67)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D67)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D67)),_xll.qlSwapRateHelperSpread($D67))</f>
-        <v>--</v>
-      </c>
-      <c r="G67" s="23" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D67)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H67" s="24" t="e">
-        <f>_xll.qlRateHelperLatestDate($D67)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I67" s="18" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="68" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D68" s="21" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E68" s="22" t="e">
-        <f>_xll.qlRateHelperRate($D68)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F68" s="22" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D68)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D68)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D68)),_xll.qlSwapRateHelperSpread($D68))</f>
-        <v>--</v>
-      </c>
-      <c r="G68" s="23" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D68)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H68" s="24" t="e">
-        <f>_xll.qlRateHelperLatestDate($D68)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I68" s="18" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="69" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D69" s="21" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E69" s="22" t="e">
-        <f>_xll.qlRateHelperRate($D69)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F69" s="22" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D69)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D69)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D69)),_xll.qlSwapRateHelperSpread($D69))</f>
-        <v>--</v>
-      </c>
-      <c r="G69" s="23" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D69)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H69" s="24" t="e">
-        <f>_xll.qlRateHelperLatestDate($D69)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I69" s="18" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="70" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D70" s="21" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E70" s="22" t="e">
-        <f>_xll.qlRateHelperRate($D70)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F70" s="22" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D70)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D70)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D70)),_xll.qlSwapRateHelperSpread($D70))</f>
-        <v>--</v>
-      </c>
-      <c r="G70" s="23" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D70)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H70" s="24" t="e">
-        <f>_xll.qlRateHelperLatestDate($D70)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I70" s="18" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="71" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D71" s="21" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E71" s="22" t="e">
-        <f>_xll.qlRateHelperRate($D71)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F71" s="22" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D71)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D71)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D71)),_xll.qlSwapRateHelperSpread($D71))</f>
-        <v>--</v>
-      </c>
-      <c r="G71" s="23" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D71)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H71" s="24" t="e">
-        <f>_xll.qlRateHelperLatestDate($D71)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I71" s="18" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="72" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D72" s="21" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E72" s="22" t="e">
-        <f>_xll.qlRateHelperRate($D72)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F72" s="22" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D72)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D72)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D72)),_xll.qlSwapRateHelperSpread($D72))</f>
-        <v>--</v>
-      </c>
-      <c r="G72" s="23" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D72)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H72" s="24" t="e">
-        <f>_xll.qlRateHelperLatestDate($D72)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I72" s="18" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="73" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D73" s="21" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E73" s="22" t="e">
-        <f>_xll.qlRateHelperRate($D73)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F73" s="22" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D73)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D73)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D73)),_xll.qlSwapRateHelperSpread($D73))</f>
-        <v>--</v>
-      </c>
-      <c r="G73" s="23" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D73)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H73" s="24" t="e">
-        <f>_xll.qlRateHelperLatestDate($D73)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I73" s="18" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="74" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D74" s="21" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E74" s="22" t="e">
-        <f>_xll.qlRateHelperRate($D74)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F74" s="22" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D74)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D74)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D74)),_xll.qlSwapRateHelperSpread($D74))</f>
-        <v>--</v>
-      </c>
-      <c r="G74" s="23" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D74)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H74" s="24" t="e">
-        <f>_xll.qlRateHelperLatestDate($D74)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I74" s="18" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="75" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D75" s="21" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E75" s="22" t="e">
-        <f>_xll.qlRateHelperRate($D75)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F75" s="22" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D75)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D75)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D75)),_xll.qlSwapRateHelperSpread($D75))</f>
-        <v>--</v>
-      </c>
-      <c r="G75" s="23" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D75)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H75" s="24" t="e">
-        <f>_xll.qlRateHelperLatestDate($D75)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I75" s="18" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="76" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D76" s="21" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E76" s="22" t="e">
-        <f>_xll.qlRateHelperRate($D76)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F76" s="22" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D76)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D76)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D76)),_xll.qlSwapRateHelperSpread($D76))</f>
-        <v>--</v>
-      </c>
-      <c r="G76" s="23" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D76)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H76" s="24" t="e">
-        <f>_xll.qlRateHelperLatestDate($D76)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I76" s="18" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="77" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D77" s="21" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E77" s="22" t="e">
-        <f>_xll.qlRateHelperRate($D77)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F77" s="22" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D77)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D77)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D77)),_xll.qlSwapRateHelperSpread($D77))</f>
-        <v>--</v>
-      </c>
-      <c r="G77" s="23" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D77)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H77" s="24" t="e">
-        <f>_xll.qlRateHelperLatestDate($D77)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I77" s="18" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="78" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D78" s="21" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E78" s="22" t="e">
-        <f>_xll.qlRateHelperRate($D78)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F78" s="22" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D78)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D78)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D78)),_xll.qlSwapRateHelperSpread($D78))</f>
-        <v>--</v>
-      </c>
-      <c r="G78" s="23" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D78)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H78" s="24" t="e">
-        <f>_xll.qlRateHelperLatestDate($D78)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I78" s="18" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="79" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D79" s="21" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E79" s="22" t="e">
-        <f>_xll.qlRateHelperRate($D79)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F79" s="22" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D79)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D79)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D79)),_xll.qlSwapRateHelperSpread($D79))</f>
-        <v>--</v>
-      </c>
-      <c r="G79" s="23" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D79)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H79" s="24" t="e">
-        <f>_xll.qlRateHelperLatestDate($D79)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I79" s="18" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="80" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D80" s="21" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E80" s="22" t="e">
-        <f>_xll.qlRateHelperRate($D80)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F80" s="22" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D80)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D80)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D80)),_xll.qlSwapRateHelperSpread($D80))</f>
-        <v>--</v>
-      </c>
-      <c r="G80" s="23" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D80)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H80" s="24" t="e">
-        <f>_xll.qlRateHelperLatestDate($D80)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I80" s="18" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="81" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D81" s="21" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E81" s="22" t="e">
-        <f>_xll.qlRateHelperRate($D81)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F81" s="22" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D81)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D81)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D81)),_xll.qlSwapRateHelperSpread($D81))</f>
-        <v>--</v>
-      </c>
-      <c r="G81" s="23" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D81)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H81" s="24" t="e">
-        <f>_xll.qlRateHelperLatestDate($D81)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I81" s="18" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="82" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D82" s="21" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E82" s="22" t="e">
-        <f>_xll.qlRateHelperRate($D82)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F82" s="22" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D82)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D82)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D82)),_xll.qlSwapRateHelperSpread($D82))</f>
-        <v>--</v>
-      </c>
-      <c r="G82" s="23" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D82)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H82" s="24" t="e">
-        <f>_xll.qlRateHelperLatestDate($D82)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I82" s="18" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="83" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D83" s="21" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E83" s="22" t="e">
-        <f>_xll.qlRateHelperRate($D83)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F83" s="22" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D83)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D83)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D83)),_xll.qlSwapRateHelperSpread($D83))</f>
-        <v>--</v>
-      </c>
-      <c r="G83" s="23" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D83)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H83" s="24" t="e">
-        <f>_xll.qlRateHelperLatestDate($D83)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I83" s="18" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="84" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D84" s="21" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E84" s="22" t="e">
-        <f>_xll.qlRateHelperRate($D84)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F84" s="22" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D84)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D84)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D84)),_xll.qlSwapRateHelperSpread($D84))</f>
-        <v>--</v>
-      </c>
-      <c r="G84" s="23" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D84)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H84" s="24" t="e">
-        <f>_xll.qlRateHelperLatestDate($D84)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I84" s="18" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="85" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D85" s="21" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E85" s="22" t="e">
-        <f>_xll.qlRateHelperRate($D85)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F85" s="22" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D85)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D85)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D85)),_xll.qlSwapRateHelperSpread($D85))</f>
-        <v>--</v>
-      </c>
-      <c r="G85" s="23" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D85)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H85" s="24" t="e">
-        <f>_xll.qlRateHelperLatestDate($D85)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I85" s="18" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="86" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D86" s="21" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E86" s="22" t="e">
-        <f>_xll.qlRateHelperRate($D86)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F86" s="22" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D86)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D86)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D86)),_xll.qlSwapRateHelperSpread($D86))</f>
-        <v>--</v>
-      </c>
-      <c r="G86" s="23" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D86)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H86" s="24" t="e">
-        <f>_xll.qlRateHelperLatestDate($D86)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I86" s="18" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="87" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D87" s="21" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E87" s="22" t="e">
-        <f>_xll.qlRateHelperRate($D87)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F87" s="22" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D87)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D87)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D87)),_xll.qlSwapRateHelperSpread($D87))</f>
-        <v>--</v>
-      </c>
-      <c r="G87" s="23" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D87)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H87" s="24" t="e">
-        <f>_xll.qlRateHelperLatestDate($D87)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I87" s="18" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="88" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D88" s="21" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E88" s="22" t="e">
-        <f>_xll.qlRateHelperRate($D88)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F88" s="22" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D88)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D88)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D88)),_xll.qlSwapRateHelperSpread($D88))</f>
-        <v>--</v>
-      </c>
-      <c r="G88" s="23" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D88)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H88" s="24" t="e">
-        <f>_xll.qlRateHelperLatestDate($D88)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I88" s="18" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="89" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D89" s="21" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E89" s="22" t="e">
-        <f>_xll.qlRateHelperRate($D89)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F89" s="22" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D89)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D89)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D89)),_xll.qlSwapRateHelperSpread($D89))</f>
-        <v>--</v>
-      </c>
-      <c r="G89" s="23" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D89)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H89" s="24" t="e">
-        <f>_xll.qlRateHelperLatestDate($D89)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I89" s="18" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="90" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D90" s="21" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E90" s="22" t="e">
-        <f>_xll.qlRateHelperRate($D90)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F90" s="22" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D90)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D90)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D90)),_xll.qlSwapRateHelperSpread($D90))</f>
-        <v>--</v>
-      </c>
-      <c r="G90" s="23" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D90)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H90" s="24" t="e">
-        <f>_xll.qlRateHelperLatestDate($D90)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I90" s="18" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="91" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D91" s="21" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E91" s="22" t="e">
-        <f>_xll.qlRateHelperRate($D91)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F91" s="22" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D91)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D91)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D91)),_xll.qlSwapRateHelperSpread($D91))</f>
-        <v>--</v>
-      </c>
-      <c r="G91" s="23" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D91)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H91" s="24" t="e">
-        <f>_xll.qlRateHelperLatestDate($D91)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I91" s="18" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="92" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D92" s="21" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E92" s="22" t="e">
-        <f>_xll.qlRateHelperRate($D92)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F92" s="22" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D92)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D92)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D92)),_xll.qlSwapRateHelperSpread($D92))</f>
-        <v>--</v>
-      </c>
-      <c r="G92" s="23" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D92)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H92" s="24" t="e">
-        <f>_xll.qlRateHelperLatestDate($D92)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I92" s="18" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="93" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D93" s="21" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E93" s="22" t="e">
-        <f>_xll.qlRateHelperRate($D93)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F93" s="22" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D93)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D93)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D93)),_xll.qlSwapRateHelperSpread($D93))</f>
-        <v>--</v>
-      </c>
-      <c r="G93" s="23" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D93)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H93" s="24" t="e">
-        <f>_xll.qlRateHelperLatestDate($D93)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I93" s="18" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="94" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D94" s="21" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E94" s="22" t="e">
-        <f>_xll.qlRateHelperRate($D94)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F94" s="22" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D94)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D94)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D94)),_xll.qlSwapRateHelperSpread($D94))</f>
-        <v>--</v>
-      </c>
-      <c r="G94" s="23" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D94)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H94" s="24" t="e">
-        <f>_xll.qlRateHelperLatestDate($D94)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I94" s="18" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="95" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D95" s="21" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E95" s="22" t="e">
-        <f>_xll.qlRateHelperRate($D95)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F95" s="22" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D95)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D95)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D95)),_xll.qlSwapRateHelperSpread($D95))</f>
-        <v>--</v>
-      </c>
-      <c r="G95" s="23" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D95)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H95" s="24" t="e">
-        <f>_xll.qlRateHelperLatestDate($D95)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I95" s="18" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="96" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D96" s="21" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E96" s="22" t="e">
-        <f>_xll.qlRateHelperRate($D96)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F96" s="22" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D96)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D96)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D96)),_xll.qlSwapRateHelperSpread($D96))</f>
-        <v>--</v>
-      </c>
-      <c r="G96" s="23" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D96)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H96" s="24" t="e">
-        <f>_xll.qlRateHelperLatestDate($D96)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I96" s="18" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="97" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D97" s="21" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E97" s="22" t="e">
-        <f>_xll.qlRateHelperRate($D97)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F97" s="22" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D97)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D97)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D97)),_xll.qlSwapRateHelperSpread($D97))</f>
-        <v>--</v>
-      </c>
-      <c r="G97" s="23" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D97)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H97" s="24" t="e">
-        <f>_xll.qlRateHelperLatestDate($D97)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I97" s="18" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="98" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D98" s="21" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E98" s="22" t="e">
-        <f>_xll.qlRateHelperRate($D98)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F98" s="22" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D98)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D98)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D98)),_xll.qlSwapRateHelperSpread($D98))</f>
-        <v>--</v>
-      </c>
-      <c r="G98" s="23" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D98)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H98" s="24" t="e">
-        <f>_xll.qlRateHelperLatestDate($D98)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I98" s="18" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="99" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D99" s="21" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E99" s="22" t="e">
-        <f>_xll.qlRateHelperRate($D99)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F99" s="22" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D99)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D99)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D99)),_xll.qlSwapRateHelperSpread($D99))</f>
-        <v>--</v>
-      </c>
-      <c r="G99" s="23" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D99)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H99" s="24" t="e">
-        <f>_xll.qlRateHelperLatestDate($D99)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I99" s="18" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="100" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D100" s="21" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E100" s="22" t="e">
-        <f>_xll.qlRateHelperRate($D100)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F100" s="22" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D100)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D100)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D100)),_xll.qlSwapRateHelperSpread($D100))</f>
-        <v>--</v>
-      </c>
-      <c r="G100" s="23" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D100)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H100" s="24" t="e">
-        <f>_xll.qlRateHelperLatestDate($D100)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I100" s="18" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="101" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D101" s="21" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E101" s="22" t="e">
-        <f>_xll.qlRateHelperRate($D101)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F101" s="22" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D101)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D101)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D101)),_xll.qlSwapRateHelperSpread($D101))</f>
-        <v>--</v>
-      </c>
-      <c r="G101" s="23" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D101)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H101" s="24" t="e">
-        <f>_xll.qlRateHelperLatestDate($D101)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I101" s="18" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="102" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D102" s="21" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E102" s="22" t="e">
-        <f>_xll.qlRateHelperRate($D102)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F102" s="22" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D102)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D102)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D102)),_xll.qlSwapRateHelperSpread($D102))</f>
-        <v>--</v>
-      </c>
-      <c r="G102" s="23" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D102)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H102" s="24" t="e">
-        <f>_xll.qlRateHelperLatestDate($D102)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I102" s="18" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="103" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D103" s="21" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E103" s="22" t="e">
-        <f>_xll.qlRateHelperRate($D103)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F103" s="22" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D103)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D103)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D103)),_xll.qlSwapRateHelperSpread($D103))</f>
-        <v>--</v>
-      </c>
-      <c r="G103" s="23" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D103)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H103" s="24" t="e">
-        <f>_xll.qlRateHelperLatestDate($D103)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I103" s="18" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="104" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D104" s="21" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E104" s="22" t="e">
-        <f>_xll.qlRateHelperRate($D104)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F104" s="22" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D104)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D104)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D104)),_xll.qlSwapRateHelperSpread($D104))</f>
-        <v>--</v>
-      </c>
-      <c r="G104" s="23" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D104)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H104" s="24" t="e">
-        <f>_xll.qlRateHelperLatestDate($D104)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I104" s="18" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="105" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D105" s="21" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E105" s="22" t="e">
-        <f>_xll.qlRateHelperRate($D105)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F105" s="22" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D105)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D105)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D105)),_xll.qlSwapRateHelperSpread($D105))</f>
-        <v>--</v>
-      </c>
-      <c r="G105" s="23" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D105)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H105" s="24" t="e">
-        <f>_xll.qlRateHelperLatestDate($D105)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I105" s="18" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="106" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D106" s="21" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E106" s="22" t="e">
-        <f>_xll.qlRateHelperRate($D106)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F106" s="22" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D106)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D106)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D106)),_xll.qlSwapRateHelperSpread($D106))</f>
-        <v>--</v>
-      </c>
-      <c r="G106" s="23" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D106)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H106" s="24" t="e">
-        <f>_xll.qlRateHelperLatestDate($D106)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I106" s="18" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="107" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D107" s="21" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E107" s="22" t="e">
-        <f>_xll.qlRateHelperRate($D107)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F107" s="22" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D107)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D107)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D107)),_xll.qlSwapRateHelperSpread($D107))</f>
-        <v>--</v>
-      </c>
-      <c r="G107" s="23" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D107)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H107" s="24" t="e">
-        <f>_xll.qlRateHelperLatestDate($D107)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I107" s="18" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="108" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D108" s="21" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E108" s="22" t="e">
-        <f>_xll.qlRateHelperRate($D108)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F108" s="22" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D108)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D108)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D108)),_xll.qlSwapRateHelperSpread($D108))</f>
-        <v>--</v>
-      </c>
-      <c r="G108" s="23" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D108)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H108" s="24" t="e">
-        <f>_xll.qlRateHelperLatestDate($D108)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I108" s="18" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="109" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D109" s="21" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E109" s="22" t="e">
-        <f>_xll.qlRateHelperRate($D109)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F109" s="22" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D109)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D109)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D109)),_xll.qlSwapRateHelperSpread($D109))</f>
-        <v>--</v>
-      </c>
-      <c r="G109" s="23" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D109)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H109" s="24" t="e">
-        <f>_xll.qlRateHelperLatestDate($D109)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I109" s="18" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="110" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D110" s="21" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E110" s="22" t="e">
-        <f>_xll.qlRateHelperRate($D110)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F110" s="22" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D110)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D110)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D110)),_xll.qlSwapRateHelperSpread($D110))</f>
-        <v>--</v>
-      </c>
-      <c r="G110" s="23" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D110)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H110" s="24" t="e">
-        <f>_xll.qlRateHelperLatestDate($D110)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I110" s="18" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="111" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D111" s="21" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E111" s="22" t="e">
-        <f>_xll.qlRateHelperRate($D111)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F111" s="22" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D111)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D111)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D111)),_xll.qlSwapRateHelperSpread($D111))</f>
-        <v>--</v>
-      </c>
-      <c r="G111" s="23" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D111)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H111" s="24" t="e">
-        <f>_xll.qlRateHelperLatestDate($D111)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I111" s="18" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="112" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D112" s="21" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E112" s="22" t="e">
-        <f>_xll.qlRateHelperRate($D112)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F112" s="22" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D112)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D112)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D112)),_xll.qlSwapRateHelperSpread($D112))</f>
-        <v>--</v>
-      </c>
-      <c r="G112" s="23" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D112)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H112" s="24" t="e">
-        <f>_xll.qlRateHelperLatestDate($D112)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I112" s="18" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="113" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D113" s="21" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E113" s="22" t="e">
-        <f>_xll.qlRateHelperRate($D113)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F113" s="22" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D113)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D113)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D113)),_xll.qlSwapRateHelperSpread($D113))</f>
-        <v>--</v>
-      </c>
-      <c r="G113" s="23" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D113)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H113" s="24" t="e">
-        <f>_xll.qlRateHelperLatestDate($D113)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I113" s="18" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="114" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D114" s="21" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E114" s="22" t="e">
-        <f>_xll.qlRateHelperRate($D114)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F114" s="22" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D114)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D114)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D114)),_xll.qlSwapRateHelperSpread($D114))</f>
-        <v>--</v>
-      </c>
-      <c r="G114" s="23" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D114)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H114" s="24" t="e">
-        <f>_xll.qlRateHelperLatestDate($D114)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I114" s="18" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="115" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D115" s="21" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E115" s="22" t="e">
-        <f>_xll.qlRateHelperRate($D115)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F115" s="22" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D115)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D115)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D115)),_xll.qlSwapRateHelperSpread($D115))</f>
-        <v>--</v>
-      </c>
-      <c r="G115" s="23" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D115)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H115" s="24" t="e">
-        <f>_xll.qlRateHelperLatestDate($D115)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I115" s="18" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="116" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D116" s="21" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E116" s="22" t="e">
-        <f>_xll.qlRateHelperRate($D116)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F116" s="22" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D116)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D116)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D116)),_xll.qlSwapRateHelperSpread($D116))</f>
-        <v>--</v>
-      </c>
-      <c r="G116" s="23" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D116)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H116" s="24" t="e">
-        <f>_xll.qlRateHelperLatestDate($D116)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I116" s="18" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="117" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D117" s="21" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E117" s="22" t="e">
-        <f>_xll.qlRateHelperRate($D117)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F117" s="22" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D117)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D117)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D117)),_xll.qlSwapRateHelperSpread($D117))</f>
-        <v>--</v>
-      </c>
-      <c r="G117" s="23" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D117)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H117" s="24" t="e">
-        <f>_xll.qlRateHelperLatestDate($D117)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I117" s="18" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="118" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D118" s="21" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E118" s="22" t="e">
-        <f>_xll.qlRateHelperRate($D118)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F118" s="22" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D118)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D118)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D118)),_xll.qlSwapRateHelperSpread($D118))</f>
-        <v>--</v>
-      </c>
-      <c r="G118" s="23" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D118)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H118" s="24" t="e">
-        <f>_xll.qlRateHelperLatestDate($D118)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I118" s="18" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="119" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D119" s="21" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E119" s="22" t="e">
-        <f>_xll.qlRateHelperRate($D119)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F119" s="22" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D119)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D119)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D119)),_xll.qlSwapRateHelperSpread($D119))</f>
-        <v>--</v>
-      </c>
-      <c r="G119" s="23" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D119)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H119" s="24" t="e">
-        <f>_xll.qlRateHelperLatestDate($D119)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I119" s="18" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="120" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D120" s="21" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E120" s="22" t="e">
-        <f>_xll.qlRateHelperRate($D120)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F120" s="22" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D120)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D120)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D120)),_xll.qlSwapRateHelperSpread($D120))</f>
-        <v>--</v>
-      </c>
-      <c r="G120" s="23" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D120)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H120" s="24" t="e">
-        <f>_xll.qlRateHelperLatestDate($D120)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I120" s="18" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="121" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D121" s="21" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E121" s="22" t="e">
-        <f>_xll.qlRateHelperRate($D121)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F121" s="22" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D121)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D121)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D121)),_xll.qlSwapRateHelperSpread($D121))</f>
-        <v>--</v>
-      </c>
-      <c r="G121" s="23" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D121)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H121" s="24" t="e">
-        <f>_xll.qlRateHelperLatestDate($D121)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I121" s="18" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="122" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D122" s="21" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E122" s="22" t="e">
-        <f>_xll.qlRateHelperRate($D122)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F122" s="22" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D122)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D122)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D122)),_xll.qlSwapRateHelperSpread($D122))</f>
-        <v>--</v>
-      </c>
-      <c r="G122" s="23" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D122)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H122" s="24" t="e">
-        <f>_xll.qlRateHelperLatestDate($D122)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I122" s="18" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="123" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D123" s="21" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E123" s="22" t="e">
-        <f>_xll.qlRateHelperRate($D123)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F123" s="22" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D123)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D123)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D123)),_xll.qlSwapRateHelperSpread($D123))</f>
-        <v>--</v>
-      </c>
-      <c r="G123" s="23" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D123)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H123" s="24" t="e">
-        <f>_xll.qlRateHelperLatestDate($D123)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I123" s="18" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="124" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D124" s="21" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E124" s="22" t="e">
-        <f>_xll.qlRateHelperRate($D124)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F124" s="22" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D124)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D124)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D124)),_xll.qlSwapRateHelperSpread($D124))</f>
-        <v>--</v>
-      </c>
-      <c r="G124" s="23" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D124)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H124" s="24" t="e">
-        <f>_xll.qlRateHelperLatestDate($D124)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I124" s="18" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="125" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D125" s="21" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E125" s="22" t="e">
-        <f>_xll.qlRateHelperRate($D125)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F125" s="22" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D125)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D125)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D125)),_xll.qlSwapRateHelperSpread($D125))</f>
-        <v>--</v>
-      </c>
-      <c r="G125" s="23" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D125)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H125" s="24" t="e">
-        <f>_xll.qlRateHelperLatestDate($D125)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I125" s="18" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="126" spans="4:9" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D126" s="31" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E126" s="32" t="e">
-        <f>_xll.qlRateHelperRate($D126)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F126" s="32" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D126)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D126)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D126)),_xll.qlSwapRateHelperSpread($D126))</f>
-        <v>--</v>
-      </c>
-      <c r="G126" s="33" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D126)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H126" s="34" t="e">
-        <f>_xll.qlRateHelperLatestDate($D126)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I126" s="18" t="e">
-        <v>#N/A</v>
-      </c>
+      <c r="D22" s="133"/>
+      <c r="I22" s="134"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
fixed HKD conventions, added fixings, smoothed out few issues
</commit_message>
<xml_diff>
--- a/QuantLibXL/Data2/XLS/HKD_YC6MBootstrapping.xlsx
+++ b/QuantLibXL/Data2/XLS/HKD_YC6MBootstrapping.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="15030" windowHeight="7785" activeTab="3"/>
+    <workbookView visibility="hidden" xWindow="22890" yWindow="-15" windowWidth="7635" windowHeight="11085" firstSheet="2" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="General Settings" sheetId="3" r:id="rId1"/>
@@ -1882,7 +1882,7 @@
       <c r="A1" s="63"/>
       <c r="B1" s="63" t="str">
         <f>_xll.qlxlVersion(TRUE,Trigger)</f>
-        <v>QuantLibXL 1.3.0 - MS VC++ 9.0 - Multithreaded Static Runtime library - Release Configuration - Nov 12 2013 12:02:30</v>
+        <v>QuantLibXL 1.3.0 - MS VC++ 9.0 - Multithreaded Dynamic Runtime library - Release Configuration - Nov  4 2013 11:55:45</v>
       </c>
       <c r="C1" s="63"/>
       <c r="D1" s="63"/>
@@ -1941,7 +1941,7 @@
         <v>6</v>
       </c>
       <c r="J4" s="72">
-        <v>41600.74664351852</v>
+        <v>41606.781886574077</v>
       </c>
       <c r="K4" s="73"/>
     </row>
@@ -2028,7 +2028,7 @@
       </c>
       <c r="J8" s="72" t="str">
         <f ca="1">SUBSTITUTE(LEFT(CELL("filename",A1),FIND("[",CELL("filename",A1),1)-1),"\XLS\","\XML\")</f>
-        <v>C:\Projects\quantlib\QuantLibXL\Data2\XML\</v>
+        <v>D:\QuantLibXL-1.3.0\Data2\XML\</v>
       </c>
       <c r="K8" s="73"/>
     </row>
@@ -2057,7 +2057,7 @@
       </c>
       <c r="D10" s="72" t="str">
         <f>_xll.qlPiecewiseYieldCurve(D12,NDays,Calendar,RateHelpersSelected,DayCounter,IF(ISERROR(D17),NA(),D15:E15),IF(ISERROR(D17),NA(),D16:E16),Accuracy,TraitsID,InterpolatorID,Permanent,,ObjectOverwrite)</f>
-        <v>_HKDYC6M#0000</v>
+        <v>HKDYC6M#0000</v>
       </c>
       <c r="E10" s="66"/>
       <c r="F10" s="67"/>
@@ -2092,8 +2092,8 @@
         <v>9</v>
       </c>
       <c r="D12" s="83" t="str">
-        <f>"_"&amp;Currency&amp;"YC"&amp;IndexTenor</f>
-        <v>_HKDYC6M</v>
+        <f>Currency&amp;"YC"&amp;IndexTenor</f>
+        <v>HKDYC6M</v>
       </c>
       <c r="E12" s="66"/>
       <c r="F12" s="67"/>
@@ -2283,7 +2283,7 @@
       <c r="B22" s="64"/>
       <c r="C22" s="95">
         <f>_xll.qlTermStructureReferenceDate(YieldCurve)</f>
-        <v>41600</v>
+        <v>41607</v>
       </c>
       <c r="D22" s="96">
         <f>MAX(_xll.ohPack(Selected!I1:I20))</f>
@@ -2302,11 +2302,11 @@
       <c r="B23" s="64"/>
       <c r="C23" s="97">
         <f>MAX(_xll.ohPack(Selected!H2:H126))</f>
-        <v>42331</v>
+        <v>42341</v>
       </c>
       <c r="D23" s="74">
         <f>MIN(_xll.ohPack(Selected!I1:I20))</f>
-        <v>0.98767931763767025</v>
+        <v>0.98769086712261345</v>
       </c>
       <c r="E23" s="66"/>
       <c r="F23" s="67"/>
@@ -2337,14 +2337,8 @@
     <row r="25" spans="1:11" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="63"/>
       <c r="B25" s="100"/>
-      <c r="C25" s="139" t="str">
-        <f>UPPER(Currency)&amp;IndexTenor</f>
-        <v>HKD6M</v>
-      </c>
-      <c r="D25" s="139" t="b">
-        <f>_xll.qlRelinkableHandleLinkTo(C25,YieldCurve)</f>
-        <v>1</v>
-      </c>
+      <c r="C25" s="139"/>
+      <c r="D25" s="139"/>
       <c r="E25" s="101"/>
       <c r="F25" s="102"/>
       <c r="G25" s="63"/>
@@ -2495,9 +2489,9 @@
         <f>$H$1&amp;"_FRAs.xml"</f>
         <v>HKD_YC6MRH_FRAs.xml</v>
       </c>
-      <c r="I2" s="48">
+      <c r="I2" s="48" t="e">
         <f ca="1">IF(Serialize,_xll.ohObjectSave(I3:I23,SerializationPath&amp;H2,FileOverwrite,,Serialize),"---")</f>
-        <v>21</v>
+        <v>#NUM!</v>
       </c>
       <c r="J2" s="47" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(I2)</f>
@@ -3381,11 +3375,11 @@
       </c>
       <c r="K2" s="114">
         <f>_xll.qlRateHelperEarliestDate($E2,Trigger)</f>
-        <v>41600</v>
+        <v>41611</v>
       </c>
       <c r="L2" s="113">
         <f>_xll.qlRateHelperLatestDate($E2,Trigger)</f>
-        <v>41781</v>
+        <v>41793</v>
       </c>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.2">
@@ -3420,11 +3414,11 @@
       </c>
       <c r="K3" s="121">
         <f>_xll.qlRateHelperEarliestDate($E3,Trigger)</f>
-        <v>41600</v>
+        <v>41611</v>
       </c>
       <c r="L3" s="120">
         <f>_xll.qlRateHelperLatestDate($E3,Trigger)</f>
-        <v>41781</v>
+        <v>41793</v>
       </c>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.2">
@@ -3459,11 +3453,11 @@
       </c>
       <c r="K4" s="107">
         <f>_xll.qlRateHelperEarliestDate($E4,Trigger)</f>
-        <v>41603</v>
+        <v>41612</v>
       </c>
       <c r="L4" s="106">
         <f>_xll.qlRateHelperLatestDate($E4,Trigger)</f>
-        <v>41785</v>
+        <v>41794</v>
       </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.2">
@@ -3498,11 +3492,11 @@
       </c>
       <c r="K5" s="114">
         <f>_xll.qlRateHelperEarliestDate($E5,Trigger)</f>
-        <v>41631</v>
+        <v>41642</v>
       </c>
       <c r="L5" s="113">
         <f>_xll.qlRateHelperLatestDate($E5,Trigger)</f>
-        <v>41813</v>
+        <v>41823</v>
       </c>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.2">
@@ -3537,11 +3531,11 @@
       </c>
       <c r="K6" s="114">
         <f>_xll.qlRateHelperEarliestDate($E6,Trigger)</f>
-        <v>41661</v>
+        <v>41673</v>
       </c>
       <c r="L6" s="113">
         <f>_xll.qlRateHelperLatestDate($E6,Trigger)</f>
-        <v>41842</v>
+        <v>41855</v>
       </c>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.2">
@@ -3576,11 +3570,11 @@
       </c>
       <c r="K7" s="114">
         <f>_xll.qlRateHelperEarliestDate($E7,Trigger)</f>
-        <v>41694</v>
+        <v>41701</v>
       </c>
       <c r="L7" s="113">
         <f>_xll.qlRateHelperLatestDate($E7,Trigger)</f>
-        <v>41876</v>
+        <v>41885</v>
       </c>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.2">
@@ -3615,11 +3609,11 @@
       </c>
       <c r="K8" s="114">
         <f>_xll.qlRateHelperEarliestDate($E8,Trigger)</f>
-        <v>41722</v>
+        <v>41732</v>
       </c>
       <c r="L8" s="113">
         <f>_xll.qlRateHelperLatestDate($E8,Trigger)</f>
-        <v>41906</v>
+        <v>41915</v>
       </c>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.2">
@@ -3654,11 +3648,11 @@
       </c>
       <c r="K9" s="114">
         <f>_xll.qlRateHelperEarliestDate($E9,Trigger)</f>
-        <v>41751</v>
+        <v>41764</v>
       </c>
       <c r="L9" s="113">
         <f>_xll.qlRateHelperLatestDate($E9,Trigger)</f>
-        <v>41934</v>
+        <v>41948</v>
       </c>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.2">
@@ -3693,11 +3687,11 @@
       </c>
       <c r="K10" s="114">
         <f>_xll.qlRateHelperEarliestDate($E10,Trigger)</f>
-        <v>41781</v>
+        <v>41793</v>
       </c>
       <c r="L10" s="113">
         <f>_xll.qlRateHelperLatestDate($E10,Trigger)</f>
-        <v>41967</v>
+        <v>41976</v>
       </c>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.2">
@@ -3732,11 +3726,11 @@
       </c>
       <c r="K11" s="114">
         <f>_xll.qlRateHelperEarliestDate($E11,Trigger)</f>
-        <v>41813</v>
+        <v>41823</v>
       </c>
       <c r="L11" s="113">
         <f>_xll.qlRateHelperLatestDate($E11,Trigger)</f>
-        <v>41996</v>
+        <v>42009</v>
       </c>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.2">
@@ -3771,11 +3765,11 @@
       </c>
       <c r="K12" s="114">
         <f>_xll.qlRateHelperEarliestDate($E12,Trigger)</f>
-        <v>41842</v>
+        <v>41855</v>
       </c>
       <c r="L12" s="113">
         <f>_xll.qlRateHelperLatestDate($E12,Trigger)</f>
-        <v>42026</v>
+        <v>42039</v>
       </c>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.2">
@@ -3810,11 +3804,11 @@
       </c>
       <c r="K13" s="114">
         <f>_xll.qlRateHelperEarliestDate($E13,Trigger)</f>
-        <v>41873</v>
+        <v>41885</v>
       </c>
       <c r="L13" s="113">
         <f>_xll.qlRateHelperLatestDate($E13,Trigger)</f>
-        <v>42058</v>
+        <v>42066</v>
       </c>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.2">
@@ -3849,11 +3843,11 @@
       </c>
       <c r="K14" s="114">
         <f>_xll.qlRateHelperEarliestDate($E14,Trigger)</f>
-        <v>41904</v>
+        <v>41915</v>
       </c>
       <c r="L14" s="113">
         <f>_xll.qlRateHelperLatestDate($E14,Trigger)</f>
-        <v>42086</v>
+        <v>42101</v>
       </c>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.2">
@@ -3888,11 +3882,11 @@
       </c>
       <c r="K15" s="114">
         <f>_xll.qlRateHelperEarliestDate($E15,Trigger)</f>
-        <v>41934</v>
+        <v>41946</v>
       </c>
       <c r="L15" s="113">
         <f>_xll.qlRateHelperLatestDate($E15,Trigger)</f>
-        <v>42116</v>
+        <v>42128</v>
       </c>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.2">
@@ -3927,11 +3921,11 @@
       </c>
       <c r="K16" s="114">
         <f>_xll.qlRateHelperEarliestDate($E16,Trigger)</f>
-        <v>41967</v>
+        <v>41976</v>
       </c>
       <c r="L16" s="113">
         <f>_xll.qlRateHelperLatestDate($E16,Trigger)</f>
-        <v>42149</v>
+        <v>42158</v>
       </c>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.2">
@@ -3966,11 +3960,11 @@
       </c>
       <c r="K17" s="114">
         <f>_xll.qlRateHelperEarliestDate($E17,Trigger)</f>
-        <v>41995</v>
+        <v>42009</v>
       </c>
       <c r="L17" s="113">
         <f>_xll.qlRateHelperLatestDate($E17,Trigger)</f>
-        <v>42177</v>
+        <v>42191</v>
       </c>
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.2">
@@ -4005,11 +3999,11 @@
       </c>
       <c r="K18" s="114">
         <f>_xll.qlRateHelperEarliestDate($E18,Trigger)</f>
-        <v>42026</v>
+        <v>42038</v>
       </c>
       <c r="L18" s="113">
         <f>_xll.qlRateHelperLatestDate($E18,Trigger)</f>
-        <v>42207</v>
+        <v>42219</v>
       </c>
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.2">
@@ -4044,11 +4038,11 @@
       </c>
       <c r="K19" s="114">
         <f>_xll.qlRateHelperEarliestDate($E19,Trigger)</f>
-        <v>42058</v>
+        <v>42066</v>
       </c>
       <c r="L19" s="113">
         <f>_xll.qlRateHelperLatestDate($E19,Trigger)</f>
-        <v>42240</v>
+        <v>42250</v>
       </c>
     </row>
     <row r="20" spans="2:12" x14ac:dyDescent="0.2">
@@ -4083,11 +4077,11 @@
       </c>
       <c r="K20" s="114">
         <f>_xll.qlRateHelperEarliestDate($E20,Trigger)</f>
-        <v>42086</v>
+        <v>42101</v>
       </c>
       <c r="L20" s="113">
         <f>_xll.qlRateHelperLatestDate($E20,Trigger)</f>
-        <v>42270</v>
+        <v>42284</v>
       </c>
     </row>
     <row r="21" spans="2:12" x14ac:dyDescent="0.2">
@@ -4122,11 +4116,11 @@
       </c>
       <c r="K21" s="114">
         <f>_xll.qlRateHelperEarliestDate($E21,Trigger)</f>
-        <v>42116</v>
+        <v>42128</v>
       </c>
       <c r="L21" s="113">
         <f>_xll.qlRateHelperLatestDate($E21,Trigger)</f>
-        <v>42299</v>
+        <v>42312</v>
       </c>
     </row>
     <row r="22" spans="2:12" x14ac:dyDescent="0.2">
@@ -4146,7 +4140,7 @@
       </c>
       <c r="F22" s="109">
         <f>_xll.qlRateHelperQuoteValue($E22,Trigger)</f>
-        <v>7.8000000000000005E-3</v>
+        <v>7.7000000000000002E-3</v>
       </c>
       <c r="G22" s="109"/>
       <c r="H22" s="108" t="b">
@@ -4161,11 +4155,11 @@
       </c>
       <c r="K22" s="107">
         <f>_xll.qlRateHelperEarliestDate($E22,Trigger)</f>
-        <v>42146</v>
+        <v>42158</v>
       </c>
       <c r="L22" s="106">
         <f>_xll.qlRateHelperLatestDate($E22,Trigger)</f>
-        <v>42331</v>
+        <v>42341</v>
       </c>
     </row>
     <row r="23" spans="2:12" x14ac:dyDescent="0.2">
@@ -5836,14 +5830,14 @@
       </c>
       <c r="G2" s="11">
         <f>_xll.qlRateHelperEarliestDate($D2)</f>
-        <v>41600</v>
+        <v>41611</v>
       </c>
       <c r="H2" s="12">
         <f>_xll.qlRateHelperLatestDate($D2)</f>
-        <v>41781</v>
+        <v>41793</v>
       </c>
       <c r="I2" s="6">
-        <v>0.99728707396165672</v>
+        <v>0.99721225668296354</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
@@ -5866,14 +5860,14 @@
       </c>
       <c r="G3" s="11">
         <f>_xll.qlRateHelperEarliestDate($D3)</f>
-        <v>41631</v>
+        <v>41642</v>
       </c>
       <c r="H3" s="12">
         <f>_xll.qlRateHelperLatestDate($D3)</f>
-        <v>41813</v>
+        <v>41823</v>
       </c>
       <c r="I3" s="6">
-        <v>0.99709863321981806</v>
+        <v>0.99705212994891101</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
@@ -5896,14 +5890,14 @@
       </c>
       <c r="G4" s="11">
         <f>_xll.qlRateHelperEarliestDate($D4)</f>
-        <v>41661</v>
+        <v>41673</v>
       </c>
       <c r="H4" s="12">
         <f>_xll.qlRateHelperLatestDate($D4)</f>
-        <v>41842</v>
+        <v>41855</v>
       </c>
       <c r="I4" s="6">
-        <v>0.99666312062440998</v>
+        <v>0.99657499044919295</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -5926,14 +5920,14 @@
       </c>
       <c r="G5" s="11">
         <f>_xll.qlRateHelperEarliestDate($D5)</f>
-        <v>41694</v>
+        <v>41701</v>
       </c>
       <c r="H5" s="12">
         <f>_xll.qlRateHelperLatestDate($D5)</f>
-        <v>41876</v>
+        <v>41885</v>
       </c>
       <c r="I5" s="6">
-        <v>0.99610671309900745</v>
+        <v>0.99607950165484438</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
@@ -5957,14 +5951,14 @@
       </c>
       <c r="G6" s="11">
         <f>_xll.qlRateHelperEarliestDate($D6)</f>
-        <v>41722</v>
+        <v>41732</v>
       </c>
       <c r="H6" s="12">
         <f>_xll.qlRateHelperLatestDate($D6)</f>
-        <v>41906</v>
+        <v>41915</v>
       </c>
       <c r="I6" s="6">
-        <v>0.99561091366603716</v>
+        <v>0.99557997474673687</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="12" thickBot="1" x14ac:dyDescent="0.25">
@@ -5989,14 +5983,14 @@
       </c>
       <c r="G7" s="11">
         <f>_xll.qlRateHelperEarliestDate($D7)</f>
-        <v>41751</v>
+        <v>41764</v>
       </c>
       <c r="H7" s="12">
         <f>_xll.qlRateHelperLatestDate($D7)</f>
-        <v>41934</v>
+        <v>41948</v>
       </c>
       <c r="I7" s="6">
-        <v>0.99514176356087747</v>
+        <v>0.99503803019528603</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
@@ -6013,14 +6007,14 @@
       </c>
       <c r="G8" s="11">
         <f>_xll.qlRateHelperEarliestDate($D8)</f>
-        <v>41781</v>
+        <v>41793</v>
       </c>
       <c r="H8" s="12">
         <f>_xll.qlRateHelperLatestDate($D8)</f>
-        <v>41967</v>
+        <v>41976</v>
       </c>
       <c r="I8" s="6">
-        <v>0.99455028954844549</v>
+        <v>0.99451969678061169</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
@@ -6037,14 +6031,14 @@
       </c>
       <c r="G9" s="11">
         <f>_xll.qlRateHelperEarliestDate($D9)</f>
-        <v>41967</v>
+        <v>41976</v>
       </c>
       <c r="H9" s="12">
         <f>_xll.qlRateHelperLatestDate($D9)</f>
-        <v>42149</v>
+        <v>42158</v>
       </c>
       <c r="I9" s="6">
-        <v>0.99153439506788554</v>
+        <v>0.99150389507018177</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
@@ -6053,7 +6047,7 @@
       </c>
       <c r="E10" s="10">
         <f>_xll.qlRateHelperRate($D10)</f>
-        <v>7.8000000000000005E-3</v>
+        <v>7.7000000000000002E-3</v>
       </c>
       <c r="F10" s="10" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D10)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D10)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D10)),_xll.qlSwapRateHelperSpread($D10))</f>
@@ -6061,14 +6055,14 @@
       </c>
       <c r="G10" s="11">
         <f>_xll.qlRateHelperEarliestDate($D10)</f>
-        <v>42146</v>
+        <v>42158</v>
       </c>
       <c r="H10" s="12">
         <f>_xll.qlRateHelperLatestDate($D10)</f>
-        <v>42331</v>
+        <v>42341</v>
       </c>
       <c r="I10" s="6">
-        <v>0.98767931763767025</v>
+        <v>0.98769086712261345</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
few more fixes for the HKD curves
</commit_message>
<xml_diff>
--- a/QuantLibXL/Data2/XLS/HKD_YC6MBootstrapping.xlsx
+++ b/QuantLibXL/Data2/XLS/HKD_YC6MBootstrapping.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView visibility="hidden" xWindow="22890" yWindow="-15" windowWidth="7635" windowHeight="11085" firstSheet="2" activeTab="3"/>
+    <workbookView xWindow="22890" yWindow="-15" windowWidth="7635" windowHeight="11085" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="General Settings" sheetId="3" r:id="rId1"/>
-    <sheet name="HKD_YCRH_FRAs_6M" sheetId="6" r:id="rId2"/>
+    <sheet name="FRAs" sheetId="6" r:id="rId2"/>
     <sheet name="RateHelpers" sheetId="7" r:id="rId3"/>
     <sheet name="Selected" sheetId="8" r:id="rId4"/>
   </sheets>
@@ -33,7 +33,7 @@
     <definedName name="ObjectOverwrite">'General Settings'!$J$6</definedName>
     <definedName name="Permanent">'General Settings'!$J$5</definedName>
     <definedName name="QuoteSuffix">'General Settings'!$J$16</definedName>
-    <definedName name="RateHelperConstructors" localSheetId="1">HKD_YCRH_FRAs_6M!$I$3:$I$22</definedName>
+    <definedName name="RateHelperConstructors" localSheetId="1">FRAs!$I$3:$I$22</definedName>
     <definedName name="RateHelperPrefix">'General Settings'!$D$8</definedName>
     <definedName name="RateHelpers">RateHelpers!$E$2:$E$59</definedName>
     <definedName name="RateHelpersIncluded">RateHelpers!$H$2:$H$59</definedName>
@@ -1941,7 +1941,7 @@
         <v>6</v>
       </c>
       <c r="J4" s="72">
-        <v>41606.781886574077</v>
+        <v>41607.530104166668</v>
       </c>
       <c r="K4" s="73"/>
     </row>
@@ -2028,7 +2028,7 @@
       </c>
       <c r="J8" s="72" t="str">
         <f ca="1">SUBSTITUTE(LEFT(CELL("filename",A1),FIND("[",CELL("filename",A1),1)-1),"\XLS\","\XML\")</f>
-        <v>D:\QuantLibXL-1.3.0\Data2\XML\</v>
+        <v>N:\QuantLibXL-1.3.0\Data2\XML\</v>
       </c>
       <c r="K8" s="73"/>
     </row>
@@ -2302,11 +2302,11 @@
       <c r="B23" s="64"/>
       <c r="C23" s="97">
         <f>MAX(_xll.ohPack(Selected!H2:H126))</f>
-        <v>42341</v>
+        <v>42338</v>
       </c>
       <c r="D23" s="74">
         <f>MIN(_xll.ohPack(Selected!I1:I20))</f>
-        <v>0.98769086712261345</v>
+        <v>0.98762426348985388</v>
       </c>
       <c r="E23" s="66"/>
       <c r="F23" s="67"/>
@@ -2433,7 +2433,7 @@
   <dimension ref="A1:K25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="G38" sqref="G38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -2495,7 +2495,7 @@
       </c>
       <c r="J2" s="47" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(I2)</f>
-        <v/>
+        <v>ohObjectSave - Invalid parent path : N:\QuantLibXL-1.3.0\Data2\XML\HKD_YC6MRH_FRAs.xml</v>
       </c>
       <c r="K2" s="30"/>
     </row>
@@ -3355,7 +3355,7 @@
         <v>99</v>
       </c>
       <c r="E2" s="117" t="str">
-        <f>HKD_YCRH_FRAs_6M!I23</f>
+        <f>FRAs!I23</f>
         <v>HkdHibor6MLastFixing#0000</v>
       </c>
       <c r="F2" s="116">
@@ -3375,11 +3375,11 @@
       </c>
       <c r="K2" s="114">
         <f>_xll.qlRateHelperEarliestDate($E2,Trigger)</f>
-        <v>41611</v>
+        <v>41607</v>
       </c>
       <c r="L2" s="113">
         <f>_xll.qlRateHelperLatestDate($E2,Trigger)</f>
-        <v>41793</v>
+        <v>41789</v>
       </c>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.2">
@@ -3414,11 +3414,11 @@
       </c>
       <c r="K3" s="121">
         <f>_xll.qlRateHelperEarliestDate($E3,Trigger)</f>
-        <v>41611</v>
+        <v>41607</v>
       </c>
       <c r="L3" s="120">
         <f>_xll.qlRateHelperLatestDate($E3,Trigger)</f>
-        <v>41793</v>
+        <v>41789</v>
       </c>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.2">
@@ -3453,11 +3453,11 @@
       </c>
       <c r="K4" s="107">
         <f>_xll.qlRateHelperEarliestDate($E4,Trigger)</f>
-        <v>41612</v>
+        <v>41610</v>
       </c>
       <c r="L4" s="106">
         <f>_xll.qlRateHelperLatestDate($E4,Trigger)</f>
-        <v>41794</v>
+        <v>41792</v>
       </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.2">
@@ -3472,7 +3472,7 @@
         <v>7F</v>
       </c>
       <c r="E5" s="117" t="str">
-        <f>HKD_YCRH_FRAs_6M!I5</f>
+        <f>FRAs!I5</f>
         <v>HKD_YC6MRH_1x7F#0000</v>
       </c>
       <c r="F5" s="116">
@@ -3492,11 +3492,11 @@
       </c>
       <c r="K5" s="114">
         <f>_xll.qlRateHelperEarliestDate($E5,Trigger)</f>
-        <v>41642</v>
+        <v>41639</v>
       </c>
       <c r="L5" s="113">
         <f>_xll.qlRateHelperLatestDate($E5,Trigger)</f>
-        <v>41823</v>
+        <v>41820</v>
       </c>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.2">
@@ -3511,7 +3511,7 @@
         <v>8F</v>
       </c>
       <c r="E6" s="117" t="str">
-        <f>HKD_YCRH_FRAs_6M!I6</f>
+        <f>FRAs!I6</f>
         <v>HKD_YC6MRH_2x8F#0000</v>
       </c>
       <c r="F6" s="116">
@@ -3531,11 +3531,11 @@
       </c>
       <c r="K6" s="114">
         <f>_xll.qlRateHelperEarliestDate($E6,Trigger)</f>
-        <v>41673</v>
+        <v>41670</v>
       </c>
       <c r="L6" s="113">
         <f>_xll.qlRateHelperLatestDate($E6,Trigger)</f>
-        <v>41855</v>
+        <v>41851</v>
       </c>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.2">
@@ -3550,7 +3550,7 @@
         <v>9F</v>
       </c>
       <c r="E7" s="117" t="str">
-        <f>HKD_YCRH_FRAs_6M!I7</f>
+        <f>FRAs!I7</f>
         <v>HKD_YC6MRH_3x9F#0000</v>
       </c>
       <c r="F7" s="116">
@@ -3570,11 +3570,11 @@
       </c>
       <c r="K7" s="114">
         <f>_xll.qlRateHelperEarliestDate($E7,Trigger)</f>
-        <v>41701</v>
+        <v>41698</v>
       </c>
       <c r="L7" s="113">
         <f>_xll.qlRateHelperLatestDate($E7,Trigger)</f>
-        <v>41885</v>
+        <v>41880</v>
       </c>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.2">
@@ -3589,7 +3589,7 @@
         <v>10F</v>
       </c>
       <c r="E8" s="117" t="str">
-        <f>HKD_YCRH_FRAs_6M!I8</f>
+        <f>FRAs!I8</f>
         <v>HKD_YC6MRH_4x10F#0000</v>
       </c>
       <c r="F8" s="116">
@@ -3609,11 +3609,11 @@
       </c>
       <c r="K8" s="114">
         <f>_xll.qlRateHelperEarliestDate($E8,Trigger)</f>
-        <v>41732</v>
+        <v>41729</v>
       </c>
       <c r="L8" s="113">
         <f>_xll.qlRateHelperLatestDate($E8,Trigger)</f>
-        <v>41915</v>
+        <v>41912</v>
       </c>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.2">
@@ -3628,7 +3628,7 @@
         <v>11F</v>
       </c>
       <c r="E9" s="117" t="str">
-        <f>HKD_YCRH_FRAs_6M!I9</f>
+        <f>FRAs!I9</f>
         <v>HKD_YC6MRH_5x11F#0000</v>
       </c>
       <c r="F9" s="116">
@@ -3648,11 +3648,11 @@
       </c>
       <c r="K9" s="114">
         <f>_xll.qlRateHelperEarliestDate($E9,Trigger)</f>
-        <v>41764</v>
+        <v>41759</v>
       </c>
       <c r="L9" s="113">
         <f>_xll.qlRateHelperLatestDate($E9,Trigger)</f>
-        <v>41948</v>
+        <v>41943</v>
       </c>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.2">
@@ -3667,7 +3667,7 @@
         <v>12F</v>
       </c>
       <c r="E10" s="117" t="str">
-        <f>HKD_YCRH_FRAs_6M!I10</f>
+        <f>FRAs!I10</f>
         <v>HKD_YC6MRH_6x12F#0000</v>
       </c>
       <c r="F10" s="116">
@@ -3687,11 +3687,11 @@
       </c>
       <c r="K10" s="114">
         <f>_xll.qlRateHelperEarliestDate($E10,Trigger)</f>
-        <v>41793</v>
+        <v>41789</v>
       </c>
       <c r="L10" s="113">
         <f>_xll.qlRateHelperLatestDate($E10,Trigger)</f>
-        <v>41976</v>
+        <v>41971</v>
       </c>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.2">
@@ -3706,7 +3706,7 @@
         <v>13F</v>
       </c>
       <c r="E11" s="117" t="str">
-        <f>HKD_YCRH_FRAs_6M!I11</f>
+        <f>FRAs!I11</f>
         <v>HKD_YC6MRH_7x13F#0000</v>
       </c>
       <c r="F11" s="116" t="e">
@@ -3726,11 +3726,11 @@
       </c>
       <c r="K11" s="114">
         <f>_xll.qlRateHelperEarliestDate($E11,Trigger)</f>
-        <v>41823</v>
+        <v>41820</v>
       </c>
       <c r="L11" s="113">
         <f>_xll.qlRateHelperLatestDate($E11,Trigger)</f>
-        <v>42009</v>
+        <v>42004</v>
       </c>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.2">
@@ -3745,7 +3745,7 @@
         <v>14F</v>
       </c>
       <c r="E12" s="117" t="str">
-        <f>HKD_YCRH_FRAs_6M!I12</f>
+        <f>FRAs!I12</f>
         <v>HKD_YC6MRH_8x14F#0000</v>
       </c>
       <c r="F12" s="116" t="e">
@@ -3765,11 +3765,11 @@
       </c>
       <c r="K12" s="114">
         <f>_xll.qlRateHelperEarliestDate($E12,Trigger)</f>
-        <v>41855</v>
+        <v>41851</v>
       </c>
       <c r="L12" s="113">
         <f>_xll.qlRateHelperLatestDate($E12,Trigger)</f>
-        <v>42039</v>
+        <v>42034</v>
       </c>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.2">
@@ -3784,7 +3784,7 @@
         <v>15F</v>
       </c>
       <c r="E13" s="117" t="str">
-        <f>HKD_YCRH_FRAs_6M!I13</f>
+        <f>FRAs!I13</f>
         <v>HKD_YC6MRH_9x15F#0000</v>
       </c>
       <c r="F13" s="116" t="e">
@@ -3804,11 +3804,11 @@
       </c>
       <c r="K13" s="114">
         <f>_xll.qlRateHelperEarliestDate($E13,Trigger)</f>
-        <v>41885</v>
+        <v>41880</v>
       </c>
       <c r="L13" s="113">
         <f>_xll.qlRateHelperLatestDate($E13,Trigger)</f>
-        <v>42066</v>
+        <v>42062</v>
       </c>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.2">
@@ -3823,7 +3823,7 @@
         <v>16F</v>
       </c>
       <c r="E14" s="117" t="str">
-        <f>HKD_YCRH_FRAs_6M!I14</f>
+        <f>FRAs!I14</f>
         <v>HKD_YC6MRH_10x16F#0000</v>
       </c>
       <c r="F14" s="116" t="e">
@@ -3843,11 +3843,11 @@
       </c>
       <c r="K14" s="114">
         <f>_xll.qlRateHelperEarliestDate($E14,Trigger)</f>
-        <v>41915</v>
+        <v>41912</v>
       </c>
       <c r="L14" s="113">
         <f>_xll.qlRateHelperLatestDate($E14,Trigger)</f>
-        <v>42101</v>
+        <v>42094</v>
       </c>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.2">
@@ -3862,7 +3862,7 @@
         <v>17F</v>
       </c>
       <c r="E15" s="117" t="str">
-        <f>HKD_YCRH_FRAs_6M!I15</f>
+        <f>FRAs!I15</f>
         <v>HKD_YC6MRH_11x17F#0000</v>
       </c>
       <c r="F15" s="116" t="e">
@@ -3882,11 +3882,11 @@
       </c>
       <c r="K15" s="114">
         <f>_xll.qlRateHelperEarliestDate($E15,Trigger)</f>
-        <v>41946</v>
+        <v>41943</v>
       </c>
       <c r="L15" s="113">
         <f>_xll.qlRateHelperLatestDate($E15,Trigger)</f>
-        <v>42128</v>
+        <v>42124</v>
       </c>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.2">
@@ -3901,12 +3901,12 @@
         <v>18F</v>
       </c>
       <c r="E16" s="117" t="str">
-        <f>HKD_YCRH_FRAs_6M!I16</f>
+        <f>FRAs!I16</f>
         <v>HKD_YC6MRH_12x18F#0000</v>
       </c>
       <c r="F16" s="116">
         <f>_xll.qlRateHelperQuoteValue($E16,Trigger)</f>
-        <v>6.1000000000000013E-3</v>
+        <v>6.1999999999999998E-3</v>
       </c>
       <c r="G16" s="116"/>
       <c r="H16" s="115" t="b">
@@ -3921,11 +3921,11 @@
       </c>
       <c r="K16" s="114">
         <f>_xll.qlRateHelperEarliestDate($E16,Trigger)</f>
-        <v>41976</v>
+        <v>41971</v>
       </c>
       <c r="L16" s="113">
         <f>_xll.qlRateHelperLatestDate($E16,Trigger)</f>
-        <v>42158</v>
+        <v>42153</v>
       </c>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.2">
@@ -3940,7 +3940,7 @@
         <v>19F</v>
       </c>
       <c r="E17" s="117" t="str">
-        <f>HKD_YCRH_FRAs_6M!I17</f>
+        <f>FRAs!I17</f>
         <v>HKD_YC6MRH_13x19F#0000</v>
       </c>
       <c r="F17" s="116" t="e">
@@ -3960,11 +3960,11 @@
       </c>
       <c r="K17" s="114">
         <f>_xll.qlRateHelperEarliestDate($E17,Trigger)</f>
-        <v>42009</v>
+        <v>42004</v>
       </c>
       <c r="L17" s="113">
         <f>_xll.qlRateHelperLatestDate($E17,Trigger)</f>
-        <v>42191</v>
+        <v>42185</v>
       </c>
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.2">
@@ -3979,7 +3979,7 @@
         <v>20F</v>
       </c>
       <c r="E18" s="117" t="str">
-        <f>HKD_YCRH_FRAs_6M!I18</f>
+        <f>FRAs!I18</f>
         <v>HKD_YC6MRH_14x20F#0000</v>
       </c>
       <c r="F18" s="116" t="e">
@@ -3999,11 +3999,11 @@
       </c>
       <c r="K18" s="114">
         <f>_xll.qlRateHelperEarliestDate($E18,Trigger)</f>
-        <v>42038</v>
+        <v>42034</v>
       </c>
       <c r="L18" s="113">
         <f>_xll.qlRateHelperLatestDate($E18,Trigger)</f>
-        <v>42219</v>
+        <v>42216</v>
       </c>
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.2">
@@ -4018,7 +4018,7 @@
         <v>21F</v>
       </c>
       <c r="E19" s="117" t="str">
-        <f>HKD_YCRH_FRAs_6M!I19</f>
+        <f>FRAs!I19</f>
         <v>HKD_YC6MRH_15x21F#0000</v>
       </c>
       <c r="F19" s="116" t="e">
@@ -4038,11 +4038,11 @@
       </c>
       <c r="K19" s="114">
         <f>_xll.qlRateHelperEarliestDate($E19,Trigger)</f>
-        <v>42066</v>
+        <v>42062</v>
       </c>
       <c r="L19" s="113">
         <f>_xll.qlRateHelperLatestDate($E19,Trigger)</f>
-        <v>42250</v>
+        <v>42247</v>
       </c>
     </row>
     <row r="20" spans="2:12" x14ac:dyDescent="0.2">
@@ -4057,7 +4057,7 @@
         <v>22F</v>
       </c>
       <c r="E20" s="117" t="str">
-        <f>HKD_YCRH_FRAs_6M!I20</f>
+        <f>FRAs!I20</f>
         <v>HKD_YC6MRH_16x22F#0000</v>
       </c>
       <c r="F20" s="116" t="e">
@@ -4077,11 +4077,11 @@
       </c>
       <c r="K20" s="114">
         <f>_xll.qlRateHelperEarliestDate($E20,Trigger)</f>
-        <v>42101</v>
+        <v>42094</v>
       </c>
       <c r="L20" s="113">
         <f>_xll.qlRateHelperLatestDate($E20,Trigger)</f>
-        <v>42284</v>
+        <v>42277</v>
       </c>
     </row>
     <row r="21" spans="2:12" x14ac:dyDescent="0.2">
@@ -4096,7 +4096,7 @@
         <v>23F</v>
       </c>
       <c r="E21" s="117" t="str">
-        <f>HKD_YCRH_FRAs_6M!I21</f>
+        <f>FRAs!I21</f>
         <v>HKD_YC6MRH_17x23F#0000</v>
       </c>
       <c r="F21" s="116" t="e">
@@ -4116,11 +4116,11 @@
       </c>
       <c r="K21" s="114">
         <f>_xll.qlRateHelperEarliestDate($E21,Trigger)</f>
-        <v>42128</v>
+        <v>42124</v>
       </c>
       <c r="L21" s="113">
         <f>_xll.qlRateHelperLatestDate($E21,Trigger)</f>
-        <v>42312</v>
+        <v>42307</v>
       </c>
     </row>
     <row r="22" spans="2:12" x14ac:dyDescent="0.2">
@@ -4135,12 +4135,12 @@
         <v>24F</v>
       </c>
       <c r="E22" s="110" t="str">
-        <f>HKD_YCRH_FRAs_6M!I22</f>
+        <f>FRAs!I22</f>
         <v>HKD_YC6MRH_18x24F#0000</v>
       </c>
       <c r="F22" s="109">
         <f>_xll.qlRateHelperQuoteValue($E22,Trigger)</f>
-        <v>7.7000000000000002E-3</v>
+        <v>7.8000000000000005E-3</v>
       </c>
       <c r="G22" s="109"/>
       <c r="H22" s="108" t="b">
@@ -4155,11 +4155,11 @@
       </c>
       <c r="K22" s="107">
         <f>_xll.qlRateHelperEarliestDate($E22,Trigger)</f>
-        <v>42158</v>
+        <v>42153</v>
       </c>
       <c r="L22" s="106">
         <f>_xll.qlRateHelperLatestDate($E22,Trigger)</f>
-        <v>42341</v>
+        <v>42338</v>
       </c>
     </row>
     <row r="23" spans="2:12" x14ac:dyDescent="0.2">
@@ -5817,7 +5817,7 @@
         <v>8</v>
       </c>
       <c r="D2" s="9" t="str">
-        <f t="array" ref="D2:D126">_xll.qlRateHelperSelection(_xll.ohFilter(RateHelpers,RateHelpersIncluded),_xll.ohFilter(RateHelpersPriority,RateHelpersIncluded),nIMMFutures,nSerialFutures,FrontFuturesRollingDays,DepoInclusionCriteria,_xll.ohFilter(MinDistance,RateHelpersIncluded),ISERROR(HKD_YCRH_FRAs_6M!RateHelperConstructors))</f>
+        <f t="array" ref="D2:D126">_xll.qlRateHelperSelection(_xll.ohFilter(RateHelpers,RateHelpersIncluded),_xll.ohFilter(RateHelpersPriority,RateHelpersIncluded),nIMMFutures,nSerialFutures,FrontFuturesRollingDays,DepoInclusionCriteria,_xll.ohFilter(MinDistance,RateHelpersIncluded),ISERROR(FRAs!RateHelperConstructors))</f>
         <v>HkdHibor6MLastFixing</v>
       </c>
       <c r="E2" s="10">
@@ -5830,14 +5830,14 @@
       </c>
       <c r="G2" s="11">
         <f>_xll.qlRateHelperEarliestDate($D2)</f>
-        <v>41611</v>
+        <v>41607</v>
       </c>
       <c r="H2" s="12">
         <f>_xll.qlRateHelperLatestDate($D2)</f>
-        <v>41793</v>
+        <v>41789</v>
       </c>
       <c r="I2" s="6">
-        <v>0.99721225668296354</v>
+        <v>0.9972721263068568</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
@@ -5860,14 +5860,14 @@
       </c>
       <c r="G3" s="11">
         <f>_xll.qlRateHelperEarliestDate($D3)</f>
-        <v>41642</v>
+        <v>41639</v>
       </c>
       <c r="H3" s="12">
         <f>_xll.qlRateHelperLatestDate($D3)</f>
-        <v>41823</v>
+        <v>41820</v>
       </c>
       <c r="I3" s="6">
-        <v>0.99705212994891101</v>
+        <v>0.99709702461977379</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
@@ -5890,14 +5890,14 @@
       </c>
       <c r="G4" s="11">
         <f>_xll.qlRateHelperEarliestDate($D4)</f>
-        <v>41673</v>
+        <v>41670</v>
       </c>
       <c r="H4" s="12">
         <f>_xll.qlRateHelperLatestDate($D4)</f>
-        <v>41855</v>
+        <v>41851</v>
       </c>
       <c r="I4" s="6">
-        <v>0.99657499044919295</v>
+        <v>0.99663321048504716</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -5920,14 +5920,14 @@
       </c>
       <c r="G5" s="11">
         <f>_xll.qlRateHelperEarliestDate($D5)</f>
-        <v>41701</v>
+        <v>41698</v>
       </c>
       <c r="H5" s="12">
         <f>_xll.qlRateHelperLatestDate($D5)</f>
-        <v>41885</v>
+        <v>41880</v>
       </c>
       <c r="I5" s="6">
-        <v>0.99607950165484438</v>
+        <v>0.99615157573737345</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
@@ -5951,14 +5951,14 @@
       </c>
       <c r="G6" s="11">
         <f>_xll.qlRateHelperEarliestDate($D6)</f>
-        <v>41732</v>
+        <v>41729</v>
       </c>
       <c r="H6" s="12">
         <f>_xll.qlRateHelperLatestDate($D6)</f>
-        <v>41915</v>
+        <v>41912</v>
       </c>
       <c r="I6" s="6">
-        <v>0.99557997474673687</v>
+        <v>0.99562480313027002</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="12" thickBot="1" x14ac:dyDescent="0.25">
@@ -5983,14 +5983,14 @@
       </c>
       <c r="G7" s="11">
         <f>_xll.qlRateHelperEarliestDate($D7)</f>
-        <v>41764</v>
+        <v>41759</v>
       </c>
       <c r="H7" s="12">
         <f>_xll.qlRateHelperLatestDate($D7)</f>
-        <v>41948</v>
+        <v>41943</v>
       </c>
       <c r="I7" s="6">
-        <v>0.99503803019528603</v>
+        <v>0.9951127046180217</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
@@ -6007,14 +6007,14 @@
       </c>
       <c r="G8" s="11">
         <f>_xll.qlRateHelperEarliestDate($D8)</f>
-        <v>41793</v>
+        <v>41789</v>
       </c>
       <c r="H8" s="12">
         <f>_xll.qlRateHelperLatestDate($D8)</f>
-        <v>41976</v>
+        <v>41971</v>
       </c>
       <c r="I8" s="6">
-        <v>0.99451969678061169</v>
+        <v>0.99459407956331003</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
@@ -6023,7 +6023,7 @@
       </c>
       <c r="E9" s="10">
         <f>_xll.qlRateHelperRate($D9)</f>
-        <v>6.1000000000000013E-3</v>
+        <v>6.1999999999999998E-3</v>
       </c>
       <c r="F9" s="10" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D9)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D9)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D9)),_xll.qlSwapRateHelperSpread($D9))</f>
@@ -6031,14 +6031,14 @@
       </c>
       <c r="G9" s="11">
         <f>_xll.qlRateHelperEarliestDate($D9)</f>
-        <v>41976</v>
+        <v>41971</v>
       </c>
       <c r="H9" s="12">
         <f>_xll.qlRateHelperLatestDate($D9)</f>
-        <v>42158</v>
+        <v>42153</v>
       </c>
       <c r="I9" s="6">
-        <v>0.99150389507018177</v>
+        <v>0.99152876160551362</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
@@ -6047,7 +6047,7 @@
       </c>
       <c r="E10" s="10">
         <f>_xll.qlRateHelperRate($D10)</f>
-        <v>7.7000000000000002E-3</v>
+        <v>7.8000000000000005E-3</v>
       </c>
       <c r="F10" s="10" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D10)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D10)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D10)),_xll.qlSwapRateHelperSpread($D10))</f>
@@ -6055,14 +6055,14 @@
       </c>
       <c r="G10" s="11">
         <f>_xll.qlRateHelperEarliestDate($D10)</f>
-        <v>42158</v>
+        <v>42153</v>
       </c>
       <c r="H10" s="12">
         <f>_xll.qlRateHelperLatestDate($D10)</f>
-        <v>42341</v>
+        <v>42338</v>
       </c>
       <c r="I10" s="6">
-        <v>0.98769086712261345</v>
+        <v>0.98762426348985388</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
fixed relinkable handles, removed jumps, fixed links, temporary enabled 1M and 6M extrapolation
</commit_message>
<xml_diff>
--- a/QuantLibXL/Data2/XLS/HKD_YC6MBootstrapping.xlsx
+++ b/QuantLibXL/Data2/XLS/HKD_YC6MBootstrapping.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="22890" yWindow="-15" windowWidth="7635" windowHeight="11085"/>
+    <workbookView xWindow="210" yWindow="270" windowWidth="15165" windowHeight="7710"/>
   </bookViews>
   <sheets>
     <sheet name="General Settings" sheetId="3" r:id="rId1"/>
@@ -1177,7 +1177,7 @@
     <xf numFmtId="173" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="173" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="151">
+  <cellXfs count="156">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1388,12 +1388,6 @@
     <xf numFmtId="170" fontId="17" fillId="9" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="17" fillId="9" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="9" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="17" fillId="9" borderId="27" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="17" fillId="9" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1498,23 +1492,29 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="27" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="10" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="27" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="166" fontId="17" fillId="9" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="19" fillId="6" borderId="16" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="19" fillId="6" borderId="20" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="29" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1524,6 +1524,21 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="30" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="30" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="10">
@@ -1838,39 +1853,41 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:K31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="2.7109375" style="146" customWidth="1"/>
-    <col min="3" max="3" width="18" style="146" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.85546875" style="146" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22" style="146" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="2.7109375" style="146" customWidth="1"/>
-    <col min="9" max="9" width="12.140625" style="146" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="48.42578125" style="146" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="2.7109375" style="146" customWidth="1"/>
-    <col min="12" max="16384" width="8" style="146"/>
+    <col min="1" max="2" width="2.7109375" style="139" customWidth="1"/>
+    <col min="3" max="3" width="18" style="139" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.85546875" style="139" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22" style="139" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="2.7109375" style="139" customWidth="1"/>
+    <col min="9" max="9" width="12.140625" style="139" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="48.42578125" style="139" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="2.7109375" style="139" customWidth="1"/>
+    <col min="12" max="16384" width="8" style="139"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="145"/>
-      <c r="B1" s="145" t="str">
+      <c r="A1" s="138"/>
+      <c r="B1" s="138" t="str">
         <f>_xll.qlxlVersion(TRUE,Trigger)</f>
-        <v>QuantLibXL 1.4.0 - MS VC++ 9.0 - Multithreaded Dynamic Runtime library - Release Configuration - Feb  7 2014 15:33:58</v>
-      </c>
-      <c r="C1" s="145"/>
-      <c r="D1" s="145"/>
-      <c r="E1" s="145"/>
-      <c r="F1" s="145"/>
-      <c r="G1" s="145"/>
-      <c r="H1" s="145"/>
-      <c r="I1" s="145"/>
-      <c r="J1" s="145"/>
-      <c r="K1" s="145"/>
+        <v>QuantLibXL 1.4.0 - MS VC++ 9.0 - Multithreaded Dynamic Runtime library - Release Configuration - Mar  3 2014 10:58:57</v>
+      </c>
+      <c r="C1" s="138"/>
+      <c r="D1" s="138"/>
+      <c r="E1" s="138"/>
+      <c r="F1" s="138"/>
+      <c r="G1" s="138"/>
+      <c r="H1" s="138"/>
+      <c r="I1" s="138"/>
+      <c r="J1" s="138"/>
+      <c r="K1" s="138"/>
     </row>
     <row r="2" spans="1:11" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="145"/>
+      <c r="A2" s="138"/>
       <c r="B2" s="147" t="s">
         <v>7</v>
       </c>
@@ -1878,7 +1895,7 @@
       <c r="D2" s="148"/>
       <c r="E2" s="148"/>
       <c r="F2" s="149"/>
-      <c r="G2" s="145"/>
+      <c r="G2" s="138"/>
       <c r="H2" s="147" t="s">
         <v>53</v>
       </c>
@@ -1887,43 +1904,43 @@
       <c r="K2" s="150"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A3" s="145"/>
+      <c r="A3" s="138"/>
       <c r="B3" s="62"/>
       <c r="C3" s="63"/>
       <c r="D3" s="64"/>
       <c r="E3" s="64"/>
       <c r="F3" s="65"/>
-      <c r="G3" s="145"/>
+      <c r="G3" s="138"/>
       <c r="H3" s="66"/>
       <c r="I3" s="67"/>
       <c r="J3" s="67"/>
       <c r="K3" s="68"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" s="145"/>
+      <c r="A4" s="138"/>
       <c r="B4" s="62"/>
-      <c r="C4" s="126" t="s">
+      <c r="C4" s="124" t="s">
         <v>33</v>
       </c>
-      <c r="D4" s="101">
+      <c r="D4" s="99">
         <v>6</v>
       </c>
       <c r="E4" s="64"/>
       <c r="F4" s="65"/>
-      <c r="G4" s="145"/>
+      <c r="G4" s="138"/>
       <c r="H4" s="66"/>
-      <c r="I4" s="134" t="s">
+      <c r="I4" s="132" t="s">
         <v>6</v>
       </c>
       <c r="J4" s="70">
-        <v>41684.564930555556</v>
+        <v>41736.631990740738</v>
       </c>
       <c r="K4" s="71"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A5" s="145"/>
+      <c r="A5" s="138"/>
       <c r="B5" s="62"/>
-      <c r="C5" s="127" t="s">
+      <c r="C5" s="125" t="s">
         <v>29</v>
       </c>
       <c r="D5" s="72" t="str">
@@ -1932,9 +1949,9 @@
       </c>
       <c r="E5" s="64"/>
       <c r="F5" s="65"/>
-      <c r="G5" s="145"/>
+      <c r="G5" s="138"/>
       <c r="H5" s="66"/>
-      <c r="I5" s="134" t="s">
+      <c r="I5" s="132" t="s">
         <v>13</v>
       </c>
       <c r="J5" s="70" t="b">
@@ -1943,9 +1960,9 @@
       <c r="K5" s="71"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6" s="145"/>
+      <c r="A6" s="138"/>
       <c r="B6" s="62"/>
-      <c r="C6" s="127" t="s">
+      <c r="C6" s="125" t="s">
         <v>34</v>
       </c>
       <c r="D6" s="72" t="s">
@@ -1953,9 +1970,9 @@
       </c>
       <c r="E6" s="64"/>
       <c r="F6" s="65"/>
-      <c r="G6" s="145"/>
+      <c r="G6" s="138"/>
       <c r="H6" s="66"/>
-      <c r="I6" s="134" t="s">
+      <c r="I6" s="132" t="s">
         <v>26</v>
       </c>
       <c r="J6" s="70" t="b">
@@ -1964,9 +1981,9 @@
       <c r="K6" s="71"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A7" s="145"/>
+      <c r="A7" s="138"/>
       <c r="B7" s="62"/>
-      <c r="C7" s="127" t="s">
+      <c r="C7" s="125" t="s">
         <v>35</v>
       </c>
       <c r="D7" s="72" t="s">
@@ -1974,9 +1991,9 @@
       </c>
       <c r="E7" s="64"/>
       <c r="F7" s="65"/>
-      <c r="G7" s="145"/>
+      <c r="G7" s="138"/>
       <c r="H7" s="66"/>
-      <c r="I7" s="134" t="s">
+      <c r="I7" s="132" t="s">
         <v>52</v>
       </c>
       <c r="J7" s="70" t="b">
@@ -1985,9 +2002,9 @@
       <c r="K7" s="71"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A8" s="145"/>
+      <c r="A8" s="138"/>
       <c r="B8" s="62"/>
-      <c r="C8" s="128" t="s">
+      <c r="C8" s="126" t="s">
         <v>23</v>
       </c>
       <c r="D8" s="76" t="str">
@@ -1996,27 +2013,27 @@
       </c>
       <c r="E8" s="64"/>
       <c r="F8" s="65"/>
-      <c r="G8" s="145"/>
+      <c r="G8" s="138"/>
       <c r="H8" s="66"/>
-      <c r="I8" s="134" t="s">
+      <c r="I8" s="132" t="s">
         <v>51</v>
       </c>
       <c r="J8" s="70" t="str">
         <f ca="1">SUBSTITUTE(LEFT(CELL("filename",A1),FIND("[",CELL("filename",A1),1)-1),"\XLS\","\XML\")</f>
-        <v>C:\Users\erik\Documents\repos\quantlib\QuantLibXL\Data2\XML\</v>
+        <v>C:\Projects\quantlib\QuantLibXL\Data2\XML\</v>
       </c>
       <c r="K8" s="71"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A9" s="145"/>
+      <c r="A9" s="138"/>
       <c r="B9" s="62"/>
-      <c r="C9" s="129"/>
+      <c r="C9" s="127"/>
       <c r="D9" s="77"/>
       <c r="E9" s="64"/>
       <c r="F9" s="65"/>
-      <c r="G9" s="145"/>
+      <c r="G9" s="138"/>
       <c r="H9" s="66"/>
-      <c r="I9" s="134" t="s">
+      <c r="I9" s="132" t="s">
         <v>50</v>
       </c>
       <c r="J9" s="70" t="b">
@@ -2025,45 +2042,45 @@
       <c r="K9" s="71"/>
     </row>
     <row r="10" spans="1:11" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="145"/>
+      <c r="A10" s="138"/>
       <c r="B10" s="62"/>
-      <c r="C10" s="130" t="s">
+      <c r="C10" s="128" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="70" t="str">
-        <f>_xll.qlPiecewiseYieldCurve(D12,NDays,Calendar,RateHelpersSelected,DayCounter,IF(ISERROR(D17),NA(),D15:E15),IF(ISERROR(D17),NA(),D16:E16),Accuracy,TraitsID,InterpolatorID,Permanent,,ObjectOverwrite)</f>
-        <v>HKDYC6M#0003</v>
+      <c r="D10" s="146" t="str">
+        <f>_xll.qlPiecewiseYieldCurve(D12,NDays,Calendar,RateHelpersSelected,DayCounter,,,Accuracy,TraitsID,InterpolatorID,Permanent,,ObjectOverwrite)</f>
+        <v>HKDYC6M#0000</v>
       </c>
       <c r="E10" s="64"/>
       <c r="F10" s="65"/>
-      <c r="G10" s="145"/>
+      <c r="G10" s="138"/>
       <c r="H10" s="73"/>
       <c r="I10" s="74"/>
       <c r="J10" s="74"/>
       <c r="K10" s="75"/>
     </row>
     <row r="11" spans="1:11" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="145"/>
+      <c r="A11" s="138"/>
       <c r="B11" s="62"/>
-      <c r="C11" s="131" t="s">
+      <c r="C11" s="129" t="s">
         <v>15</v>
       </c>
-      <c r="D11" s="70" t="str">
+      <c r="D11" s="145" t="str">
         <f>_xll.ohRangeRetrieveError(YieldCurve)</f>
         <v/>
       </c>
       <c r="E11" s="64"/>
       <c r="F11" s="65"/>
-      <c r="G11" s="145"/>
-      <c r="H11" s="145"/>
-      <c r="I11" s="145"/>
-      <c r="J11" s="145"/>
-      <c r="K11" s="145"/>
+      <c r="G11" s="138"/>
+      <c r="H11" s="138"/>
+      <c r="I11" s="138"/>
+      <c r="J11" s="138"/>
+      <c r="K11" s="138"/>
     </row>
     <row r="12" spans="1:11" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="145"/>
+      <c r="A12" s="138"/>
       <c r="B12" s="62"/>
-      <c r="C12" s="130" t="s">
+      <c r="C12" s="128" t="s">
         <v>9</v>
       </c>
       <c r="D12" s="81" t="str">
@@ -2072,7 +2089,7 @@
       </c>
       <c r="E12" s="64"/>
       <c r="F12" s="65"/>
-      <c r="G12" s="145"/>
+      <c r="G12" s="138"/>
       <c r="H12" s="147" t="s">
         <v>49</v>
       </c>
@@ -2081,9 +2098,9 @@
       <c r="K12" s="150"/>
     </row>
     <row r="13" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A13" s="145"/>
+      <c r="A13" s="138"/>
       <c r="B13" s="62"/>
-      <c r="C13" s="132" t="s">
+      <c r="C13" s="130" t="s">
         <v>10</v>
       </c>
       <c r="D13" s="82">
@@ -2091,24 +2108,24 @@
       </c>
       <c r="E13" s="64"/>
       <c r="F13" s="65"/>
-      <c r="G13" s="145"/>
+      <c r="G13" s="138"/>
       <c r="H13" s="78"/>
       <c r="I13" s="79"/>
       <c r="J13" s="79"/>
       <c r="K13" s="80"/>
     </row>
     <row r="14" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A14" s="145"/>
+      <c r="A14" s="138"/>
       <c r="B14" s="62"/>
-      <c r="C14" s="132" t="s">
+      <c r="C14" s="130" t="s">
         <v>8</v>
       </c>
       <c r="D14" s="86"/>
       <c r="E14" s="64"/>
       <c r="F14" s="65"/>
-      <c r="G14" s="145"/>
+      <c r="G14" s="138"/>
       <c r="H14" s="78"/>
-      <c r="I14" s="134" t="s">
+      <c r="I14" s="132" t="s">
         <v>5</v>
       </c>
       <c r="J14" s="70" t="s">
@@ -2117,9 +2134,9 @@
       <c r="K14" s="80"/>
     </row>
     <row r="15" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A15" s="145"/>
+      <c r="A15" s="138"/>
       <c r="B15" s="62"/>
-      <c r="C15" s="132" t="s">
+      <c r="C15" s="130" t="s">
         <v>31</v>
       </c>
       <c r="D15" s="87" t="str">
@@ -2131,9 +2148,9 @@
         <v>HKDTOY2_SYNTH6M_Quote</v>
       </c>
       <c r="F15" s="65"/>
-      <c r="G15" s="145"/>
+      <c r="G15" s="138"/>
       <c r="H15" s="78"/>
-      <c r="I15" s="134" t="s">
+      <c r="I15" s="132" t="s">
         <v>48</v>
       </c>
       <c r="J15" s="70" t="s">
@@ -2142,9 +2159,9 @@
       <c r="K15" s="80"/>
     </row>
     <row r="16" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A16" s="145"/>
+      <c r="A16" s="138"/>
       <c r="B16" s="62"/>
-      <c r="C16" s="132" t="s">
+      <c r="C16" s="130" t="s">
         <v>32</v>
       </c>
       <c r="D16" s="88">
@@ -2156,9 +2173,9 @@
         <v>42369</v>
       </c>
       <c r="F16" s="65"/>
-      <c r="G16" s="145"/>
+      <c r="G16" s="138"/>
       <c r="H16" s="78"/>
-      <c r="I16" s="134" t="s">
+      <c r="I16" s="132" t="s">
         <v>46</v>
       </c>
       <c r="J16" s="70" t="s">
@@ -2167,9 +2184,9 @@
       <c r="K16" s="80"/>
     </row>
     <row r="17" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A17" s="145"/>
+      <c r="A17" s="138"/>
       <c r="B17" s="62"/>
-      <c r="C17" s="132" t="s">
+      <c r="C17" s="130" t="s">
         <v>36</v>
       </c>
       <c r="D17" s="90" t="e">
@@ -2181,35 +2198,35 @@
         <v>#N/A</v>
       </c>
       <c r="F17" s="65"/>
-      <c r="G17" s="145"/>
-      <c r="H17" s="133"/>
-      <c r="I17" s="134" t="s">
+      <c r="G17" s="138"/>
+      <c r="H17" s="131"/>
+      <c r="I17" s="132" t="s">
         <v>4</v>
       </c>
-      <c r="J17" s="135" t="s">
+      <c r="J17" s="133" t="s">
         <v>43</v>
       </c>
-      <c r="K17" s="136"/>
+      <c r="K17" s="134"/>
     </row>
     <row r="18" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="145"/>
+      <c r="A18" s="138"/>
       <c r="B18" s="62"/>
-      <c r="C18" s="132" t="s">
+      <c r="C18" s="130" t="s">
         <v>22</v>
       </c>
       <c r="D18" s="92"/>
       <c r="E18" s="64"/>
       <c r="F18" s="65"/>
-      <c r="G18" s="145"/>
+      <c r="G18" s="138"/>
       <c r="H18" s="83"/>
       <c r="I18" s="84"/>
       <c r="J18" s="84"/>
       <c r="K18" s="85"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A19" s="145"/>
+      <c r="A19" s="138"/>
       <c r="B19" s="62"/>
-      <c r="C19" s="132" t="s">
+      <c r="C19" s="130" t="s">
         <v>11</v>
       </c>
       <c r="D19" s="72" t="s">
@@ -2217,16 +2234,16 @@
       </c>
       <c r="E19" s="64"/>
       <c r="F19" s="65"/>
-      <c r="G19" s="145"/>
-      <c r="H19" s="145"/>
-      <c r="I19" s="145"/>
-      <c r="J19" s="145"/>
-      <c r="K19" s="145"/>
+      <c r="G19" s="138"/>
+      <c r="H19" s="138"/>
+      <c r="I19" s="138"/>
+      <c r="J19" s="138"/>
+      <c r="K19" s="138"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A20" s="145"/>
+      <c r="A20" s="138"/>
       <c r="B20" s="62"/>
-      <c r="C20" s="131" t="s">
+      <c r="C20" s="129" t="s">
         <v>12</v>
       </c>
       <c r="D20" s="76" t="s">
@@ -2234,31 +2251,31 @@
       </c>
       <c r="E20" s="64"/>
       <c r="F20" s="65"/>
-      <c r="G20" s="145"/>
-      <c r="H20" s="145"/>
-      <c r="I20" s="145"/>
-      <c r="J20" s="145"/>
-      <c r="K20" s="145"/>
+      <c r="G20" s="138"/>
+      <c r="H20" s="138"/>
+      <c r="I20" s="138"/>
+      <c r="J20" s="138"/>
+      <c r="K20" s="138"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A21" s="145"/>
+      <c r="A21" s="138"/>
       <c r="B21" s="62"/>
       <c r="C21" s="77"/>
       <c r="D21" s="77"/>
       <c r="E21" s="64"/>
       <c r="F21" s="65"/>
-      <c r="G21" s="145"/>
-      <c r="H21" s="145"/>
-      <c r="I21" s="145"/>
-      <c r="J21" s="145"/>
-      <c r="K21" s="145"/>
+      <c r="G21" s="138"/>
+      <c r="H21" s="138"/>
+      <c r="I21" s="138"/>
+      <c r="J21" s="138"/>
+      <c r="K21" s="138"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A22" s="145"/>
+      <c r="A22" s="138"/>
       <c r="B22" s="62"/>
       <c r="C22" s="93">
         <f>_xll.qlTermStructureReferenceDate(YieldCurve)</f>
-        <v>41684</v>
+        <v>41736</v>
       </c>
       <c r="D22" s="94">
         <f>MAX(_xll.ohPack(Selected!I1:I20))</f>
@@ -2266,107 +2283,121 @@
       </c>
       <c r="E22" s="64"/>
       <c r="F22" s="65"/>
-      <c r="G22" s="145"/>
-      <c r="H22" s="145"/>
-      <c r="I22" s="145"/>
-      <c r="J22" s="145"/>
-      <c r="K22" s="145"/>
+      <c r="G22" s="138"/>
+      <c r="H22" s="138"/>
+      <c r="I22" s="138"/>
+      <c r="J22" s="138"/>
+      <c r="K22" s="138"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A23" s="145"/>
+      <c r="A23" s="138"/>
       <c r="B23" s="62"/>
       <c r="C23" s="95">
         <f>MAX(_xll.ohPack(Selected!H2:H126))</f>
-        <v>42415</v>
+        <v>42467</v>
       </c>
       <c r="D23" s="72">
         <f>MIN(_xll.ohPack(Selected!I1:I20))</f>
-        <v>0.98772918348282057</v>
+        <v>0.98384748690248558</v>
       </c>
       <c r="E23" s="64"/>
       <c r="F23" s="65"/>
-      <c r="G23" s="145"/>
-      <c r="H23" s="145"/>
-      <c r="I23" s="145"/>
-      <c r="J23" s="145"/>
-      <c r="K23" s="145"/>
+      <c r="G23" s="138"/>
+      <c r="H23" s="138"/>
+      <c r="I23" s="138"/>
+      <c r="J23" s="138"/>
+      <c r="K23" s="138"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A24" s="145"/>
+      <c r="A24" s="138"/>
       <c r="B24" s="62"/>
-      <c r="C24" s="96" t="s">
+      <c r="C24" s="141" t="s">
         <v>15</v>
       </c>
-      <c r="D24" s="97" t="str">
+      <c r="D24" s="142" t="str">
         <f>_xll.ohRangeRetrieveError(Selected!I1)</f>
         <v/>
       </c>
       <c r="E24" s="64"/>
       <c r="F24" s="65"/>
-      <c r="G24" s="145"/>
-      <c r="H24" s="145"/>
-      <c r="I24" s="145"/>
-      <c r="J24" s="145"/>
-      <c r="K24" s="145"/>
-    </row>
-    <row r="25" spans="1:11" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="145"/>
-      <c r="B25" s="98"/>
-      <c r="C25" s="137"/>
-      <c r="D25" s="137"/>
-      <c r="E25" s="99"/>
-      <c r="F25" s="100"/>
-      <c r="G25" s="145"/>
-      <c r="H25" s="145"/>
-      <c r="I25" s="145"/>
-      <c r="J25" s="145"/>
-      <c r="K25" s="145"/>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A26" s="145"/>
-      <c r="G26" s="145"/>
-      <c r="H26" s="145"/>
-      <c r="I26" s="145"/>
-      <c r="J26" s="145"/>
-      <c r="K26" s="145"/>
+      <c r="G24" s="138"/>
+      <c r="H24" s="138"/>
+      <c r="I24" s="138"/>
+      <c r="J24" s="138"/>
+      <c r="K24" s="138"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A25" s="138"/>
+      <c r="B25" s="62"/>
+      <c r="C25" s="143" t="str">
+        <f>UPPER(Currency)&amp;"6M"</f>
+        <v>HKD6M</v>
+      </c>
+      <c r="D25" s="144" t="b">
+        <f>_xll.qlRelinkableHandleLinkTo(C25,YieldCurve)</f>
+        <v>1</v>
+      </c>
+      <c r="E25" s="64"/>
+      <c r="F25" s="65"/>
+      <c r="G25" s="138"/>
+      <c r="H25" s="138"/>
+      <c r="I25" s="138"/>
+      <c r="J25" s="138"/>
+      <c r="K25" s="138"/>
+    </row>
+    <row r="26" spans="1:11" ht="12" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="138"/>
+      <c r="B26" s="96"/>
+      <c r="C26" s="140"/>
+      <c r="D26" s="135" t="b">
+        <f>_xll.qlExtrapolatorEnableExtrapolation(YieldCurve,TRUE)</f>
+        <v>1</v>
+      </c>
+      <c r="E26" s="97"/>
+      <c r="F26" s="98"/>
+      <c r="G26" s="138"/>
+      <c r="H26" s="138"/>
+      <c r="I26" s="138"/>
+      <c r="J26" s="138"/>
+      <c r="K26" s="138"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A27" s="145"/>
-      <c r="G27" s="145"/>
-      <c r="H27" s="145"/>
-      <c r="I27" s="145"/>
-      <c r="J27" s="145"/>
-      <c r="K27" s="145"/>
+      <c r="A27" s="138"/>
+      <c r="G27" s="138"/>
+      <c r="H27" s="138"/>
+      <c r="I27" s="138"/>
+      <c r="J27" s="138"/>
+      <c r="K27" s="138"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A28" s="145"/>
-      <c r="G28" s="145"/>
-      <c r="H28" s="145"/>
-      <c r="I28" s="145"/>
-      <c r="J28" s="145"/>
-      <c r="K28" s="145"/>
+      <c r="A28" s="138"/>
+      <c r="G28" s="138"/>
+      <c r="H28" s="138"/>
+      <c r="I28" s="138"/>
+      <c r="J28" s="138"/>
+      <c r="K28" s="138"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A29" s="145"/>
-      <c r="G29" s="145"/>
-      <c r="H29" s="145"/>
-      <c r="I29" s="145"/>
-      <c r="J29" s="145"/>
-      <c r="K29" s="145"/>
+      <c r="A29" s="138"/>
+      <c r="G29" s="138"/>
+      <c r="H29" s="138"/>
+      <c r="I29" s="138"/>
+      <c r="J29" s="138"/>
+      <c r="K29" s="138"/>
     </row>
     <row r="30" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="145"/>
-      <c r="G30" s="145"/>
-      <c r="H30" s="145"/>
-      <c r="I30" s="145"/>
-      <c r="J30" s="145"/>
-      <c r="K30" s="145"/>
+      <c r="A30" s="138"/>
+      <c r="G30" s="138"/>
+      <c r="H30" s="138"/>
+      <c r="I30" s="138"/>
+      <c r="J30" s="138"/>
+      <c r="K30" s="138"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="H31" s="145"/>
-      <c r="I31" s="145"/>
-      <c r="J31" s="145"/>
-      <c r="K31" s="145"/>
+      <c r="H31" s="138"/>
+      <c r="I31" s="138"/>
+      <c r="J31" s="138"/>
+      <c r="K31" s="138"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -2375,7 +2406,7 @@
     <mergeCell ref="H12:K12"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
-  <dataValidations count="6">
+  <dataValidations disablePrompts="1" count="6">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D14">
       <formula1>"Actual/Actual (ISDA),Actual/360,30/360 (Bond Basis),30E/360 (Eurobond Basis),Actual/365 (Fixed),Actual/Actual (ISMA),Actual/Actual (AFB),'1/1,30/360 (Italian),Simple"</formula1>
     </dataValidation>
@@ -2501,7 +2532,7 @@
       </c>
       <c r="I3" s="38" t="str">
         <f>_xll.qlFraRateHelper(H3,G3,B3,E3,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC6MRH_T6F1#0002</v>
+        <v>HKD_YC6MRH_T6F1#0000</v>
       </c>
       <c r="J3" s="47" t="str">
         <f>_xll.ohRangeRetrieveError(I3)</f>
@@ -2538,7 +2569,7 @@
       </c>
       <c r="I4" s="43" t="str">
         <f>_xll.qlFraRateHelper(H4,G4,B4,E4,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC6MRH_TOM6F1#0002</v>
+        <v>HKD_YC6MRH_TOM6F1#0000</v>
       </c>
       <c r="J4" s="42" t="str">
         <f>_xll.ohRangeRetrieveError(I4)</f>
@@ -2576,7 +2607,7 @@
       </c>
       <c r="I5" s="38" t="str">
         <f>_xll.qlFraRateHelper(H5,G5,B5,E5,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC6MRH_1x7F#0002</v>
+        <v>HKD_YC6MRH_1x7F#0000</v>
       </c>
       <c r="J5" s="37" t="str">
         <f>_xll.ohRangeRetrieveError(I5)</f>
@@ -2614,7 +2645,7 @@
       </c>
       <c r="I6" s="32" t="str">
         <f>_xll.qlFraRateHelper(H6,G6,B6,E6,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC6MRH_2x8F#0002</v>
+        <v>HKD_YC6MRH_2x8F#0000</v>
       </c>
       <c r="J6" s="31" t="str">
         <f>_xll.ohRangeRetrieveError(I6)</f>
@@ -2652,7 +2683,7 @@
       </c>
       <c r="I7" s="32" t="str">
         <f>_xll.qlFraRateHelper(H7,G7,B7,E7,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC6MRH_3x9F#0002</v>
+        <v>HKD_YC6MRH_3x9F#0000</v>
       </c>
       <c r="J7" s="31" t="str">
         <f>_xll.ohRangeRetrieveError(I7)</f>
@@ -2690,7 +2721,7 @@
       </c>
       <c r="I8" s="32" t="str">
         <f>_xll.qlFraRateHelper(H8,G8,B8,E8,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC6MRH_4x10F#0002</v>
+        <v>HKD_YC6MRH_4x10F#0000</v>
       </c>
       <c r="J8" s="31" t="str">
         <f>_xll.ohRangeRetrieveError(I8)</f>
@@ -2728,7 +2759,7 @@
       </c>
       <c r="I9" s="32" t="str">
         <f>_xll.qlFraRateHelper(H9,G9,B9,E9,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC6MRH_5x11F#0002</v>
+        <v>HKD_YC6MRH_5x11F#0000</v>
       </c>
       <c r="J9" s="31" t="str">
         <f>_xll.ohRangeRetrieveError(I9)</f>
@@ -2766,7 +2797,7 @@
       </c>
       <c r="I10" s="32" t="str">
         <f>_xll.qlFraRateHelper(H10,G10,B10,E10,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC6MRH_6x12F#0002</v>
+        <v>HKD_YC6MRH_6x12F#0000</v>
       </c>
       <c r="J10" s="31" t="str">
         <f>_xll.ohRangeRetrieveError(I10)</f>
@@ -2804,7 +2835,7 @@
       </c>
       <c r="I11" s="32" t="str">
         <f>_xll.qlFraRateHelper(H11,G11,B11,E11,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC6MRH_7x13F#0002</v>
+        <v>HKD_YC6MRH_7x13F#0000</v>
       </c>
       <c r="J11" s="31" t="str">
         <f>_xll.ohRangeRetrieveError(I11)</f>
@@ -2842,7 +2873,7 @@
       </c>
       <c r="I12" s="32" t="str">
         <f>_xll.qlFraRateHelper(H12,G12,B12,E12,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC6MRH_8x14F#0002</v>
+        <v>HKD_YC6MRH_8x14F#0000</v>
       </c>
       <c r="J12" s="31" t="str">
         <f>_xll.ohRangeRetrieveError(I12)</f>
@@ -2880,7 +2911,7 @@
       </c>
       <c r="I13" s="32" t="str">
         <f>_xll.qlFraRateHelper(H13,G13,B13,E13,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC6MRH_9x15F#0002</v>
+        <v>HKD_YC6MRH_9x15F#0000</v>
       </c>
       <c r="J13" s="31" t="str">
         <f>_xll.ohRangeRetrieveError(I13)</f>
@@ -2918,7 +2949,7 @@
       </c>
       <c r="I14" s="32" t="str">
         <f>_xll.qlFraRateHelper(H14,G14,B14,E14,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC6MRH_10x16F#0002</v>
+        <v>HKD_YC6MRH_10x16F#0000</v>
       </c>
       <c r="J14" s="31" t="str">
         <f>_xll.ohRangeRetrieveError(I14)</f>
@@ -2956,7 +2987,7 @@
       </c>
       <c r="I15" s="32" t="str">
         <f>_xll.qlFraRateHelper(H15,G15,B15,E15,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC6MRH_11x17F#0002</v>
+        <v>HKD_YC6MRH_11x17F#0000</v>
       </c>
       <c r="J15" s="31" t="str">
         <f>_xll.ohRangeRetrieveError(I15)</f>
@@ -2994,7 +3025,7 @@
       </c>
       <c r="I16" s="32" t="str">
         <f>_xll.qlFraRateHelper(H16,G16,B16,E16,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC6MRH_12x18F#0002</v>
+        <v>HKD_YC6MRH_12x18F#0000</v>
       </c>
       <c r="J16" s="31" t="str">
         <f>_xll.ohRangeRetrieveError(I16)</f>
@@ -3032,7 +3063,7 @@
       </c>
       <c r="I17" s="32" t="str">
         <f>_xll.qlFraRateHelper(H17,G17,B17,E17,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC6MRH_13x19F#0002</v>
+        <v>HKD_YC6MRH_13x19F#0000</v>
       </c>
       <c r="J17" s="31" t="str">
         <f>_xll.ohRangeRetrieveError(I17)</f>
@@ -3070,7 +3101,7 @@
       </c>
       <c r="I18" s="32" t="str">
         <f>_xll.qlFraRateHelper(H18,G18,B18,E18,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC6MRH_14x20F#0002</v>
+        <v>HKD_YC6MRH_14x20F#0000</v>
       </c>
       <c r="J18" s="31" t="str">
         <f>_xll.ohRangeRetrieveError(I18)</f>
@@ -3108,7 +3139,7 @@
       </c>
       <c r="I19" s="32" t="str">
         <f>_xll.qlFraRateHelper(H19,G19,B19,E19,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC6MRH_15x21F#0002</v>
+        <v>HKD_YC6MRH_15x21F#0000</v>
       </c>
       <c r="J19" s="31" t="str">
         <f>_xll.ohRangeRetrieveError(I19)</f>
@@ -3146,7 +3177,7 @@
       </c>
       <c r="I20" s="32" t="str">
         <f>_xll.qlFraRateHelper(H20,G20,B20,E20,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC6MRH_16x22F#0002</v>
+        <v>HKD_YC6MRH_16x22F#0000</v>
       </c>
       <c r="J20" s="31" t="str">
         <f>_xll.ohRangeRetrieveError(I20)</f>
@@ -3184,7 +3215,7 @@
       </c>
       <c r="I21" s="32" t="str">
         <f>_xll.qlFraRateHelper(H21,G21,B21,E21,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC6MRH_17x23F#0002</v>
+        <v>HKD_YC6MRH_17x23F#0000</v>
       </c>
       <c r="J21" s="31" t="str">
         <f>_xll.ohRangeRetrieveError(I21)</f>
@@ -3222,7 +3253,7 @@
       </c>
       <c r="I22" s="32" t="str">
         <f>_xll.qlFraRateHelper(H22,G22,B22,E22,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC6MRH_18x24F#0002</v>
+        <v>HKD_YC6MRH_18x24F#0000</v>
       </c>
       <c r="J22" s="31" t="str">
         <f>_xll.ohRangeRetrieveError(I22)</f>
@@ -3239,15 +3270,15 @@
         <v>101</v>
       </c>
       <c r="F23" s="28"/>
-      <c r="G23" s="138" t="s">
+      <c r="G23" s="136" t="s">
         <v>102</v>
       </c>
-      <c r="H23" s="138" t="s">
+      <c r="H23" s="136" t="s">
         <v>103</v>
       </c>
-      <c r="I23" s="139" t="str">
+      <c r="I23" s="137" t="str">
         <f>_xll.qlDepositRateHelper(H23,G23,E23,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HkdHibor6MLastFixing#0001</v>
+        <v>HkdHibor6MLastFixing#0000</v>
       </c>
       <c r="J23" s="27"/>
       <c r="K23" s="26"/>
@@ -3268,34 +3299,34 @@
   <dimension ref="B1:L59"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.7109375" style="102" customWidth="1"/>
-    <col min="2" max="2" width="5" style="103" customWidth="1"/>
-    <col min="3" max="3" width="8.5703125" style="103" customWidth="1"/>
-    <col min="4" max="4" width="4.42578125" style="103" customWidth="1"/>
-    <col min="5" max="5" width="23.28515625" style="103" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="7.140625" style="103" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="6.7109375" style="103" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.7109375" style="103" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.28515625" style="103" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.140625" style="103" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="2.7109375" style="102" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.5703125" style="102" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="28.140625" style="102" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="3.5703125" style="102" customWidth="1"/>
-    <col min="17" max="16384" width="9.140625" style="102"/>
+    <col min="1" max="1" width="5.7109375" style="100" customWidth="1"/>
+    <col min="2" max="2" width="5" style="101" customWidth="1"/>
+    <col min="3" max="3" width="8.5703125" style="101" customWidth="1"/>
+    <col min="4" max="4" width="4.42578125" style="101" customWidth="1"/>
+    <col min="5" max="5" width="23.28515625" style="101" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="7.140625" style="101" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="6.7109375" style="101" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.7109375" style="101" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.28515625" style="101" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.140625" style="101" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="2.7109375" style="100" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.5703125" style="100" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="28.140625" style="100" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="3.5703125" style="100" customWidth="1"/>
+    <col min="17" max="16384" width="9.140625" style="100"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:12" ht="33.75" x14ac:dyDescent="0.2">
-      <c r="B1" s="140" t="s">
+      <c r="B1" s="151" t="s">
         <v>100</v>
       </c>
-      <c r="C1" s="141"/>
-      <c r="D1" s="142"/>
+      <c r="C1" s="152"/>
+      <c r="D1" s="153"/>
       <c r="E1" s="1" t="s">
         <v>19</v>
       </c>
@@ -3322,2406 +3353,2406 @@
       </c>
     </row>
     <row r="2" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B2" s="125"/>
-      <c r="C2" s="116"/>
-      <c r="D2" s="115" t="s">
+      <c r="B2" s="123"/>
+      <c r="C2" s="114"/>
+      <c r="D2" s="113" t="s">
         <v>99</v>
       </c>
-      <c r="E2" s="115" t="str">
+      <c r="E2" s="113" t="str">
         <f>FRAs!I23</f>
-        <v>HkdHibor6MLastFixing#0001</v>
-      </c>
-      <c r="F2" s="114">
+        <v>HkdHibor6MLastFixing#0000</v>
+      </c>
+      <c r="F2" s="112">
         <f>_xll.qlRateHelperQuoteValue($E2,Trigger)</f>
         <v>5.4856999999999996E-3</v>
       </c>
-      <c r="G2" s="114"/>
-      <c r="H2" s="113" t="b">
+      <c r="G2" s="112"/>
+      <c r="H2" s="111" t="b">
         <f>IF(ISERROR(F2),FALSE,TRUE)</f>
         <v>1</v>
       </c>
-      <c r="I2" s="113">
+      <c r="I2" s="111">
         <v>70</v>
       </c>
-      <c r="J2" s="113">
+      <c r="J2" s="111">
         <v>1</v>
       </c>
-      <c r="K2" s="112">
+      <c r="K2" s="110">
         <f>_xll.qlRateHelperEarliestDate($E2,Trigger)</f>
-        <v>41684</v>
-      </c>
-      <c r="L2" s="111">
+        <v>41736</v>
+      </c>
+      <c r="L2" s="109">
         <f>_xll.qlRateHelperLatestDate($E2,Trigger)</f>
-        <v>41865</v>
+        <v>41919</v>
       </c>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B3" s="124" t="s">
+      <c r="B3" s="122" t="s">
         <v>98</v>
       </c>
-      <c r="C3" s="123">
+      <c r="C3" s="121">
         <f>Months</f>
         <v>6</v>
       </c>
-      <c r="D3" s="122" t="s">
+      <c r="D3" s="120" t="s">
         <v>38</v>
       </c>
-      <c r="E3" s="122" t="str">
+      <c r="E3" s="120" t="str">
         <f t="shared" ref="E3:E4" si="0">RateHelperPrefix&amp;"_"&amp;$B3&amp;$C3&amp;$D3</f>
         <v>HKD_YC6MRH_T6F1</v>
       </c>
-      <c r="F3" s="121" t="e">
+      <c r="F3" s="119" t="e">
         <f>_xll.qlRateHelperQuoteValue($E3,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="G3" s="121"/>
-      <c r="H3" s="120" t="b">
+      <c r="G3" s="119"/>
+      <c r="H3" s="118" t="b">
         <f t="shared" ref="H3:H22" si="1">IF(ISERROR(F3),FALSE,TRUE)</f>
         <v>0</v>
       </c>
-      <c r="I3" s="120">
+      <c r="I3" s="118">
         <v>20</v>
       </c>
-      <c r="J3" s="120">
+      <c r="J3" s="118">
         <v>1</v>
       </c>
-      <c r="K3" s="119">
+      <c r="K3" s="117">
         <f>_xll.qlRateHelperEarliestDate($E3,Trigger)</f>
-        <v>41684</v>
-      </c>
-      <c r="L3" s="118">
+        <v>41736</v>
+      </c>
+      <c r="L3" s="116">
         <f>_xll.qlRateHelperLatestDate($E3,Trigger)</f>
-        <v>41865</v>
+        <v>41919</v>
       </c>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B4" s="110" t="s">
+      <c r="B4" s="108" t="s">
         <v>97</v>
       </c>
-      <c r="C4" s="109">
+      <c r="C4" s="107">
         <f>Months</f>
         <v>6</v>
       </c>
-      <c r="D4" s="108" t="s">
+      <c r="D4" s="106" t="s">
         <v>38</v>
       </c>
-      <c r="E4" s="108" t="str">
+      <c r="E4" s="106" t="str">
         <f t="shared" si="0"/>
         <v>HKD_YC6MRH_TOM6F1</v>
       </c>
-      <c r="F4" s="107" t="e">
+      <c r="F4" s="105" t="e">
         <f>_xll.qlRateHelperQuoteValue($E4,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="G4" s="107"/>
-      <c r="H4" s="106" t="b">
+      <c r="G4" s="105"/>
+      <c r="H4" s="104" t="b">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I4" s="106">
+      <c r="I4" s="104">
         <v>20</v>
       </c>
-      <c r="J4" s="106">
+      <c r="J4" s="104">
         <v>1</v>
       </c>
-      <c r="K4" s="105">
+      <c r="K4" s="103">
         <f>_xll.qlRateHelperEarliestDate($E4,Trigger)</f>
-        <v>41687</v>
-      </c>
-      <c r="L4" s="104">
+        <v>41737</v>
+      </c>
+      <c r="L4" s="102">
         <f>_xll.qlRateHelperLatestDate($E4,Trigger)</f>
-        <v>41869</v>
+        <v>41920</v>
       </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B5" s="117">
+      <c r="B5" s="115">
         <v>1</v>
       </c>
-      <c r="C5" s="116" t="s">
+      <c r="C5" s="114" t="s">
         <v>96</v>
       </c>
-      <c r="D5" s="115" t="str">
+      <c r="D5" s="113" t="str">
         <f t="shared" ref="D5:D22" si="2">(B5+Months)&amp;"F"</f>
         <v>7F</v>
       </c>
-      <c r="E5" s="115" t="str">
+      <c r="E5" s="113" t="str">
         <f>FRAs!I5</f>
-        <v>HKD_YC6MRH_1x7F#0002</v>
-      </c>
-      <c r="F5" s="114">
+        <v>HKD_YC6MRH_1x7F#0000</v>
+      </c>
+      <c r="F5" s="112">
         <f>_xll.qlRateHelperQuoteValue($E5,Trigger)</f>
-        <v>4.8999999999999998E-3</v>
-      </c>
-      <c r="G5" s="114"/>
-      <c r="H5" s="113" t="b">
+        <v>4.7999999999999996E-3</v>
+      </c>
+      <c r="G5" s="112"/>
+      <c r="H5" s="111" t="b">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="I5" s="113">
+      <c r="I5" s="111">
         <v>20</v>
       </c>
-      <c r="J5" s="113">
+      <c r="J5" s="111">
         <v>1</v>
       </c>
-      <c r="K5" s="112">
+      <c r="K5" s="110">
         <f>_xll.qlRateHelperEarliestDate($E5,Trigger)</f>
-        <v>41712</v>
-      </c>
-      <c r="L5" s="111">
+        <v>41766</v>
+      </c>
+      <c r="L5" s="109">
         <f>_xll.qlRateHelperLatestDate($E5,Trigger)</f>
-        <v>41897</v>
+        <v>41950</v>
       </c>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B6" s="117">
+      <c r="B6" s="115">
         <v>2</v>
       </c>
-      <c r="C6" s="116" t="s">
+      <c r="C6" s="114" t="s">
         <v>96</v>
       </c>
-      <c r="D6" s="115" t="str">
+      <c r="D6" s="113" t="str">
         <f t="shared" si="2"/>
         <v>8F</v>
       </c>
-      <c r="E6" s="115" t="str">
+      <c r="E6" s="113" t="str">
         <f>FRAs!I6</f>
-        <v>HKD_YC6MRH_2x8F#0002</v>
-      </c>
-      <c r="F6" s="114">
+        <v>HKD_YC6MRH_2x8F#0000</v>
+      </c>
+      <c r="F6" s="112">
         <f>_xll.qlRateHelperQuoteValue($E6,Trigger)</f>
-        <v>4.8999999999999998E-3</v>
-      </c>
-      <c r="G6" s="114"/>
-      <c r="H6" s="113" t="b">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="G6" s="112"/>
+      <c r="H6" s="111" t="b">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="I6" s="113">
+      <c r="I6" s="111">
         <v>20</v>
       </c>
-      <c r="J6" s="113">
+      <c r="J6" s="111">
         <v>1</v>
       </c>
-      <c r="K6" s="112">
+      <c r="K6" s="110">
         <f>_xll.qlRateHelperEarliestDate($E6,Trigger)</f>
-        <v>41743</v>
-      </c>
-      <c r="L6" s="111">
+        <v>41799</v>
+      </c>
+      <c r="L6" s="109">
         <f>_xll.qlRateHelperLatestDate($E6,Trigger)</f>
-        <v>41926</v>
+        <v>41982</v>
       </c>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B7" s="117">
+      <c r="B7" s="115">
         <v>3</v>
       </c>
-      <c r="C7" s="116" t="s">
+      <c r="C7" s="114" t="s">
         <v>96</v>
       </c>
-      <c r="D7" s="115" t="str">
+      <c r="D7" s="113" t="str">
         <f t="shared" si="2"/>
         <v>9F</v>
       </c>
-      <c r="E7" s="115" t="str">
+      <c r="E7" s="113" t="str">
         <f>FRAs!I7</f>
-        <v>HKD_YC6MRH_3x9F#0002</v>
-      </c>
-      <c r="F7" s="114">
+        <v>HKD_YC6MRH_3x9F#0000</v>
+      </c>
+      <c r="F7" s="112">
         <f>_xll.qlRateHelperQuoteValue($E7,Trigger)</f>
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="G7" s="114"/>
-      <c r="H7" s="113" t="b">
+        <v>5.1000000000000004E-3</v>
+      </c>
+      <c r="G7" s="112"/>
+      <c r="H7" s="111" t="b">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="I7" s="113">
+      <c r="I7" s="111">
         <v>20</v>
       </c>
-      <c r="J7" s="113">
+      <c r="J7" s="111">
         <v>1</v>
       </c>
-      <c r="K7" s="112">
+      <c r="K7" s="110">
         <f>_xll.qlRateHelperEarliestDate($E7,Trigger)</f>
-        <v>41773</v>
-      </c>
-      <c r="L7" s="111">
+        <v>41827</v>
+      </c>
+      <c r="L7" s="109">
         <f>_xll.qlRateHelperLatestDate($E7,Trigger)</f>
-        <v>41957</v>
+        <v>42011</v>
       </c>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B8" s="117">
+      <c r="B8" s="115">
         <v>4</v>
       </c>
-      <c r="C8" s="116" t="s">
+      <c r="C8" s="114" t="s">
         <v>96</v>
       </c>
-      <c r="D8" s="115" t="str">
+      <c r="D8" s="113" t="str">
         <f t="shared" si="2"/>
         <v>10F</v>
       </c>
-      <c r="E8" s="115" t="str">
+      <c r="E8" s="113" t="str">
         <f>FRAs!I8</f>
-        <v>HKD_YC6MRH_4x10F#0002</v>
-      </c>
-      <c r="F8" s="114">
+        <v>HKD_YC6MRH_4x10F#0000</v>
+      </c>
+      <c r="F8" s="112">
         <f>_xll.qlRateHelperQuoteValue($E8,Trigger)</f>
-        <v>5.1000000000000004E-3</v>
-      </c>
-      <c r="G8" s="114"/>
-      <c r="H8" s="113" t="b">
+        <v>5.3E-3</v>
+      </c>
+      <c r="G8" s="112"/>
+      <c r="H8" s="111" t="b">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="I8" s="113">
+      <c r="I8" s="111">
         <v>20</v>
       </c>
-      <c r="J8" s="113">
+      <c r="J8" s="111">
         <v>1</v>
       </c>
-      <c r="K8" s="112">
+      <c r="K8" s="110">
         <f>_xll.qlRateHelperEarliestDate($E8,Trigger)</f>
-        <v>41806</v>
-      </c>
-      <c r="L8" s="111">
+        <v>41858</v>
+      </c>
+      <c r="L8" s="109">
         <f>_xll.qlRateHelperLatestDate($E8,Trigger)</f>
-        <v>41989</v>
+        <v>42044</v>
       </c>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B9" s="117">
+      <c r="B9" s="115">
         <v>5</v>
       </c>
-      <c r="C9" s="116" t="s">
+      <c r="C9" s="114" t="s">
         <v>96</v>
       </c>
-      <c r="D9" s="115" t="str">
+      <c r="D9" s="113" t="str">
         <f t="shared" si="2"/>
         <v>11F</v>
       </c>
-      <c r="E9" s="115" t="str">
+      <c r="E9" s="113" t="str">
         <f>FRAs!I9</f>
-        <v>HKD_YC6MRH_5x11F#0002</v>
-      </c>
-      <c r="F9" s="114">
+        <v>HKD_YC6MRH_5x11F#0000</v>
+      </c>
+      <c r="F9" s="112">
         <f>_xll.qlRateHelperQuoteValue($E9,Trigger)</f>
-        <v>5.1999999999999998E-3</v>
-      </c>
-      <c r="G9" s="114"/>
-      <c r="H9" s="113" t="b">
+        <v>5.5000000000000005E-3</v>
+      </c>
+      <c r="G9" s="112"/>
+      <c r="H9" s="111" t="b">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="I9" s="113">
+      <c r="I9" s="111">
         <v>20</v>
       </c>
-      <c r="J9" s="113">
+      <c r="J9" s="111">
         <v>1</v>
       </c>
-      <c r="K9" s="112">
+      <c r="K9" s="110">
         <f>_xll.qlRateHelperEarliestDate($E9,Trigger)</f>
-        <v>41834</v>
-      </c>
-      <c r="L9" s="111">
+        <v>41890</v>
+      </c>
+      <c r="L9" s="109">
         <f>_xll.qlRateHelperLatestDate($E9,Trigger)</f>
-        <v>42018</v>
+        <v>42072</v>
       </c>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B10" s="117">
+      <c r="B10" s="115">
         <v>6</v>
       </c>
-      <c r="C10" s="116" t="s">
+      <c r="C10" s="114" t="s">
         <v>96</v>
       </c>
-      <c r="D10" s="115" t="str">
+      <c r="D10" s="113" t="str">
         <f t="shared" si="2"/>
         <v>12F</v>
       </c>
-      <c r="E10" s="115" t="str">
+      <c r="E10" s="113" t="str">
         <f>FRAs!I10</f>
-        <v>HKD_YC6MRH_6x12F#0002</v>
-      </c>
-      <c r="F10" s="114">
+        <v>HKD_YC6MRH_6x12F#0000</v>
+      </c>
+      <c r="F10" s="112">
         <f>_xll.qlRateHelperQuoteValue($E10,Trigger)</f>
-        <v>5.4000000000000003E-3</v>
-      </c>
-      <c r="G10" s="114"/>
-      <c r="H10" s="113" t="b">
+        <v>5.8000000000000005E-3</v>
+      </c>
+      <c r="G10" s="112"/>
+      <c r="H10" s="111" t="b">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="I10" s="113">
+      <c r="I10" s="111">
         <v>20</v>
       </c>
-      <c r="J10" s="113">
+      <c r="J10" s="111">
         <v>1</v>
       </c>
-      <c r="K10" s="112">
+      <c r="K10" s="110">
         <f>_xll.qlRateHelperEarliestDate($E10,Trigger)</f>
-        <v>41865</v>
-      </c>
-      <c r="L10" s="111">
+        <v>41919</v>
+      </c>
+      <c r="L10" s="109">
         <f>_xll.qlRateHelperLatestDate($E10,Trigger)</f>
-        <v>42051</v>
+        <v>42101</v>
       </c>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B11" s="117">
+      <c r="B11" s="115">
         <v>7</v>
       </c>
-      <c r="C11" s="116" t="s">
+      <c r="C11" s="114" t="s">
         <v>96</v>
       </c>
-      <c r="D11" s="115" t="str">
+      <c r="D11" s="113" t="str">
         <f t="shared" si="2"/>
         <v>13F</v>
       </c>
-      <c r="E11" s="115" t="str">
+      <c r="E11" s="113" t="str">
         <f>FRAs!I11</f>
-        <v>HKD_YC6MRH_7x13F#0002</v>
-      </c>
-      <c r="F11" s="114" t="e">
+        <v>HKD_YC6MRH_7x13F#0000</v>
+      </c>
+      <c r="F11" s="112" t="e">
         <f>_xll.qlRateHelperQuoteValue($E11,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="G11" s="114"/>
-      <c r="H11" s="113" t="b">
+      <c r="G11" s="112"/>
+      <c r="H11" s="111" t="b">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I11" s="113">
+      <c r="I11" s="111">
         <v>20</v>
       </c>
-      <c r="J11" s="113">
+      <c r="J11" s="111">
         <v>1</v>
       </c>
-      <c r="K11" s="112">
+      <c r="K11" s="110">
         <f>_xll.qlRateHelperEarliestDate($E11,Trigger)</f>
-        <v>41897</v>
-      </c>
-      <c r="L11" s="111">
+        <v>41950</v>
+      </c>
+      <c r="L11" s="109">
         <f>_xll.qlRateHelperLatestDate($E11,Trigger)</f>
-        <v>42079</v>
+        <v>42131</v>
       </c>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B12" s="117">
+      <c r="B12" s="115">
         <v>8</v>
       </c>
-      <c r="C12" s="116" t="s">
+      <c r="C12" s="114" t="s">
         <v>96</v>
       </c>
-      <c r="D12" s="115" t="str">
+      <c r="D12" s="113" t="str">
         <f t="shared" si="2"/>
         <v>14F</v>
       </c>
-      <c r="E12" s="115" t="str">
+      <c r="E12" s="113" t="str">
         <f>FRAs!I12</f>
-        <v>HKD_YC6MRH_8x14F#0002</v>
-      </c>
-      <c r="F12" s="114" t="e">
+        <v>HKD_YC6MRH_8x14F#0000</v>
+      </c>
+      <c r="F12" s="112" t="e">
         <f>_xll.qlRateHelperQuoteValue($E12,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="G12" s="114"/>
-      <c r="H12" s="113" t="b">
+      <c r="G12" s="112"/>
+      <c r="H12" s="111" t="b">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I12" s="113">
+      <c r="I12" s="111">
         <v>20</v>
       </c>
-      <c r="J12" s="113">
+      <c r="J12" s="111">
         <v>1</v>
       </c>
-      <c r="K12" s="112">
+      <c r="K12" s="110">
         <f>_xll.qlRateHelperEarliestDate($E12,Trigger)</f>
-        <v>41926</v>
-      </c>
-      <c r="L12" s="111">
+        <v>41981</v>
+      </c>
+      <c r="L12" s="109">
         <f>_xll.qlRateHelperLatestDate($E12,Trigger)</f>
-        <v>42108</v>
+        <v>42163</v>
       </c>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B13" s="117">
+      <c r="B13" s="115">
         <v>9</v>
       </c>
-      <c r="C13" s="116" t="s">
+      <c r="C13" s="114" t="s">
         <v>96</v>
       </c>
-      <c r="D13" s="115" t="str">
+      <c r="D13" s="113" t="str">
         <f t="shared" si="2"/>
         <v>15F</v>
       </c>
-      <c r="E13" s="115" t="str">
+      <c r="E13" s="113" t="str">
         <f>FRAs!I13</f>
-        <v>HKD_YC6MRH_9x15F#0002</v>
-      </c>
-      <c r="F13" s="114" t="e">
+        <v>HKD_YC6MRH_9x15F#0000</v>
+      </c>
+      <c r="F13" s="112" t="e">
         <f>_xll.qlRateHelperQuoteValue($E13,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="G13" s="114"/>
-      <c r="H13" s="113" t="b">
+      <c r="G13" s="112"/>
+      <c r="H13" s="111" t="b">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I13" s="113">
+      <c r="I13" s="111">
         <v>20</v>
       </c>
-      <c r="J13" s="113">
+      <c r="J13" s="111">
         <v>1</v>
       </c>
-      <c r="K13" s="112">
+      <c r="K13" s="110">
         <f>_xll.qlRateHelperEarliestDate($E13,Trigger)</f>
-        <v>41957</v>
-      </c>
-      <c r="L13" s="111">
+        <v>42011</v>
+      </c>
+      <c r="L13" s="109">
         <f>_xll.qlRateHelperLatestDate($E13,Trigger)</f>
-        <v>42138</v>
+        <v>42192</v>
       </c>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B14" s="117">
+      <c r="B14" s="115">
         <v>10</v>
       </c>
-      <c r="C14" s="116" t="s">
+      <c r="C14" s="114" t="s">
         <v>96</v>
       </c>
-      <c r="D14" s="115" t="str">
+      <c r="D14" s="113" t="str">
         <f t="shared" si="2"/>
         <v>16F</v>
       </c>
-      <c r="E14" s="115" t="str">
+      <c r="E14" s="113" t="str">
         <f>FRAs!I14</f>
-        <v>HKD_YC6MRH_10x16F#0002</v>
-      </c>
-      <c r="F14" s="114" t="e">
+        <v>HKD_YC6MRH_10x16F#0000</v>
+      </c>
+      <c r="F14" s="112" t="e">
         <f>_xll.qlRateHelperQuoteValue($E14,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="G14" s="114"/>
-      <c r="H14" s="113" t="b">
+      <c r="G14" s="112"/>
+      <c r="H14" s="111" t="b">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I14" s="113">
+      <c r="I14" s="111">
         <v>20</v>
       </c>
-      <c r="J14" s="113">
+      <c r="J14" s="111">
         <v>1</v>
       </c>
-      <c r="K14" s="112">
+      <c r="K14" s="110">
         <f>_xll.qlRateHelperEarliestDate($E14,Trigger)</f>
-        <v>41988</v>
-      </c>
-      <c r="L14" s="111">
+        <v>42044</v>
+      </c>
+      <c r="L14" s="109">
         <f>_xll.qlRateHelperLatestDate($E14,Trigger)</f>
-        <v>42170</v>
+        <v>42226</v>
       </c>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B15" s="117">
+      <c r="B15" s="115">
         <v>11</v>
       </c>
-      <c r="C15" s="116" t="s">
+      <c r="C15" s="114" t="s">
         <v>96</v>
       </c>
-      <c r="D15" s="115" t="str">
+      <c r="D15" s="113" t="str">
         <f t="shared" si="2"/>
         <v>17F</v>
       </c>
-      <c r="E15" s="115" t="str">
+      <c r="E15" s="113" t="str">
         <f>FRAs!I15</f>
-        <v>HKD_YC6MRH_11x17F#0002</v>
-      </c>
-      <c r="F15" s="114" t="e">
+        <v>HKD_YC6MRH_11x17F#0000</v>
+      </c>
+      <c r="F15" s="112" t="e">
         <f>_xll.qlRateHelperQuoteValue($E15,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="G15" s="114"/>
-      <c r="H15" s="113" t="b">
+      <c r="G15" s="112"/>
+      <c r="H15" s="111" t="b">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I15" s="113">
+      <c r="I15" s="111">
         <v>20</v>
       </c>
-      <c r="J15" s="113">
+      <c r="J15" s="111">
         <v>1</v>
       </c>
-      <c r="K15" s="112">
+      <c r="K15" s="110">
         <f>_xll.qlRateHelperEarliestDate($E15,Trigger)</f>
-        <v>42018</v>
-      </c>
-      <c r="L15" s="111">
+        <v>42072</v>
+      </c>
+      <c r="L15" s="109">
         <f>_xll.qlRateHelperLatestDate($E15,Trigger)</f>
-        <v>42199</v>
+        <v>42256</v>
       </c>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B16" s="117">
+      <c r="B16" s="115">
         <v>12</v>
       </c>
-      <c r="C16" s="116" t="s">
+      <c r="C16" s="114" t="s">
         <v>96</v>
       </c>
-      <c r="D16" s="115" t="str">
+      <c r="D16" s="113" t="str">
         <f t="shared" si="2"/>
         <v>18F</v>
       </c>
-      <c r="E16" s="115" t="str">
+      <c r="E16" s="113" t="str">
         <f>FRAs!I16</f>
-        <v>HKD_YC6MRH_12x18F#0002</v>
-      </c>
-      <c r="F16" s="114">
+        <v>HKD_YC6MRH_12x18F#0000</v>
+      </c>
+      <c r="F16" s="112">
         <f>_xll.qlRateHelperQuoteValue($E16,Trigger)</f>
-        <v>6.1000000000000013E-3</v>
-      </c>
-      <c r="G16" s="114"/>
-      <c r="H16" s="113" t="b">
+        <v>8.8000000000000005E-3</v>
+      </c>
+      <c r="G16" s="112"/>
+      <c r="H16" s="111" t="b">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="I16" s="113">
+      <c r="I16" s="111">
         <v>20</v>
       </c>
-      <c r="J16" s="113">
+      <c r="J16" s="111">
         <v>1</v>
       </c>
-      <c r="K16" s="112">
+      <c r="K16" s="110">
         <f>_xll.qlRateHelperEarliestDate($E16,Trigger)</f>
-        <v>42051</v>
-      </c>
-      <c r="L16" s="111">
+        <v>42101</v>
+      </c>
+      <c r="L16" s="109">
         <f>_xll.qlRateHelperLatestDate($E16,Trigger)</f>
-        <v>42233</v>
+        <v>42284</v>
       </c>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B17" s="117">
+      <c r="B17" s="115">
         <v>13</v>
       </c>
-      <c r="C17" s="116" t="s">
+      <c r="C17" s="114" t="s">
         <v>96</v>
       </c>
-      <c r="D17" s="115" t="str">
+      <c r="D17" s="113" t="str">
         <f t="shared" si="2"/>
         <v>19F</v>
       </c>
-      <c r="E17" s="115" t="str">
+      <c r="E17" s="113" t="str">
         <f>FRAs!I17</f>
-        <v>HKD_YC6MRH_13x19F#0002</v>
-      </c>
-      <c r="F17" s="114" t="e">
+        <v>HKD_YC6MRH_13x19F#0000</v>
+      </c>
+      <c r="F17" s="112" t="e">
         <f>_xll.qlRateHelperQuoteValue($E17,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="G17" s="114"/>
-      <c r="H17" s="113" t="b">
+      <c r="G17" s="112"/>
+      <c r="H17" s="111" t="b">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I17" s="113">
+      <c r="I17" s="111">
         <v>20</v>
       </c>
-      <c r="J17" s="113">
+      <c r="J17" s="111">
         <v>1</v>
       </c>
-      <c r="K17" s="112">
+      <c r="K17" s="110">
         <f>_xll.qlRateHelperEarliestDate($E17,Trigger)</f>
-        <v>42079</v>
-      </c>
-      <c r="L17" s="111">
+        <v>42131</v>
+      </c>
+      <c r="L17" s="109">
         <f>_xll.qlRateHelperLatestDate($E17,Trigger)</f>
-        <v>42263</v>
+        <v>42317</v>
       </c>
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B18" s="117">
+      <c r="B18" s="115">
         <v>14</v>
       </c>
-      <c r="C18" s="116" t="s">
+      <c r="C18" s="114" t="s">
         <v>96</v>
       </c>
-      <c r="D18" s="115" t="str">
+      <c r="D18" s="113" t="str">
         <f t="shared" si="2"/>
         <v>20F</v>
       </c>
-      <c r="E18" s="115" t="str">
+      <c r="E18" s="113" t="str">
         <f>FRAs!I18</f>
-        <v>HKD_YC6MRH_14x20F#0002</v>
-      </c>
-      <c r="F18" s="114" t="e">
+        <v>HKD_YC6MRH_14x20F#0000</v>
+      </c>
+      <c r="F18" s="112" t="e">
         <f>_xll.qlRateHelperQuoteValue($E18,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="G18" s="114"/>
-      <c r="H18" s="113" t="b">
+      <c r="G18" s="112"/>
+      <c r="H18" s="111" t="b">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I18" s="113">
+      <c r="I18" s="111">
         <v>20</v>
       </c>
-      <c r="J18" s="113">
+      <c r="J18" s="111">
         <v>1</v>
       </c>
-      <c r="K18" s="112">
+      <c r="K18" s="110">
         <f>_xll.qlRateHelperEarliestDate($E18,Trigger)</f>
-        <v>42108</v>
-      </c>
-      <c r="L18" s="111">
+        <v>42163</v>
+      </c>
+      <c r="L18" s="109">
         <f>_xll.qlRateHelperLatestDate($E18,Trigger)</f>
-        <v>42291</v>
+        <v>42346</v>
       </c>
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B19" s="117">
+      <c r="B19" s="115">
         <v>15</v>
       </c>
-      <c r="C19" s="116" t="s">
+      <c r="C19" s="114" t="s">
         <v>96</v>
       </c>
-      <c r="D19" s="115" t="str">
+      <c r="D19" s="113" t="str">
         <f t="shared" si="2"/>
         <v>21F</v>
       </c>
-      <c r="E19" s="115" t="str">
+      <c r="E19" s="113" t="str">
         <f>FRAs!I19</f>
-        <v>HKD_YC6MRH_15x21F#0002</v>
-      </c>
-      <c r="F19" s="114" t="e">
+        <v>HKD_YC6MRH_15x21F#0000</v>
+      </c>
+      <c r="F19" s="112" t="e">
         <f>_xll.qlRateHelperQuoteValue($E19,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="G19" s="114"/>
-      <c r="H19" s="113" t="b">
+      <c r="G19" s="112"/>
+      <c r="H19" s="111" t="b">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I19" s="113">
+      <c r="I19" s="111">
         <v>20</v>
       </c>
-      <c r="J19" s="113">
+      <c r="J19" s="111">
         <v>1</v>
       </c>
-      <c r="K19" s="112">
+      <c r="K19" s="110">
         <f>_xll.qlRateHelperEarliestDate($E19,Trigger)</f>
-        <v>42138</v>
-      </c>
-      <c r="L19" s="111">
+        <v>42192</v>
+      </c>
+      <c r="L19" s="109">
         <f>_xll.qlRateHelperLatestDate($E19,Trigger)</f>
-        <v>42324</v>
+        <v>42376</v>
       </c>
     </row>
     <row r="20" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B20" s="117">
+      <c r="B20" s="115">
         <v>16</v>
       </c>
-      <c r="C20" s="116" t="s">
+      <c r="C20" s="114" t="s">
         <v>96</v>
       </c>
-      <c r="D20" s="115" t="str">
+      <c r="D20" s="113" t="str">
         <f t="shared" si="2"/>
         <v>22F</v>
       </c>
-      <c r="E20" s="115" t="str">
+      <c r="E20" s="113" t="str">
         <f>FRAs!I20</f>
-        <v>HKD_YC6MRH_16x22F#0002</v>
-      </c>
-      <c r="F20" s="114" t="e">
+        <v>HKD_YC6MRH_16x22F#0000</v>
+      </c>
+      <c r="F20" s="112" t="e">
         <f>_xll.qlRateHelperQuoteValue($E20,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="G20" s="114"/>
-      <c r="H20" s="113" t="b">
+      <c r="G20" s="112"/>
+      <c r="H20" s="111" t="b">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I20" s="113">
+      <c r="I20" s="111">
         <v>20</v>
       </c>
-      <c r="J20" s="113">
+      <c r="J20" s="111">
         <v>1</v>
       </c>
-      <c r="K20" s="112">
+      <c r="K20" s="110">
         <f>_xll.qlRateHelperEarliestDate($E20,Trigger)</f>
-        <v>42170</v>
-      </c>
-      <c r="L20" s="111">
+        <v>42223</v>
+      </c>
+      <c r="L20" s="109">
         <f>_xll.qlRateHelperLatestDate($E20,Trigger)</f>
-        <v>42353</v>
+        <v>42408</v>
       </c>
     </row>
     <row r="21" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B21" s="117">
+      <c r="B21" s="115">
         <v>17</v>
       </c>
-      <c r="C21" s="116" t="s">
+      <c r="C21" s="114" t="s">
         <v>96</v>
       </c>
-      <c r="D21" s="115" t="str">
+      <c r="D21" s="113" t="str">
         <f t="shared" si="2"/>
         <v>23F</v>
       </c>
-      <c r="E21" s="115" t="str">
+      <c r="E21" s="113" t="str">
         <f>FRAs!I21</f>
-        <v>HKD_YC6MRH_17x23F#0002</v>
-      </c>
-      <c r="F21" s="114" t="e">
+        <v>HKD_YC6MRH_17x23F#0000</v>
+      </c>
+      <c r="F21" s="112" t="e">
         <f>_xll.qlRateHelperQuoteValue($E21,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="G21" s="114"/>
-      <c r="H21" s="113" t="b">
+      <c r="G21" s="112"/>
+      <c r="H21" s="111" t="b">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I21" s="113">
+      <c r="I21" s="111">
         <v>20</v>
       </c>
-      <c r="J21" s="113">
+      <c r="J21" s="111">
         <v>1</v>
       </c>
-      <c r="K21" s="112">
+      <c r="K21" s="110">
         <f>_xll.qlRateHelperEarliestDate($E21,Trigger)</f>
-        <v>42199</v>
-      </c>
-      <c r="L21" s="111">
+        <v>42254</v>
+      </c>
+      <c r="L21" s="109">
         <f>_xll.qlRateHelperLatestDate($E21,Trigger)</f>
-        <v>42383</v>
+        <v>42436</v>
       </c>
     </row>
     <row r="22" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B22" s="110">
+      <c r="B22" s="108">
         <v>18</v>
       </c>
-      <c r="C22" s="109" t="s">
+      <c r="C22" s="107" t="s">
         <v>96</v>
       </c>
-      <c r="D22" s="108" t="str">
+      <c r="D22" s="106" t="str">
         <f t="shared" si="2"/>
         <v>24F</v>
       </c>
-      <c r="E22" s="108" t="str">
+      <c r="E22" s="106" t="str">
         <f>FRAs!I22</f>
-        <v>HKD_YC6MRH_18x24F#0002</v>
-      </c>
-      <c r="F22" s="107">
+        <v>HKD_YC6MRH_18x24F#0000</v>
+      </c>
+      <c r="F22" s="105">
         <f>_xll.qlRateHelperQuoteValue($E22,Trigger)</f>
-        <v>7.7000000000000002E-3</v>
-      </c>
-      <c r="G22" s="107"/>
-      <c r="H22" s="106" t="b">
+        <v>1.2500000000000001E-2</v>
+      </c>
+      <c r="G22" s="105"/>
+      <c r="H22" s="104" t="b">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="I22" s="106">
+      <c r="I22" s="104">
         <v>20</v>
       </c>
-      <c r="J22" s="106">
+      <c r="J22" s="104">
         <v>1</v>
       </c>
-      <c r="K22" s="105">
+      <c r="K22" s="103">
         <f>_xll.qlRateHelperEarliestDate($E22,Trigger)</f>
-        <v>42230</v>
-      </c>
-      <c r="L22" s="104">
+        <v>42284</v>
+      </c>
+      <c r="L22" s="102">
         <f>_xll.qlRateHelperLatestDate($E22,Trigger)</f>
-        <v>42415</v>
+        <v>42467</v>
       </c>
     </row>
     <row r="23" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B23" s="117" t="str">
+      <c r="B23" s="115" t="str">
         <f t="shared" ref="B23:B49" si="3">SwapFixedFreq</f>
         <v>QM</v>
       </c>
-      <c r="C23" s="116" t="str">
+      <c r="C23" s="114" t="str">
         <f t="shared" ref="C23:C59" si="4">IborType&amp;"BASIS"</f>
         <v>3HBASIS</v>
       </c>
-      <c r="D23" s="115" t="s">
+      <c r="D23" s="113" t="s">
         <v>95</v>
       </c>
-      <c r="E23" s="115" t="str">
+      <c r="E23" s="113" t="str">
         <f t="shared" ref="E23:E51" si="5">RateHelperPrefix&amp;"_"&amp;$B23&amp;$C23&amp;$D23</f>
         <v>HKD_YC6MRH_QM3HBASIS1Y</v>
       </c>
-      <c r="F23" s="114" t="e">
+      <c r="F23" s="112" t="e">
         <f>_xll.qlRateHelperQuoteValue($E23,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="G23" s="114" t="e">
+      <c r="G23" s="112" t="e">
         <f>_xll.qlSwapRateHelperSpread($E23,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="H23" s="113" t="b">
+      <c r="H23" s="111" t="b">
         <f t="shared" ref="H23:H33" si="6">IF(ISERROR(F23),FALSE,TRUE)</f>
         <v>0</v>
       </c>
-      <c r="I23" s="113">
+      <c r="I23" s="111">
         <v>40</v>
       </c>
-      <c r="J23" s="113">
+      <c r="J23" s="111">
         <v>1</v>
       </c>
-      <c r="K23" s="112" t="e">
+      <c r="K23" s="110" t="e">
         <f>_xll.qlRateHelperEarliestDate($E23,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="L23" s="111" t="e">
+      <c r="L23" s="109" t="e">
         <f>_xll.qlRateHelperLatestDate($E23,Trigger)</f>
         <v>#NUM!</v>
       </c>
     </row>
     <row r="24" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B24" s="117" t="str">
+      <c r="B24" s="115" t="str">
         <f t="shared" si="3"/>
         <v>QM</v>
       </c>
-      <c r="C24" s="116" t="str">
+      <c r="C24" s="114" t="str">
         <f t="shared" si="4"/>
         <v>3HBASIS</v>
       </c>
-      <c r="D24" s="115" t="s">
+      <c r="D24" s="113" t="s">
         <v>94</v>
       </c>
-      <c r="E24" s="115" t="str">
+      <c r="E24" s="113" t="str">
         <f t="shared" si="5"/>
         <v>HKD_YC6MRH_QM3HBASIS15M</v>
       </c>
-      <c r="F24" s="114" t="e">
+      <c r="F24" s="112" t="e">
         <f>_xll.qlRateHelperQuoteValue($E24,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="G24" s="114" t="e">
+      <c r="G24" s="112" t="e">
         <f>_xll.qlSwapRateHelperSpread($E24,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="H24" s="113" t="b">
+      <c r="H24" s="111" t="b">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="I24" s="113">
+      <c r="I24" s="111">
         <v>40</v>
       </c>
-      <c r="J24" s="113">
+      <c r="J24" s="111">
         <v>1</v>
       </c>
-      <c r="K24" s="112" t="e">
+      <c r="K24" s="110" t="e">
         <f>_xll.qlRateHelperEarliestDate($E24,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="L24" s="111" t="e">
+      <c r="L24" s="109" t="e">
         <f>_xll.qlRateHelperLatestDate($E24,Trigger)</f>
         <v>#NUM!</v>
       </c>
     </row>
     <row r="25" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B25" s="117" t="str">
+      <c r="B25" s="115" t="str">
         <f t="shared" si="3"/>
         <v>QM</v>
       </c>
-      <c r="C25" s="116" t="str">
+      <c r="C25" s="114" t="str">
         <f t="shared" si="4"/>
         <v>3HBASIS</v>
       </c>
-      <c r="D25" s="115" t="s">
+      <c r="D25" s="113" t="s">
         <v>93</v>
       </c>
-      <c r="E25" s="115" t="str">
+      <c r="E25" s="113" t="str">
         <f t="shared" si="5"/>
         <v>HKD_YC6MRH_QM3HBASIS18M</v>
       </c>
-      <c r="F25" s="114" t="e">
+      <c r="F25" s="112" t="e">
         <f>_xll.qlRateHelperQuoteValue($E25,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="G25" s="114" t="e">
+      <c r="G25" s="112" t="e">
         <f>_xll.qlSwapRateHelperSpread($E25,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="H25" s="113" t="b">
+      <c r="H25" s="111" t="b">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="I25" s="113">
+      <c r="I25" s="111">
         <v>40</v>
       </c>
-      <c r="J25" s="113">
+      <c r="J25" s="111">
         <v>1</v>
       </c>
-      <c r="K25" s="112" t="e">
+      <c r="K25" s="110" t="e">
         <f>_xll.qlRateHelperEarliestDate($E25,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="L25" s="111" t="e">
+      <c r="L25" s="109" t="e">
         <f>_xll.qlRateHelperLatestDate($E25,Trigger)</f>
         <v>#NUM!</v>
       </c>
     </row>
     <row r="26" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B26" s="117" t="str">
+      <c r="B26" s="115" t="str">
         <f t="shared" si="3"/>
         <v>QM</v>
       </c>
-      <c r="C26" s="116" t="str">
+      <c r="C26" s="114" t="str">
         <f t="shared" si="4"/>
         <v>3HBASIS</v>
       </c>
-      <c r="D26" s="115" t="s">
+      <c r="D26" s="113" t="s">
         <v>92</v>
       </c>
-      <c r="E26" s="115" t="str">
+      <c r="E26" s="113" t="str">
         <f t="shared" si="5"/>
         <v>HKD_YC6MRH_QM3HBASIS21M</v>
       </c>
-      <c r="F26" s="114" t="e">
+      <c r="F26" s="112" t="e">
         <f>_xll.qlRateHelperQuoteValue($E26,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="G26" s="114" t="e">
+      <c r="G26" s="112" t="e">
         <f>_xll.qlSwapRateHelperSpread($E26,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="H26" s="113" t="b">
+      <c r="H26" s="111" t="b">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="I26" s="113">
+      <c r="I26" s="111">
         <v>40</v>
       </c>
-      <c r="J26" s="113">
+      <c r="J26" s="111">
         <v>1</v>
       </c>
-      <c r="K26" s="112" t="e">
+      <c r="K26" s="110" t="e">
         <f>_xll.qlRateHelperEarliestDate($E26,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="L26" s="111" t="e">
+      <c r="L26" s="109" t="e">
         <f>_xll.qlRateHelperLatestDate($E26,Trigger)</f>
         <v>#NUM!</v>
       </c>
     </row>
     <row r="27" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B27" s="117" t="str">
+      <c r="B27" s="115" t="str">
         <f t="shared" si="3"/>
         <v>QM</v>
       </c>
-      <c r="C27" s="116" t="str">
+      <c r="C27" s="114" t="str">
         <f t="shared" si="4"/>
         <v>3HBASIS</v>
       </c>
-      <c r="D27" s="115" t="s">
+      <c r="D27" s="113" t="s">
         <v>91</v>
       </c>
-      <c r="E27" s="115" t="str">
+      <c r="E27" s="113" t="str">
         <f t="shared" si="5"/>
         <v>HKD_YC6MRH_QM3HBASIS2Y</v>
       </c>
-      <c r="F27" s="114" t="e">
+      <c r="F27" s="112" t="e">
         <f>_xll.qlRateHelperQuoteValue($E27,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="G27" s="114" t="e">
+      <c r="G27" s="112" t="e">
         <f>_xll.qlSwapRateHelperSpread($E27,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="H27" s="113" t="b">
+      <c r="H27" s="111" t="b">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="I27" s="113">
+      <c r="I27" s="111">
         <v>40</v>
       </c>
-      <c r="J27" s="113">
+      <c r="J27" s="111">
         <v>1</v>
       </c>
-      <c r="K27" s="112" t="e">
+      <c r="K27" s="110" t="e">
         <f>_xll.qlRateHelperEarliestDate($E27,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="L27" s="111" t="e">
+      <c r="L27" s="109" t="e">
         <f>_xll.qlRateHelperLatestDate($E27,Trigger)</f>
         <v>#NUM!</v>
       </c>
     </row>
     <row r="28" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B28" s="117" t="str">
+      <c r="B28" s="115" t="str">
         <f t="shared" si="3"/>
         <v>QM</v>
       </c>
-      <c r="C28" s="116" t="str">
+      <c r="C28" s="114" t="str">
         <f t="shared" si="4"/>
         <v>3HBASIS</v>
       </c>
-      <c r="D28" s="115" t="s">
+      <c r="D28" s="113" t="s">
         <v>90</v>
       </c>
-      <c r="E28" s="115" t="str">
+      <c r="E28" s="113" t="str">
         <f t="shared" si="5"/>
         <v>HKD_YC6MRH_QM3HBASIS3Y</v>
       </c>
-      <c r="F28" s="114" t="e">
+      <c r="F28" s="112" t="e">
         <f>_xll.qlRateHelperQuoteValue($E28,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="G28" s="114" t="e">
+      <c r="G28" s="112" t="e">
         <f>_xll.qlSwapRateHelperSpread($E28,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="H28" s="113" t="b">
+      <c r="H28" s="111" t="b">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="I28" s="113">
+      <c r="I28" s="111">
         <v>40</v>
       </c>
-      <c r="J28" s="113">
+      <c r="J28" s="111">
         <v>1</v>
       </c>
-      <c r="K28" s="112" t="e">
+      <c r="K28" s="110" t="e">
         <f>_xll.qlRateHelperEarliestDate($E28,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="L28" s="111" t="e">
+      <c r="L28" s="109" t="e">
         <f>_xll.qlRateHelperLatestDate($E28,Trigger)</f>
         <v>#NUM!</v>
       </c>
     </row>
     <row r="29" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B29" s="117" t="str">
+      <c r="B29" s="115" t="str">
         <f t="shared" si="3"/>
         <v>QM</v>
       </c>
-      <c r="C29" s="116" t="str">
+      <c r="C29" s="114" t="str">
         <f t="shared" si="4"/>
         <v>3HBASIS</v>
       </c>
-      <c r="D29" s="115" t="s">
+      <c r="D29" s="113" t="s">
         <v>89</v>
       </c>
-      <c r="E29" s="115" t="str">
+      <c r="E29" s="113" t="str">
         <f t="shared" si="5"/>
         <v>HKD_YC6MRH_QM3HBASIS4Y</v>
       </c>
-      <c r="F29" s="114" t="e">
+      <c r="F29" s="112" t="e">
         <f>_xll.qlRateHelperQuoteValue($E29,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="G29" s="114" t="e">
+      <c r="G29" s="112" t="e">
         <f>_xll.qlSwapRateHelperSpread($E29,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="H29" s="113" t="b">
+      <c r="H29" s="111" t="b">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="I29" s="113">
+      <c r="I29" s="111">
         <v>40</v>
       </c>
-      <c r="J29" s="113">
+      <c r="J29" s="111">
         <v>1</v>
       </c>
-      <c r="K29" s="112" t="e">
+      <c r="K29" s="110" t="e">
         <f>_xll.qlRateHelperEarliestDate($E29,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="L29" s="111" t="e">
+      <c r="L29" s="109" t="e">
         <f>_xll.qlRateHelperLatestDate($E29,Trigger)</f>
         <v>#NUM!</v>
       </c>
     </row>
     <row r="30" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B30" s="117" t="str">
+      <c r="B30" s="115" t="str">
         <f t="shared" si="3"/>
         <v>QM</v>
       </c>
-      <c r="C30" s="116" t="str">
+      <c r="C30" s="114" t="str">
         <f t="shared" si="4"/>
         <v>3HBASIS</v>
       </c>
-      <c r="D30" s="115" t="s">
+      <c r="D30" s="113" t="s">
         <v>88</v>
       </c>
-      <c r="E30" s="115" t="str">
+      <c r="E30" s="113" t="str">
         <f t="shared" si="5"/>
         <v>HKD_YC6MRH_QM3HBASIS5Y</v>
       </c>
-      <c r="F30" s="114" t="e">
+      <c r="F30" s="112" t="e">
         <f>_xll.qlRateHelperQuoteValue($E30,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="G30" s="114" t="e">
+      <c r="G30" s="112" t="e">
         <f>_xll.qlSwapRateHelperSpread($E30,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="H30" s="113" t="b">
+      <c r="H30" s="111" t="b">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="I30" s="113">
+      <c r="I30" s="111">
         <v>40</v>
       </c>
-      <c r="J30" s="113">
+      <c r="J30" s="111">
         <v>1</v>
       </c>
-      <c r="K30" s="112" t="e">
+      <c r="K30" s="110" t="e">
         <f>_xll.qlRateHelperEarliestDate($E30,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="L30" s="111" t="e">
+      <c r="L30" s="109" t="e">
         <f>_xll.qlRateHelperLatestDate($E30,Trigger)</f>
         <v>#NUM!</v>
       </c>
     </row>
     <row r="31" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B31" s="117" t="str">
+      <c r="B31" s="115" t="str">
         <f t="shared" si="3"/>
         <v>QM</v>
       </c>
-      <c r="C31" s="116" t="str">
+      <c r="C31" s="114" t="str">
         <f t="shared" si="4"/>
         <v>3HBASIS</v>
       </c>
-      <c r="D31" s="115" t="s">
+      <c r="D31" s="113" t="s">
         <v>87</v>
       </c>
-      <c r="E31" s="115" t="str">
+      <c r="E31" s="113" t="str">
         <f t="shared" si="5"/>
         <v>HKD_YC6MRH_QM3HBASIS6Y</v>
       </c>
-      <c r="F31" s="114" t="e">
+      <c r="F31" s="112" t="e">
         <f>_xll.qlRateHelperQuoteValue($E31,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="G31" s="114" t="e">
+      <c r="G31" s="112" t="e">
         <f>_xll.qlSwapRateHelperSpread($E31,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="H31" s="113" t="b">
+      <c r="H31" s="111" t="b">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="I31" s="113">
+      <c r="I31" s="111">
         <v>40</v>
       </c>
-      <c r="J31" s="113">
+      <c r="J31" s="111">
         <v>1</v>
       </c>
-      <c r="K31" s="112" t="e">
+      <c r="K31" s="110" t="e">
         <f>_xll.qlRateHelperEarliestDate($E31,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="L31" s="111" t="e">
+      <c r="L31" s="109" t="e">
         <f>_xll.qlRateHelperLatestDate($E31,Trigger)</f>
         <v>#NUM!</v>
       </c>
     </row>
     <row r="32" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B32" s="117" t="str">
+      <c r="B32" s="115" t="str">
         <f t="shared" si="3"/>
         <v>QM</v>
       </c>
-      <c r="C32" s="116" t="str">
+      <c r="C32" s="114" t="str">
         <f t="shared" si="4"/>
         <v>3HBASIS</v>
       </c>
-      <c r="D32" s="115" t="s">
+      <c r="D32" s="113" t="s">
         <v>86</v>
       </c>
-      <c r="E32" s="115" t="str">
+      <c r="E32" s="113" t="str">
         <f t="shared" si="5"/>
         <v>HKD_YC6MRH_QM3HBASIS7Y</v>
       </c>
-      <c r="F32" s="114" t="e">
+      <c r="F32" s="112" t="e">
         <f>_xll.qlRateHelperQuoteValue($E32,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="G32" s="114" t="e">
+      <c r="G32" s="112" t="e">
         <f>_xll.qlSwapRateHelperSpread($E32,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="H32" s="113" t="b">
+      <c r="H32" s="111" t="b">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="I32" s="113">
+      <c r="I32" s="111">
         <v>40</v>
       </c>
-      <c r="J32" s="113">
+      <c r="J32" s="111">
         <v>1</v>
       </c>
-      <c r="K32" s="112" t="e">
+      <c r="K32" s="110" t="e">
         <f>_xll.qlRateHelperEarliestDate($E32,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="L32" s="111" t="e">
+      <c r="L32" s="109" t="e">
         <f>_xll.qlRateHelperLatestDate($E32,Trigger)</f>
         <v>#NUM!</v>
       </c>
     </row>
     <row r="33" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B33" s="117" t="str">
+      <c r="B33" s="115" t="str">
         <f t="shared" si="3"/>
         <v>QM</v>
       </c>
-      <c r="C33" s="116" t="str">
+      <c r="C33" s="114" t="str">
         <f t="shared" si="4"/>
         <v>3HBASIS</v>
       </c>
-      <c r="D33" s="115" t="s">
+      <c r="D33" s="113" t="s">
         <v>85</v>
       </c>
-      <c r="E33" s="115" t="str">
+      <c r="E33" s="113" t="str">
         <f t="shared" si="5"/>
         <v>HKD_YC6MRH_QM3HBASIS8Y</v>
       </c>
-      <c r="F33" s="114" t="e">
+      <c r="F33" s="112" t="e">
         <f>_xll.qlRateHelperQuoteValue($E33,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="G33" s="114" t="e">
+      <c r="G33" s="112" t="e">
         <f>_xll.qlSwapRateHelperSpread($E33,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="H33" s="113" t="b">
+      <c r="H33" s="111" t="b">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="I33" s="113">
+      <c r="I33" s="111">
         <v>40</v>
       </c>
-      <c r="J33" s="113">
+      <c r="J33" s="111">
         <v>1</v>
       </c>
-      <c r="K33" s="112" t="e">
+      <c r="K33" s="110" t="e">
         <f>_xll.qlRateHelperEarliestDate($E33,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="L33" s="111" t="e">
+      <c r="L33" s="109" t="e">
         <f>_xll.qlRateHelperLatestDate($E33,Trigger)</f>
         <v>#NUM!</v>
       </c>
     </row>
     <row r="34" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B34" s="117" t="str">
+      <c r="B34" s="115" t="str">
         <f t="shared" si="3"/>
         <v>QM</v>
       </c>
-      <c r="C34" s="116" t="str">
+      <c r="C34" s="114" t="str">
         <f t="shared" si="4"/>
         <v>3HBASIS</v>
       </c>
-      <c r="D34" s="115" t="s">
+      <c r="D34" s="113" t="s">
         <v>84</v>
       </c>
-      <c r="E34" s="115" t="str">
+      <c r="E34" s="113" t="str">
         <f t="shared" si="5"/>
         <v>HKD_YC6MRH_QM3HBASIS9Y</v>
       </c>
-      <c r="F34" s="114" t="e">
+      <c r="F34" s="112" t="e">
         <f>_xll.qlRateHelperQuoteValue($E34,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="G34" s="114" t="e">
+      <c r="G34" s="112" t="e">
         <f>_xll.qlSwapRateHelperSpread($E34,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="H34" s="113" t="b">
+      <c r="H34" s="111" t="b">
         <f t="shared" ref="H34:H59" si="7">IF(ISERROR(F34),FALSE,TRUE)</f>
         <v>0</v>
       </c>
-      <c r="I34" s="113">
+      <c r="I34" s="111">
         <v>40</v>
       </c>
-      <c r="J34" s="113">
+      <c r="J34" s="111">
         <v>1</v>
       </c>
-      <c r="K34" s="112" t="e">
+      <c r="K34" s="110" t="e">
         <f>_xll.qlRateHelperEarliestDate($E34,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="L34" s="111" t="e">
+      <c r="L34" s="109" t="e">
         <f>_xll.qlRateHelperLatestDate($E34,Trigger)</f>
         <v>#NUM!</v>
       </c>
     </row>
     <row r="35" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B35" s="117" t="str">
+      <c r="B35" s="115" t="str">
         <f t="shared" si="3"/>
         <v>QM</v>
       </c>
-      <c r="C35" s="116" t="str">
+      <c r="C35" s="114" t="str">
         <f t="shared" si="4"/>
         <v>3HBASIS</v>
       </c>
-      <c r="D35" s="115" t="s">
+      <c r="D35" s="113" t="s">
         <v>83</v>
       </c>
-      <c r="E35" s="115" t="str">
+      <c r="E35" s="113" t="str">
         <f t="shared" si="5"/>
         <v>HKD_YC6MRH_QM3HBASIS10Y</v>
       </c>
-      <c r="F35" s="114" t="e">
+      <c r="F35" s="112" t="e">
         <f>_xll.qlRateHelperQuoteValue($E35,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="G35" s="114" t="e">
+      <c r="G35" s="112" t="e">
         <f>_xll.qlSwapRateHelperSpread($E35,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="H35" s="113" t="b">
+      <c r="H35" s="111" t="b">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="I35" s="113">
+      <c r="I35" s="111">
         <v>40</v>
       </c>
-      <c r="J35" s="113">
+      <c r="J35" s="111">
         <v>1</v>
       </c>
-      <c r="K35" s="112" t="e">
+      <c r="K35" s="110" t="e">
         <f>_xll.qlRateHelperEarliestDate($E35,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="L35" s="111" t="e">
+      <c r="L35" s="109" t="e">
         <f>_xll.qlRateHelperLatestDate($E35,Trigger)</f>
         <v>#NUM!</v>
       </c>
     </row>
     <row r="36" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B36" s="117" t="str">
+      <c r="B36" s="115" t="str">
         <f t="shared" si="3"/>
         <v>QM</v>
       </c>
-      <c r="C36" s="116" t="str">
+      <c r="C36" s="114" t="str">
         <f t="shared" si="4"/>
         <v>3HBASIS</v>
       </c>
-      <c r="D36" s="115" t="s">
+      <c r="D36" s="113" t="s">
         <v>82</v>
       </c>
-      <c r="E36" s="115" t="str">
+      <c r="E36" s="113" t="str">
         <f t="shared" si="5"/>
         <v>HKD_YC6MRH_QM3HBASIS11Y</v>
       </c>
-      <c r="F36" s="114" t="e">
+      <c r="F36" s="112" t="e">
         <f>_xll.qlRateHelperQuoteValue($E36,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="G36" s="114" t="e">
+      <c r="G36" s="112" t="e">
         <f>_xll.qlSwapRateHelperSpread($E36,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="H36" s="113" t="b">
+      <c r="H36" s="111" t="b">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="I36" s="113">
+      <c r="I36" s="111">
         <v>40</v>
       </c>
-      <c r="J36" s="113">
+      <c r="J36" s="111">
         <v>1</v>
       </c>
-      <c r="K36" s="112" t="e">
+      <c r="K36" s="110" t="e">
         <f>_xll.qlRateHelperEarliestDate($E36,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="L36" s="111" t="e">
+      <c r="L36" s="109" t="e">
         <f>_xll.qlRateHelperLatestDate($E36,Trigger)</f>
         <v>#NUM!</v>
       </c>
     </row>
     <row r="37" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B37" s="117" t="str">
+      <c r="B37" s="115" t="str">
         <f t="shared" si="3"/>
         <v>QM</v>
       </c>
-      <c r="C37" s="116" t="str">
+      <c r="C37" s="114" t="str">
         <f t="shared" si="4"/>
         <v>3HBASIS</v>
       </c>
-      <c r="D37" s="115" t="s">
+      <c r="D37" s="113" t="s">
         <v>81</v>
       </c>
-      <c r="E37" s="115" t="str">
+      <c r="E37" s="113" t="str">
         <f t="shared" si="5"/>
         <v>HKD_YC6MRH_QM3HBASIS12Y</v>
       </c>
-      <c r="F37" s="114" t="e">
+      <c r="F37" s="112" t="e">
         <f>_xll.qlRateHelperQuoteValue($E37,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="G37" s="114" t="e">
+      <c r="G37" s="112" t="e">
         <f>_xll.qlSwapRateHelperSpread($E37,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="H37" s="113" t="b">
+      <c r="H37" s="111" t="b">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="I37" s="113">
+      <c r="I37" s="111">
         <v>40</v>
       </c>
-      <c r="J37" s="113">
+      <c r="J37" s="111">
         <v>1</v>
       </c>
-      <c r="K37" s="112" t="e">
+      <c r="K37" s="110" t="e">
         <f>_xll.qlRateHelperEarliestDate($E37,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="L37" s="111" t="e">
+      <c r="L37" s="109" t="e">
         <f>_xll.qlRateHelperLatestDate($E37,Trigger)</f>
         <v>#NUM!</v>
       </c>
     </row>
     <row r="38" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B38" s="117" t="str">
+      <c r="B38" s="115" t="str">
         <f t="shared" si="3"/>
         <v>QM</v>
       </c>
-      <c r="C38" s="116" t="str">
+      <c r="C38" s="114" t="str">
         <f t="shared" si="4"/>
         <v>3HBASIS</v>
       </c>
-      <c r="D38" s="115" t="s">
+      <c r="D38" s="113" t="s">
         <v>80</v>
       </c>
-      <c r="E38" s="115" t="str">
+      <c r="E38" s="113" t="str">
         <f t="shared" si="5"/>
         <v>HKD_YC6MRH_QM3HBASIS13Y</v>
       </c>
-      <c r="F38" s="114" t="e">
+      <c r="F38" s="112" t="e">
         <f>_xll.qlRateHelperQuoteValue($E38,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="G38" s="114" t="e">
+      <c r="G38" s="112" t="e">
         <f>_xll.qlSwapRateHelperSpread($E38,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="H38" s="113" t="b">
+      <c r="H38" s="111" t="b">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="I38" s="113">
+      <c r="I38" s="111">
         <v>40</v>
       </c>
-      <c r="J38" s="113">
+      <c r="J38" s="111">
         <v>1</v>
       </c>
-      <c r="K38" s="112" t="e">
+      <c r="K38" s="110" t="e">
         <f>_xll.qlRateHelperEarliestDate($E38,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="L38" s="111" t="e">
+      <c r="L38" s="109" t="e">
         <f>_xll.qlRateHelperLatestDate($E38,Trigger)</f>
         <v>#NUM!</v>
       </c>
     </row>
     <row r="39" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B39" s="117" t="str">
+      <c r="B39" s="115" t="str">
         <f t="shared" si="3"/>
         <v>QM</v>
       </c>
-      <c r="C39" s="116" t="str">
+      <c r="C39" s="114" t="str">
         <f t="shared" si="4"/>
         <v>3HBASIS</v>
       </c>
-      <c r="D39" s="115" t="s">
+      <c r="D39" s="113" t="s">
         <v>79</v>
       </c>
-      <c r="E39" s="115" t="str">
+      <c r="E39" s="113" t="str">
         <f t="shared" si="5"/>
         <v>HKD_YC6MRH_QM3HBASIS14Y</v>
       </c>
-      <c r="F39" s="114" t="e">
+      <c r="F39" s="112" t="e">
         <f>_xll.qlRateHelperQuoteValue($E39,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="G39" s="114" t="e">
+      <c r="G39" s="112" t="e">
         <f>_xll.qlSwapRateHelperSpread($E39,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="H39" s="113" t="b">
+      <c r="H39" s="111" t="b">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="I39" s="113">
+      <c r="I39" s="111">
         <v>40</v>
       </c>
-      <c r="J39" s="113">
+      <c r="J39" s="111">
         <v>1</v>
       </c>
-      <c r="K39" s="112" t="e">
+      <c r="K39" s="110" t="e">
         <f>_xll.qlRateHelperEarliestDate($E39,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="L39" s="111" t="e">
+      <c r="L39" s="109" t="e">
         <f>_xll.qlRateHelperLatestDate($E39,Trigger)</f>
         <v>#NUM!</v>
       </c>
     </row>
     <row r="40" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B40" s="117" t="str">
+      <c r="B40" s="115" t="str">
         <f t="shared" si="3"/>
         <v>QM</v>
       </c>
-      <c r="C40" s="116" t="str">
+      <c r="C40" s="114" t="str">
         <f t="shared" si="4"/>
         <v>3HBASIS</v>
       </c>
-      <c r="D40" s="115" t="s">
+      <c r="D40" s="113" t="s">
         <v>78</v>
       </c>
-      <c r="E40" s="115" t="str">
+      <c r="E40" s="113" t="str">
         <f t="shared" si="5"/>
         <v>HKD_YC6MRH_QM3HBASIS15Y</v>
       </c>
-      <c r="F40" s="114" t="e">
+      <c r="F40" s="112" t="e">
         <f>_xll.qlRateHelperQuoteValue($E40,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="G40" s="114" t="e">
+      <c r="G40" s="112" t="e">
         <f>_xll.qlSwapRateHelperSpread($E40,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="H40" s="113" t="b">
+      <c r="H40" s="111" t="b">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="I40" s="113">
+      <c r="I40" s="111">
         <v>40</v>
       </c>
-      <c r="J40" s="113">
+      <c r="J40" s="111">
         <v>1</v>
       </c>
-      <c r="K40" s="112" t="e">
+      <c r="K40" s="110" t="e">
         <f>_xll.qlRateHelperEarliestDate($E40,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="L40" s="111" t="e">
+      <c r="L40" s="109" t="e">
         <f>_xll.qlRateHelperLatestDate($E40,Trigger)</f>
         <v>#NUM!</v>
       </c>
     </row>
     <row r="41" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B41" s="117" t="str">
+      <c r="B41" s="115" t="str">
         <f t="shared" si="3"/>
         <v>QM</v>
       </c>
-      <c r="C41" s="116" t="str">
+      <c r="C41" s="114" t="str">
         <f t="shared" si="4"/>
         <v>3HBASIS</v>
       </c>
-      <c r="D41" s="115" t="s">
+      <c r="D41" s="113" t="s">
         <v>77</v>
       </c>
-      <c r="E41" s="115" t="str">
+      <c r="E41" s="113" t="str">
         <f t="shared" si="5"/>
         <v>HKD_YC6MRH_QM3HBASIS16Y</v>
       </c>
-      <c r="F41" s="114" t="e">
+      <c r="F41" s="112" t="e">
         <f>_xll.qlRateHelperQuoteValue($E41,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="G41" s="114" t="e">
+      <c r="G41" s="112" t="e">
         <f>_xll.qlSwapRateHelperSpread($E41,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="H41" s="113" t="b">
+      <c r="H41" s="111" t="b">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="I41" s="113">
+      <c r="I41" s="111">
         <v>40</v>
       </c>
-      <c r="J41" s="113">
+      <c r="J41" s="111">
         <v>1</v>
       </c>
-      <c r="K41" s="112" t="e">
+      <c r="K41" s="110" t="e">
         <f>_xll.qlRateHelperEarliestDate($E41,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="L41" s="111" t="e">
+      <c r="L41" s="109" t="e">
         <f>_xll.qlRateHelperLatestDate($E41,Trigger)</f>
         <v>#NUM!</v>
       </c>
     </row>
     <row r="42" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B42" s="117" t="str">
+      <c r="B42" s="115" t="str">
         <f t="shared" si="3"/>
         <v>QM</v>
       </c>
-      <c r="C42" s="116" t="str">
+      <c r="C42" s="114" t="str">
         <f t="shared" si="4"/>
         <v>3HBASIS</v>
       </c>
-      <c r="D42" s="115" t="s">
+      <c r="D42" s="113" t="s">
         <v>76</v>
       </c>
-      <c r="E42" s="115" t="str">
+      <c r="E42" s="113" t="str">
         <f t="shared" si="5"/>
         <v>HKD_YC6MRH_QM3HBASIS17Y</v>
       </c>
-      <c r="F42" s="114" t="e">
+      <c r="F42" s="112" t="e">
         <f>_xll.qlRateHelperQuoteValue($E42,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="G42" s="114" t="e">
+      <c r="G42" s="112" t="e">
         <f>_xll.qlSwapRateHelperSpread($E42,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="H42" s="113" t="b">
+      <c r="H42" s="111" t="b">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="I42" s="113">
+      <c r="I42" s="111">
         <v>40</v>
       </c>
-      <c r="J42" s="113">
+      <c r="J42" s="111">
         <v>1</v>
       </c>
-      <c r="K42" s="112" t="e">
+      <c r="K42" s="110" t="e">
         <f>_xll.qlRateHelperEarliestDate($E42,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="L42" s="111" t="e">
+      <c r="L42" s="109" t="e">
         <f>_xll.qlRateHelperLatestDate($E42,Trigger)</f>
         <v>#NUM!</v>
       </c>
     </row>
     <row r="43" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B43" s="117" t="str">
+      <c r="B43" s="115" t="str">
         <f t="shared" si="3"/>
         <v>QM</v>
       </c>
-      <c r="C43" s="116" t="str">
+      <c r="C43" s="114" t="str">
         <f t="shared" si="4"/>
         <v>3HBASIS</v>
       </c>
-      <c r="D43" s="115" t="s">
+      <c r="D43" s="113" t="s">
         <v>75</v>
       </c>
-      <c r="E43" s="115" t="str">
+      <c r="E43" s="113" t="str">
         <f t="shared" si="5"/>
         <v>HKD_YC6MRH_QM3HBASIS18Y</v>
       </c>
-      <c r="F43" s="114" t="e">
+      <c r="F43" s="112" t="e">
         <f>_xll.qlRateHelperQuoteValue($E43,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="G43" s="114" t="e">
+      <c r="G43" s="112" t="e">
         <f>_xll.qlSwapRateHelperSpread($E43,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="H43" s="113" t="b">
+      <c r="H43" s="111" t="b">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="I43" s="113">
+      <c r="I43" s="111">
         <v>40</v>
       </c>
-      <c r="J43" s="113">
+      <c r="J43" s="111">
         <v>1</v>
       </c>
-      <c r="K43" s="112" t="e">
+      <c r="K43" s="110" t="e">
         <f>_xll.qlRateHelperEarliestDate($E43,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="L43" s="111" t="e">
+      <c r="L43" s="109" t="e">
         <f>_xll.qlRateHelperLatestDate($E43,Trigger)</f>
         <v>#NUM!</v>
       </c>
     </row>
     <row r="44" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B44" s="117" t="str">
+      <c r="B44" s="115" t="str">
         <f t="shared" si="3"/>
         <v>QM</v>
       </c>
-      <c r="C44" s="116" t="str">
+      <c r="C44" s="114" t="str">
         <f t="shared" si="4"/>
         <v>3HBASIS</v>
       </c>
-      <c r="D44" s="115" t="s">
+      <c r="D44" s="113" t="s">
         <v>74</v>
       </c>
-      <c r="E44" s="115" t="str">
+      <c r="E44" s="113" t="str">
         <f t="shared" si="5"/>
         <v>HKD_YC6MRH_QM3HBASIS19Y</v>
       </c>
-      <c r="F44" s="114" t="e">
+      <c r="F44" s="112" t="e">
         <f>_xll.qlRateHelperQuoteValue($E44,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="G44" s="114" t="e">
+      <c r="G44" s="112" t="e">
         <f>_xll.qlSwapRateHelperSpread($E44,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="H44" s="113" t="b">
+      <c r="H44" s="111" t="b">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="I44" s="113">
+      <c r="I44" s="111">
         <v>40</v>
       </c>
-      <c r="J44" s="113">
+      <c r="J44" s="111">
         <v>1</v>
       </c>
-      <c r="K44" s="112" t="e">
+      <c r="K44" s="110" t="e">
         <f>_xll.qlRateHelperEarliestDate($E44,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="L44" s="111" t="e">
+      <c r="L44" s="109" t="e">
         <f>_xll.qlRateHelperLatestDate($E44,Trigger)</f>
         <v>#NUM!</v>
       </c>
     </row>
     <row r="45" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B45" s="117" t="str">
+      <c r="B45" s="115" t="str">
         <f t="shared" si="3"/>
         <v>QM</v>
       </c>
-      <c r="C45" s="116" t="str">
+      <c r="C45" s="114" t="str">
         <f t="shared" si="4"/>
         <v>3HBASIS</v>
       </c>
-      <c r="D45" s="115" t="s">
+      <c r="D45" s="113" t="s">
         <v>73</v>
       </c>
-      <c r="E45" s="115" t="str">
+      <c r="E45" s="113" t="str">
         <f t="shared" si="5"/>
         <v>HKD_YC6MRH_QM3HBASIS20Y</v>
       </c>
-      <c r="F45" s="114" t="e">
+      <c r="F45" s="112" t="e">
         <f>_xll.qlRateHelperQuoteValue($E45,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="G45" s="114" t="e">
+      <c r="G45" s="112" t="e">
         <f>_xll.qlSwapRateHelperSpread($E45,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="H45" s="113" t="b">
+      <c r="H45" s="111" t="b">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="I45" s="113">
+      <c r="I45" s="111">
         <v>40</v>
       </c>
-      <c r="J45" s="113">
+      <c r="J45" s="111">
         <v>1</v>
       </c>
-      <c r="K45" s="112" t="e">
+      <c r="K45" s="110" t="e">
         <f>_xll.qlRateHelperEarliestDate($E45,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="L45" s="111" t="e">
+      <c r="L45" s="109" t="e">
         <f>_xll.qlRateHelperLatestDate($E45,Trigger)</f>
         <v>#NUM!</v>
       </c>
     </row>
     <row r="46" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B46" s="117" t="str">
+      <c r="B46" s="115" t="str">
         <f t="shared" si="3"/>
         <v>QM</v>
       </c>
-      <c r="C46" s="116" t="str">
+      <c r="C46" s="114" t="str">
         <f t="shared" si="4"/>
         <v>3HBASIS</v>
       </c>
-      <c r="D46" s="115" t="s">
+      <c r="D46" s="113" t="s">
         <v>72</v>
       </c>
-      <c r="E46" s="115" t="str">
+      <c r="E46" s="113" t="str">
         <f t="shared" si="5"/>
         <v>HKD_YC6MRH_QM3HBASIS21Y</v>
       </c>
-      <c r="F46" s="114" t="e">
+      <c r="F46" s="112" t="e">
         <f>_xll.qlRateHelperQuoteValue($E46,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="G46" s="114" t="e">
+      <c r="G46" s="112" t="e">
         <f>_xll.qlSwapRateHelperSpread($E46,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="H46" s="113" t="b">
+      <c r="H46" s="111" t="b">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="I46" s="113">
+      <c r="I46" s="111">
         <v>40</v>
       </c>
-      <c r="J46" s="113">
+      <c r="J46" s="111">
         <v>1</v>
       </c>
-      <c r="K46" s="112" t="e">
+      <c r="K46" s="110" t="e">
         <f>_xll.qlRateHelperEarliestDate($E46,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="L46" s="111" t="e">
+      <c r="L46" s="109" t="e">
         <f>_xll.qlRateHelperLatestDate($E46,Trigger)</f>
         <v>#NUM!</v>
       </c>
     </row>
     <row r="47" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B47" s="117" t="str">
+      <c r="B47" s="115" t="str">
         <f t="shared" si="3"/>
         <v>QM</v>
       </c>
-      <c r="C47" s="116" t="str">
+      <c r="C47" s="114" t="str">
         <f t="shared" si="4"/>
         <v>3HBASIS</v>
       </c>
-      <c r="D47" s="115" t="s">
+      <c r="D47" s="113" t="s">
         <v>71</v>
       </c>
-      <c r="E47" s="115" t="str">
+      <c r="E47" s="113" t="str">
         <f t="shared" si="5"/>
         <v>HKD_YC6MRH_QM3HBASIS22Y</v>
       </c>
-      <c r="F47" s="114" t="e">
+      <c r="F47" s="112" t="e">
         <f>_xll.qlRateHelperQuoteValue($E47,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="G47" s="114" t="e">
+      <c r="G47" s="112" t="e">
         <f>_xll.qlSwapRateHelperSpread($E47,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="H47" s="113" t="b">
+      <c r="H47" s="111" t="b">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="I47" s="113">
+      <c r="I47" s="111">
         <v>40</v>
       </c>
-      <c r="J47" s="113">
+      <c r="J47" s="111">
         <v>1</v>
       </c>
-      <c r="K47" s="112" t="e">
+      <c r="K47" s="110" t="e">
         <f>_xll.qlRateHelperEarliestDate($E47,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="L47" s="111" t="e">
+      <c r="L47" s="109" t="e">
         <f>_xll.qlRateHelperLatestDate($E47,Trigger)</f>
         <v>#NUM!</v>
       </c>
     </row>
     <row r="48" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B48" s="117" t="str">
+      <c r="B48" s="115" t="str">
         <f t="shared" si="3"/>
         <v>QM</v>
       </c>
-      <c r="C48" s="116" t="str">
+      <c r="C48" s="114" t="str">
         <f t="shared" si="4"/>
         <v>3HBASIS</v>
       </c>
-      <c r="D48" s="115" t="s">
+      <c r="D48" s="113" t="s">
         <v>70</v>
       </c>
-      <c r="E48" s="115" t="str">
+      <c r="E48" s="113" t="str">
         <f t="shared" si="5"/>
         <v>HKD_YC6MRH_QM3HBASIS23Y</v>
       </c>
-      <c r="F48" s="114" t="e">
+      <c r="F48" s="112" t="e">
         <f>_xll.qlRateHelperQuoteValue($E48,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="G48" s="114" t="e">
+      <c r="G48" s="112" t="e">
         <f>_xll.qlSwapRateHelperSpread($E48,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="H48" s="113" t="b">
+      <c r="H48" s="111" t="b">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="I48" s="113">
+      <c r="I48" s="111">
         <v>40</v>
       </c>
-      <c r="J48" s="113">
+      <c r="J48" s="111">
         <v>1</v>
       </c>
-      <c r="K48" s="112" t="e">
+      <c r="K48" s="110" t="e">
         <f>_xll.qlRateHelperEarliestDate($E48,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="L48" s="111" t="e">
+      <c r="L48" s="109" t="e">
         <f>_xll.qlRateHelperLatestDate($E48,Trigger)</f>
         <v>#NUM!</v>
       </c>
     </row>
     <row r="49" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B49" s="117" t="str">
+      <c r="B49" s="115" t="str">
         <f t="shared" si="3"/>
         <v>QM</v>
       </c>
-      <c r="C49" s="116" t="str">
+      <c r="C49" s="114" t="str">
         <f t="shared" si="4"/>
         <v>3HBASIS</v>
       </c>
-      <c r="D49" s="115" t="s">
+      <c r="D49" s="113" t="s">
         <v>69</v>
       </c>
-      <c r="E49" s="115" t="str">
+      <c r="E49" s="113" t="str">
         <f t="shared" si="5"/>
         <v>HKD_YC6MRH_QM3HBASIS24Y</v>
       </c>
-      <c r="F49" s="114" t="e">
+      <c r="F49" s="112" t="e">
         <f>_xll.qlRateHelperQuoteValue($E49,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="G49" s="114" t="e">
+      <c r="G49" s="112" t="e">
         <f>_xll.qlSwapRateHelperSpread($E49,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="H49" s="113" t="b">
+      <c r="H49" s="111" t="b">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="I49" s="113">
+      <c r="I49" s="111">
         <v>40</v>
       </c>
-      <c r="J49" s="113">
+      <c r="J49" s="111">
         <v>1</v>
       </c>
-      <c r="K49" s="112" t="e">
+      <c r="K49" s="110" t="e">
         <f>_xll.qlRateHelperEarliestDate($E49,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="L49" s="111" t="e">
+      <c r="L49" s="109" t="e">
         <f>_xll.qlRateHelperLatestDate($E49,Trigger)</f>
         <v>#NUM!</v>
       </c>
     </row>
     <row r="50" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B50" s="117" t="str">
+      <c r="B50" s="115" t="str">
         <f t="shared" ref="B50:B59" si="8">SwapFixedFreq</f>
         <v>QM</v>
       </c>
-      <c r="C50" s="116" t="str">
+      <c r="C50" s="114" t="str">
         <f t="shared" si="4"/>
         <v>3HBASIS</v>
       </c>
-      <c r="D50" s="115" t="s">
+      <c r="D50" s="113" t="s">
         <v>68</v>
       </c>
-      <c r="E50" s="115" t="str">
+      <c r="E50" s="113" t="str">
         <f t="shared" si="5"/>
         <v>HKD_YC6MRH_QM3HBASIS25Y</v>
       </c>
-      <c r="F50" s="114" t="e">
+      <c r="F50" s="112" t="e">
         <f>_xll.qlRateHelperQuoteValue($E50,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="G50" s="114" t="e">
+      <c r="G50" s="112" t="e">
         <f>_xll.qlSwapRateHelperSpread($E50,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="H50" s="113" t="b">
+      <c r="H50" s="111" t="b">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="I50" s="113">
+      <c r="I50" s="111">
         <v>40</v>
       </c>
-      <c r="J50" s="113">
+      <c r="J50" s="111">
         <v>1</v>
       </c>
-      <c r="K50" s="112" t="e">
+      <c r="K50" s="110" t="e">
         <f>_xll.qlRateHelperEarliestDate($E50,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="L50" s="111" t="e">
+      <c r="L50" s="109" t="e">
         <f>_xll.qlRateHelperLatestDate($E50,Trigger)</f>
         <v>#NUM!</v>
       </c>
     </row>
     <row r="51" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B51" s="117" t="str">
+      <c r="B51" s="115" t="str">
         <f t="shared" si="8"/>
         <v>QM</v>
       </c>
-      <c r="C51" s="116" t="str">
+      <c r="C51" s="114" t="str">
         <f t="shared" si="4"/>
         <v>3HBASIS</v>
       </c>
-      <c r="D51" s="115" t="s">
+      <c r="D51" s="113" t="s">
         <v>67</v>
       </c>
-      <c r="E51" s="115" t="str">
+      <c r="E51" s="113" t="str">
         <f t="shared" si="5"/>
         <v>HKD_YC6MRH_QM3HBASIS26Y</v>
       </c>
-      <c r="F51" s="114" t="e">
+      <c r="F51" s="112" t="e">
         <f>_xll.qlRateHelperQuoteValue($E51,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="G51" s="114" t="e">
+      <c r="G51" s="112" t="e">
         <f>_xll.qlSwapRateHelperSpread($E51,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="H51" s="113" t="b">
+      <c r="H51" s="111" t="b">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="I51" s="113">
+      <c r="I51" s="111">
         <v>40</v>
       </c>
-      <c r="J51" s="113">
+      <c r="J51" s="111">
         <v>1</v>
       </c>
-      <c r="K51" s="112" t="e">
+      <c r="K51" s="110" t="e">
         <f>_xll.qlRateHelperEarliestDate($E51,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="L51" s="111" t="e">
+      <c r="L51" s="109" t="e">
         <f>_xll.qlRateHelperLatestDate($E51,Trigger)</f>
         <v>#NUM!</v>
       </c>
     </row>
     <row r="52" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B52" s="117" t="str">
+      <c r="B52" s="115" t="str">
         <f t="shared" si="8"/>
         <v>QM</v>
       </c>
-      <c r="C52" s="116" t="str">
+      <c r="C52" s="114" t="str">
         <f t="shared" si="4"/>
         <v>3HBASIS</v>
       </c>
-      <c r="D52" s="115" t="s">
+      <c r="D52" s="113" t="s">
         <v>66</v>
       </c>
-      <c r="E52" s="115" t="str">
+      <c r="E52" s="113" t="str">
         <f t="shared" ref="E52:E59" si="9">RateHelperPrefix&amp;"_"&amp;$B52&amp;$C52&amp;$D52</f>
         <v>HKD_YC6MRH_QM3HBASIS27Y</v>
       </c>
-      <c r="F52" s="114" t="e">
+      <c r="F52" s="112" t="e">
         <f>_xll.qlRateHelperQuoteValue($E52,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="G52" s="114" t="e">
+      <c r="G52" s="112" t="e">
         <f>_xll.qlSwapRateHelperSpread($E52,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="H52" s="113" t="b">
+      <c r="H52" s="111" t="b">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="I52" s="113">
+      <c r="I52" s="111">
         <v>40</v>
       </c>
-      <c r="J52" s="113">
+      <c r="J52" s="111">
         <v>1</v>
       </c>
-      <c r="K52" s="112" t="e">
+      <c r="K52" s="110" t="e">
         <f>_xll.qlRateHelperEarliestDate($E52,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="L52" s="111" t="e">
+      <c r="L52" s="109" t="e">
         <f>_xll.qlRateHelperLatestDate($E52,Trigger)</f>
         <v>#NUM!</v>
       </c>
     </row>
     <row r="53" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B53" s="117" t="str">
+      <c r="B53" s="115" t="str">
         <f t="shared" si="8"/>
         <v>QM</v>
       </c>
-      <c r="C53" s="116" t="str">
+      <c r="C53" s="114" t="str">
         <f t="shared" si="4"/>
         <v>3HBASIS</v>
       </c>
-      <c r="D53" s="115" t="s">
+      <c r="D53" s="113" t="s">
         <v>65</v>
       </c>
-      <c r="E53" s="115" t="str">
+      <c r="E53" s="113" t="str">
         <f t="shared" si="9"/>
         <v>HKD_YC6MRH_QM3HBASIS28Y</v>
       </c>
-      <c r="F53" s="114" t="e">
+      <c r="F53" s="112" t="e">
         <f>_xll.qlRateHelperQuoteValue($E53,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="G53" s="114" t="e">
+      <c r="G53" s="112" t="e">
         <f>_xll.qlSwapRateHelperSpread($E53,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="H53" s="113" t="b">
+      <c r="H53" s="111" t="b">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="I53" s="113">
+      <c r="I53" s="111">
         <v>40</v>
       </c>
-      <c r="J53" s="113">
+      <c r="J53" s="111">
         <v>1</v>
       </c>
-      <c r="K53" s="112" t="e">
+      <c r="K53" s="110" t="e">
         <f>_xll.qlRateHelperEarliestDate($E53,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="L53" s="111" t="e">
+      <c r="L53" s="109" t="e">
         <f>_xll.qlRateHelperLatestDate($E53,Trigger)</f>
         <v>#NUM!</v>
       </c>
     </row>
     <row r="54" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B54" s="117" t="str">
+      <c r="B54" s="115" t="str">
         <f t="shared" si="8"/>
         <v>QM</v>
       </c>
-      <c r="C54" s="116" t="str">
+      <c r="C54" s="114" t="str">
         <f t="shared" si="4"/>
         <v>3HBASIS</v>
       </c>
-      <c r="D54" s="115" t="s">
+      <c r="D54" s="113" t="s">
         <v>64</v>
       </c>
-      <c r="E54" s="115" t="str">
+      <c r="E54" s="113" t="str">
         <f t="shared" si="9"/>
         <v>HKD_YC6MRH_QM3HBASIS29Y</v>
       </c>
-      <c r="F54" s="114" t="e">
+      <c r="F54" s="112" t="e">
         <f>_xll.qlRateHelperQuoteValue($E54,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="G54" s="114" t="e">
+      <c r="G54" s="112" t="e">
         <f>_xll.qlSwapRateHelperSpread($E54,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="H54" s="113" t="b">
+      <c r="H54" s="111" t="b">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="I54" s="113">
+      <c r="I54" s="111">
         <v>40</v>
       </c>
-      <c r="J54" s="113">
+      <c r="J54" s="111">
         <v>1</v>
       </c>
-      <c r="K54" s="112" t="e">
+      <c r="K54" s="110" t="e">
         <f>_xll.qlRateHelperEarliestDate($E54,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="L54" s="111" t="e">
+      <c r="L54" s="109" t="e">
         <f>_xll.qlRateHelperLatestDate($E54,Trigger)</f>
         <v>#NUM!</v>
       </c>
     </row>
     <row r="55" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B55" s="117" t="str">
+      <c r="B55" s="115" t="str">
         <f t="shared" si="8"/>
         <v>QM</v>
       </c>
-      <c r="C55" s="116" t="str">
+      <c r="C55" s="114" t="str">
         <f t="shared" si="4"/>
         <v>3HBASIS</v>
       </c>
-      <c r="D55" s="115" t="s">
+      <c r="D55" s="113" t="s">
         <v>63</v>
       </c>
-      <c r="E55" s="115" t="str">
+      <c r="E55" s="113" t="str">
         <f t="shared" si="9"/>
         <v>HKD_YC6MRH_QM3HBASIS30Y</v>
       </c>
-      <c r="F55" s="114" t="e">
+      <c r="F55" s="112" t="e">
         <f>_xll.qlRateHelperQuoteValue($E55,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="G55" s="114" t="e">
+      <c r="G55" s="112" t="e">
         <f>_xll.qlSwapRateHelperSpread($E55,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="H55" s="113" t="b">
+      <c r="H55" s="111" t="b">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="I55" s="113">
+      <c r="I55" s="111">
         <v>40</v>
       </c>
-      <c r="J55" s="113">
+      <c r="J55" s="111">
         <v>1</v>
       </c>
-      <c r="K55" s="112" t="e">
+      <c r="K55" s="110" t="e">
         <f>_xll.qlRateHelperEarliestDate($E55,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="L55" s="111" t="e">
+      <c r="L55" s="109" t="e">
         <f>_xll.qlRateHelperLatestDate($E55,Trigger)</f>
         <v>#NUM!</v>
       </c>
     </row>
     <row r="56" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B56" s="117" t="str">
+      <c r="B56" s="115" t="str">
         <f t="shared" si="8"/>
         <v>QM</v>
       </c>
-      <c r="C56" s="116" t="str">
+      <c r="C56" s="114" t="str">
         <f t="shared" si="4"/>
         <v>3HBASIS</v>
       </c>
-      <c r="D56" s="115" t="s">
+      <c r="D56" s="113" t="s">
         <v>62</v>
       </c>
-      <c r="E56" s="115" t="str">
+      <c r="E56" s="113" t="str">
         <f t="shared" si="9"/>
         <v>HKD_YC6MRH_QM3HBASIS35Y</v>
       </c>
-      <c r="F56" s="114" t="e">
+      <c r="F56" s="112" t="e">
         <f>_xll.qlRateHelperQuoteValue($E56,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="G56" s="114" t="e">
+      <c r="G56" s="112" t="e">
         <f>_xll.qlSwapRateHelperSpread($E56,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="H56" s="113" t="b">
+      <c r="H56" s="111" t="b">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="I56" s="113">
+      <c r="I56" s="111">
         <v>40</v>
       </c>
-      <c r="J56" s="113">
+      <c r="J56" s="111">
         <v>1</v>
       </c>
-      <c r="K56" s="112" t="e">
+      <c r="K56" s="110" t="e">
         <f>_xll.qlRateHelperEarliestDate($E56,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="L56" s="111" t="e">
+      <c r="L56" s="109" t="e">
         <f>_xll.qlRateHelperLatestDate($E56,Trigger)</f>
         <v>#NUM!</v>
       </c>
     </row>
     <row r="57" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B57" s="117" t="str">
+      <c r="B57" s="115" t="str">
         <f t="shared" si="8"/>
         <v>QM</v>
       </c>
-      <c r="C57" s="116" t="str">
+      <c r="C57" s="114" t="str">
         <f t="shared" si="4"/>
         <v>3HBASIS</v>
       </c>
-      <c r="D57" s="115" t="s">
+      <c r="D57" s="113" t="s">
         <v>61</v>
       </c>
-      <c r="E57" s="115" t="str">
+      <c r="E57" s="113" t="str">
         <f t="shared" si="9"/>
         <v>HKD_YC6MRH_QM3HBASIS40Y</v>
       </c>
-      <c r="F57" s="114" t="e">
+      <c r="F57" s="112" t="e">
         <f>_xll.qlRateHelperQuoteValue($E57,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="G57" s="114" t="e">
+      <c r="G57" s="112" t="e">
         <f>_xll.qlSwapRateHelperSpread($E57,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="H57" s="113" t="b">
+      <c r="H57" s="111" t="b">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="I57" s="113">
+      <c r="I57" s="111">
         <v>40</v>
       </c>
-      <c r="J57" s="113">
+      <c r="J57" s="111">
         <v>1</v>
       </c>
-      <c r="K57" s="112" t="e">
+      <c r="K57" s="110" t="e">
         <f>_xll.qlRateHelperEarliestDate($E57,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="L57" s="111" t="e">
+      <c r="L57" s="109" t="e">
         <f>_xll.qlRateHelperLatestDate($E57,Trigger)</f>
         <v>#NUM!</v>
       </c>
     </row>
     <row r="58" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B58" s="117" t="str">
+      <c r="B58" s="115" t="str">
         <f t="shared" si="8"/>
         <v>QM</v>
       </c>
-      <c r="C58" s="116" t="str">
+      <c r="C58" s="114" t="str">
         <f t="shared" si="4"/>
         <v>3HBASIS</v>
       </c>
-      <c r="D58" s="115" t="s">
+      <c r="D58" s="113" t="s">
         <v>60</v>
       </c>
-      <c r="E58" s="115" t="str">
+      <c r="E58" s="113" t="str">
         <f t="shared" si="9"/>
         <v>HKD_YC6MRH_QM3HBASIS50Y</v>
       </c>
-      <c r="F58" s="114" t="e">
+      <c r="F58" s="112" t="e">
         <f>_xll.qlRateHelperQuoteValue($E58,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="G58" s="114" t="e">
+      <c r="G58" s="112" t="e">
         <f>_xll.qlSwapRateHelperSpread($E58,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="H58" s="113" t="b">
+      <c r="H58" s="111" t="b">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="I58" s="113">
+      <c r="I58" s="111">
         <v>40</v>
       </c>
-      <c r="J58" s="113">
+      <c r="J58" s="111">
         <v>1</v>
       </c>
-      <c r="K58" s="112" t="e">
+      <c r="K58" s="110" t="e">
         <f>_xll.qlRateHelperEarliestDate($E58,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="L58" s="111" t="e">
+      <c r="L58" s="109" t="e">
         <f>_xll.qlRateHelperLatestDate($E58,Trigger)</f>
         <v>#NUM!</v>
       </c>
     </row>
     <row r="59" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B59" s="110" t="str">
+      <c r="B59" s="108" t="str">
         <f t="shared" si="8"/>
         <v>QM</v>
       </c>
-      <c r="C59" s="109" t="str">
+      <c r="C59" s="107" t="str">
         <f t="shared" si="4"/>
         <v>3HBASIS</v>
       </c>
-      <c r="D59" s="108" t="s">
+      <c r="D59" s="106" t="s">
         <v>59</v>
       </c>
-      <c r="E59" s="108" t="str">
+      <c r="E59" s="106" t="str">
         <f t="shared" si="9"/>
         <v>HKD_YC6MRH_QM3HBASIS60Y</v>
       </c>
-      <c r="F59" s="107" t="e">
+      <c r="F59" s="105" t="e">
         <f>_xll.qlRateHelperQuoteValue($E59,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="G59" s="107" t="e">
+      <c r="G59" s="105" t="e">
         <f>_xll.qlSwapRateHelperSpread($E59,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="H59" s="106" t="b">
+      <c r="H59" s="104" t="b">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="I59" s="106">
+      <c r="I59" s="104">
         <v>40</v>
       </c>
-      <c r="J59" s="106">
+      <c r="J59" s="104">
         <v>1</v>
       </c>
-      <c r="K59" s="105" t="e">
+      <c r="K59" s="103" t="e">
         <f>_xll.qlRateHelperEarliestDate($E59,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="L59" s="104" t="e">
+      <c r="L59" s="102" t="e">
         <f>_xll.qlRateHelperLatestDate($E59,Trigger)</f>
         <v>#NUM!</v>
       </c>
@@ -5743,7 +5774,7 @@
   <dimension ref="A1:I126"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -5760,10 +5791,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="23.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="143" t="s">
+      <c r="A1" s="154" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="144"/>
+      <c r="B1" s="155"/>
       <c r="D1" s="3" t="s">
         <v>20</v>
       </c>
@@ -5803,14 +5834,14 @@
       </c>
       <c r="G2" s="11">
         <f>_xll.qlRateHelperEarliestDate($D2)</f>
-        <v>41684</v>
+        <v>41736</v>
       </c>
       <c r="H2" s="12">
         <f>_xll.qlRateHelperLatestDate($D2)</f>
-        <v>41865</v>
+        <v>41919</v>
       </c>
       <c r="I2" s="6">
-        <v>0.99728707396165672</v>
+        <v>0.99725717910013068</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
@@ -5825,7 +5856,7 @@
       </c>
       <c r="E3" s="10">
         <f>_xll.qlRateHelperRate($D3)</f>
-        <v>4.8999999999999998E-3</v>
+        <v>4.7999999999999996E-3</v>
       </c>
       <c r="F3" s="10" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D3)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D3)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D3)),_xll.qlSwapRateHelperSpread($D3))</f>
@@ -5833,14 +5864,14 @@
       </c>
       <c r="G3" s="11">
         <f>_xll.qlRateHelperEarliestDate($D3)</f>
-        <v>41712</v>
+        <v>41766</v>
       </c>
       <c r="H3" s="12">
         <f>_xll.qlRateHelperLatestDate($D3)</f>
-        <v>41897</v>
+        <v>41950</v>
       </c>
       <c r="I3" s="6">
-        <v>0.99710347088010043</v>
+        <v>0.99713704235265099</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
@@ -5855,7 +5886,7 @@
       </c>
       <c r="E4" s="10">
         <f>_xll.qlRateHelperRate($D4)</f>
-        <v>4.8999999999999998E-3</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="F4" s="10" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D4)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D4)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D4)),_xll.qlSwapRateHelperSpread($D4))</f>
@@ -5863,14 +5894,14 @@
       </c>
       <c r="G4" s="11">
         <f>_xll.qlRateHelperEarliestDate($D4)</f>
-        <v>41743</v>
+        <v>41799</v>
       </c>
       <c r="H4" s="12">
         <f>_xll.qlRateHelperLatestDate($D4)</f>
-        <v>41926</v>
+        <v>41982</v>
       </c>
       <c r="I4" s="6">
-        <v>0.99666634378377073</v>
+        <v>0.99655668230754935</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -5885,7 +5916,7 @@
       </c>
       <c r="E5" s="10">
         <f>_xll.qlRateHelperRate($D5)</f>
-        <v>5.0000000000000001E-3</v>
+        <v>5.1000000000000004E-3</v>
       </c>
       <c r="F5" s="10" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D5)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D5)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D5)),_xll.qlSwapRateHelperSpread($D5))</f>
@@ -5893,14 +5924,14 @@
       </c>
       <c r="G5" s="11">
         <f>_xll.qlRateHelperEarliestDate($D5)</f>
-        <v>41773</v>
+        <v>41827</v>
       </c>
       <c r="H5" s="12">
         <f>_xll.qlRateHelperLatestDate($D5)</f>
-        <v>41957</v>
+        <v>42011</v>
       </c>
       <c r="I5" s="6">
-        <v>0.99615424425997234</v>
+        <v>0.99607427591799991</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
@@ -5916,7 +5947,7 @@
       </c>
       <c r="E6" s="10">
         <f>_xll.qlRateHelperRate($D6)</f>
-        <v>5.1000000000000004E-3</v>
+        <v>5.3E-3</v>
       </c>
       <c r="F6" s="10" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D6)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D6)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D6)),_xll.qlSwapRateHelperSpread($D6))</f>
@@ -5924,20 +5955,20 @@
       </c>
       <c r="G6" s="11">
         <f>_xll.qlRateHelperEarliestDate($D6)</f>
-        <v>41806</v>
+        <v>41858</v>
       </c>
       <c r="H6" s="12">
         <f>_xll.qlRateHelperLatestDate($D6)</f>
-        <v>41989</v>
+        <v>42044</v>
       </c>
       <c r="I6" s="6">
-        <v>0.99562478946159827</v>
+        <v>0.99548199622234712</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="str">
         <f>_xll.ohGroup(RateHelperPrefix&amp;"_RateHelpersSelected",_xll.ohPack(Selected!D2:D126),TRUE,,ObjectOverwrite)</f>
-        <v>HKD_YC6MRH_RateHelpersSelected#0003</v>
+        <v>HKD_YC6MRH_RateHelpersSelected#0000</v>
       </c>
       <c r="B7" s="18" t="str">
         <f>_xll.ohRangeRetrieveError(RateHelpersSelected)</f>
@@ -5948,7 +5979,7 @@
       </c>
       <c r="E7" s="10">
         <f>_xll.qlRateHelperRate($D7)</f>
-        <v>5.1999999999999998E-3</v>
+        <v>5.5000000000000005E-3</v>
       </c>
       <c r="F7" s="10" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D7)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D7)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D7)),_xll.qlSwapRateHelperSpread($D7))</f>
@@ -5956,14 +5987,14 @@
       </c>
       <c r="G7" s="11">
         <f>_xll.qlRateHelperEarliestDate($D7)</f>
-        <v>41834</v>
+        <v>41890</v>
       </c>
       <c r="H7" s="12">
         <f>_xll.qlRateHelperLatestDate($D7)</f>
-        <v>42018</v>
+        <v>42072</v>
       </c>
       <c r="I7" s="6">
-        <v>0.99514255915862948</v>
+        <v>0.99496268054121861</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
@@ -5972,7 +6003,7 @@
       </c>
       <c r="E8" s="10">
         <f>_xll.qlRateHelperRate($D8)</f>
-        <v>5.4000000000000003E-3</v>
+        <v>5.8000000000000005E-3</v>
       </c>
       <c r="F8" s="10" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D8)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D8)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D8)),_xll.qlSwapRateHelperSpread($D8))</f>
@@ -5980,14 +6011,14 @@
       </c>
       <c r="G8" s="11">
         <f>_xll.qlRateHelperEarliestDate($D8)</f>
-        <v>41865</v>
+        <v>41919</v>
       </c>
       <c r="H8" s="12">
         <f>_xll.qlRateHelperLatestDate($D8)</f>
-        <v>42051</v>
+        <v>42101</v>
       </c>
       <c r="I8" s="6">
-        <v>0.99455028954844549</v>
+        <v>0.9943813736807966</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
@@ -5996,7 +6027,7 @@
       </c>
       <c r="E9" s="10">
         <f>_xll.qlRateHelperRate($D9)</f>
-        <v>6.1000000000000013E-3</v>
+        <v>8.8000000000000005E-3</v>
       </c>
       <c r="F9" s="10" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D9)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D9)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D9)),_xll.qlSwapRateHelperSpread($D9))</f>
@@ -6004,14 +6035,14 @@
       </c>
       <c r="G9" s="11">
         <f>_xll.qlRateHelperEarliestDate($D9)</f>
-        <v>42051</v>
+        <v>42101</v>
       </c>
       <c r="H9" s="12">
         <f>_xll.qlRateHelperLatestDate($D9)</f>
-        <v>42233</v>
+        <v>42284</v>
       </c>
       <c r="I9" s="6">
-        <v>0.99153439506788554</v>
+        <v>0.99001338039916709</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
@@ -6020,7 +6051,7 @@
       </c>
       <c r="E10" s="10">
         <f>_xll.qlRateHelperRate($D10)</f>
-        <v>7.7000000000000002E-3</v>
+        <v>1.2500000000000001E-2</v>
       </c>
       <c r="F10" s="10" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D10)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D10)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D10)),_xll.qlSwapRateHelperSpread($D10))</f>
@@ -6028,14 +6059,14 @@
       </c>
       <c r="G10" s="11">
         <f>_xll.qlRateHelperEarliestDate($D10)</f>
-        <v>42230</v>
+        <v>42284</v>
       </c>
       <c r="H10" s="12">
         <f>_xll.qlRateHelperLatestDate($D10)</f>
-        <v>42415</v>
+        <v>42467</v>
       </c>
       <c r="I10" s="6">
-        <v>0.98772918348282057</v>
+        <v>0.98384748690248558</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">

</xml_diff>